<commit_message>
Bhatti Charger Scheduling Algo Time rolling
</commit_message>
<xml_diff>
--- a/EVbehaviour.xlsx
+++ b/EVbehaviour.xlsx
@@ -28,904 +28,904 @@
     <t>Time of Day</t>
   </si>
   <si>
-    <t>08:43:56.808339</t>
-  </si>
-  <si>
-    <t>10:16:40.879501</t>
-  </si>
-  <si>
-    <t>08:46:04.986303</t>
-  </si>
-  <si>
-    <t>08:55:36.708207</t>
-  </si>
-  <si>
-    <t>09:46:14.068636</t>
-  </si>
-  <si>
-    <t>08:28:15.440368</t>
-  </si>
-  <si>
-    <t>08:57:49.969860</t>
-  </si>
-  <si>
-    <t>09:37:47.397520</t>
-  </si>
-  <si>
-    <t>09:21:27.972485</t>
-  </si>
-  <si>
-    <t>09:03:46.931063</t>
-  </si>
-  <si>
-    <t>09:15:36.722892</t>
-  </si>
-  <si>
-    <t>08:38:42.883597</t>
-  </si>
-  <si>
-    <t>08:50:53.167786</t>
-  </si>
-  <si>
-    <t>09:46:46.211272</t>
-  </si>
-  <si>
-    <t>08:39:21.255741</t>
-  </si>
-  <si>
-    <t>08:28:41.791264</t>
-  </si>
-  <si>
-    <t>09:14:19.322928</t>
-  </si>
-  <si>
-    <t>10:12:34.066191</t>
-  </si>
-  <si>
-    <t>08:37:27.320411</t>
-  </si>
-  <si>
-    <t>09:25:27.997564</t>
-  </si>
-  <si>
-    <t>09:10:40.635618</t>
-  </si>
-  <si>
-    <t>08:46:23.031376</t>
-  </si>
-  <si>
-    <t>08:29:07.802634</t>
-  </si>
-  <si>
-    <t>08:24:53.009238</t>
-  </si>
-  <si>
-    <t>09:33:16.734534</t>
-  </si>
-  <si>
-    <t>09:53:35.634794</t>
-  </si>
-  <si>
-    <t>08:43:26.098360</t>
-  </si>
-  <si>
-    <t>08:52:53.607480</t>
-  </si>
-  <si>
-    <t>08:36:31.278670</t>
-  </si>
-  <si>
-    <t>09:26:59.501522</t>
-  </si>
-  <si>
-    <t>09:00:13.007778</t>
-  </si>
-  <si>
-    <t>09:02:21.760938</t>
-  </si>
-  <si>
-    <t>09:22:55.781703</t>
-  </si>
-  <si>
-    <t>08:44:48.615427</t>
-  </si>
-  <si>
-    <t>09:19:20.709940</t>
-  </si>
-  <si>
-    <t>08:42:07.582018</t>
-  </si>
-  <si>
-    <t>09:16:35.057103</t>
-  </si>
-  <si>
-    <t>09:54:17.543385</t>
-  </si>
-  <si>
-    <t>08:21:10.825591</t>
-  </si>
-  <si>
-    <t>09:49:32.208482</t>
-  </si>
-  <si>
-    <t>09:52:03.455459</t>
-  </si>
-  <si>
-    <t>09:03:32.904138</t>
-  </si>
-  <si>
-    <t>09:08:41.143134</t>
-  </si>
-  <si>
-    <t>08:37:01.422872</t>
-  </si>
-  <si>
-    <t>09:41:49.898195</t>
-  </si>
-  <si>
-    <t>09:00:42.956171</t>
-  </si>
-  <si>
-    <t>09:49:28.217037</t>
-  </si>
-  <si>
-    <t>09:04:33.701367</t>
-  </si>
-  <si>
-    <t>08:45:00.888208</t>
-  </si>
-  <si>
-    <t>09:37:07.395608</t>
-  </si>
-  <si>
-    <t>08:46:56.477274</t>
-  </si>
-  <si>
-    <t>09:48:19.353813</t>
-  </si>
-  <si>
-    <t>09:48:46.526865</t>
-  </si>
-  <si>
-    <t>11:29:53.579709</t>
-  </si>
-  <si>
-    <t>09:25:27.847450</t>
-  </si>
-  <si>
-    <t>08:39:56.471674</t>
-  </si>
-  <si>
-    <t>09:14:33.348240</t>
-  </si>
-  <si>
-    <t>10:13:38.900786</t>
-  </si>
-  <si>
-    <t>08:32:47.962970</t>
-  </si>
-  <si>
-    <t>08:54:23.158170</t>
-  </si>
-  <si>
-    <t>09:56:37.382997</t>
-  </si>
-  <si>
-    <t>08:49:44.544387</t>
-  </si>
-  <si>
-    <t>07:35:28.291552</t>
-  </si>
-  <si>
-    <t>09:07:56.822132</t>
-  </si>
-  <si>
-    <t>08:30:46.200973</t>
-  </si>
-  <si>
-    <t>10:24:40.493158</t>
-  </si>
-  <si>
-    <t>09:17:28.510290</t>
-  </si>
-  <si>
-    <t>08:54:09.730266</t>
-  </si>
-  <si>
-    <t>09:03:16.953312</t>
-  </si>
-  <si>
-    <t>08:50:08.580776</t>
-  </si>
-  <si>
-    <t>08:22:04.131049</t>
-  </si>
-  <si>
-    <t>08:37:39.583287</t>
-  </si>
-  <si>
-    <t>09:12:38.737237</t>
-  </si>
-  <si>
-    <t>08:55:37.723688</t>
-  </si>
-  <si>
-    <t>08:36:20.519837</t>
-  </si>
-  <si>
-    <t>08:35:16.828087</t>
-  </si>
-  <si>
-    <t>08:47:12.683959</t>
-  </si>
-  <si>
-    <t>09:07:57.779107</t>
-  </si>
-  <si>
-    <t>09:56:13.142453</t>
-  </si>
-  <si>
-    <t>09:46:44.180439</t>
-  </si>
-  <si>
-    <t>08:48:48.053167</t>
-  </si>
-  <si>
-    <t>10:54:30.334947</t>
-  </si>
-  <si>
-    <t>08:21:07.403850</t>
-  </si>
-  <si>
-    <t>08:11:30.636864</t>
-  </si>
-  <si>
-    <t>09:23:32.210066</t>
-  </si>
-  <si>
-    <t>09:42:03.325432</t>
-  </si>
-  <si>
-    <t>10:02:20.366267</t>
-  </si>
-  <si>
-    <t>08:51:10.231385</t>
-  </si>
-  <si>
-    <t>09:06:46.247851</t>
-  </si>
-  <si>
-    <t>09:13:39.275881</t>
-  </si>
-  <si>
-    <t>09:37:45.400225</t>
-  </si>
-  <si>
-    <t>08:45:18.562171</t>
-  </si>
-  <si>
-    <t>09:24:45.854245</t>
-  </si>
-  <si>
-    <t>08:59:53.007465</t>
-  </si>
-  <si>
-    <t>10:30:08.993859</t>
-  </si>
-  <si>
-    <t>08:17:33.332064</t>
-  </si>
-  <si>
-    <t>09:18:50.942037</t>
-  </si>
-  <si>
-    <t>09:42:37.485245</t>
-  </si>
-  <si>
-    <t>10:21:03.607151</t>
-  </si>
-  <si>
-    <t>10:01:46.676075</t>
-  </si>
-  <si>
-    <t>08:35:10.743597</t>
-  </si>
-  <si>
-    <t>08:38:58.162382</t>
-  </si>
-  <si>
-    <t>09:02:53.491748</t>
-  </si>
-  <si>
-    <t>09:00:55.418300</t>
-  </si>
-  <si>
-    <t>08:54:55.654946</t>
-  </si>
-  <si>
-    <t>08:15:03.475244</t>
-  </si>
-  <si>
-    <t>09:15:55.657972</t>
-  </si>
-  <si>
-    <t>08:57:00.417412</t>
-  </si>
-  <si>
-    <t>11:35:05.380695</t>
-  </si>
-  <si>
-    <t>08:43:11.280655</t>
-  </si>
-  <si>
-    <t>10:00:08.523988</t>
-  </si>
-  <si>
-    <t>09:52:30.931887</t>
-  </si>
-  <si>
-    <t>09:01:39.868866</t>
-  </si>
-  <si>
-    <t>08:20:26.988167</t>
-  </si>
-  <si>
-    <t>08:46:06.451334</t>
-  </si>
-  <si>
-    <t>09:07:26.955180</t>
-  </si>
-  <si>
-    <t>08:39:01.823426</t>
-  </si>
-  <si>
-    <t>08:11:10.122016</t>
-  </si>
-  <si>
-    <t>10:11:17.912111</t>
-  </si>
-  <si>
-    <t>08:22:25.503414</t>
-  </si>
-  <si>
-    <t>09:48:33.676163</t>
-  </si>
-  <si>
-    <t>10:11:28.470343</t>
-  </si>
-  <si>
-    <t>10:17:12.401889</t>
-  </si>
-  <si>
-    <t>09:04:10.498931</t>
-  </si>
-  <si>
-    <t>08:44:33.436242</t>
-  </si>
-  <si>
-    <t>09:17:59.373955</t>
-  </si>
-  <si>
-    <t>10:10:37.420532</t>
-  </si>
-  <si>
-    <t>12:26:49.126766</t>
-  </si>
-  <si>
-    <t>10:21:19.275567</t>
-  </si>
-  <si>
-    <t>08:21:53.358975</t>
-  </si>
-  <si>
-    <t>11:05:31.885418</t>
-  </si>
-  <si>
-    <t>08:14:45.525858</t>
-  </si>
-  <si>
-    <t>08:18:49.526164</t>
-  </si>
-  <si>
-    <t>09:36:59.288642</t>
-  </si>
-  <si>
-    <t>09:16:38.011645</t>
-  </si>
-  <si>
-    <t>09:56:54.747268</t>
-  </si>
-  <si>
-    <t>08:52:16.889237</t>
-  </si>
-  <si>
-    <t>10:06:05.832408</t>
-  </si>
-  <si>
-    <t>09:24:05.009645</t>
-  </si>
-  <si>
-    <t>09:40:08.079093</t>
-  </si>
-  <si>
-    <t>07:47:10.916581</t>
-  </si>
-  <si>
-    <t>09:06:07.520894</t>
-  </si>
-  <si>
-    <t>08:29:04.029156</t>
-  </si>
-  <si>
-    <t>08:30:17.611976</t>
-  </si>
-  <si>
-    <t>09:01:17.441732</t>
-  </si>
-  <si>
-    <t>09:49:08.065360</t>
-  </si>
-  <si>
-    <t>10:48:01.968579</t>
-  </si>
-  <si>
-    <t>10:05:19.575071</t>
-  </si>
-  <si>
-    <t>09:19:44.950436</t>
-  </si>
-  <si>
-    <t>09:50:20.812359</t>
-  </si>
-  <si>
-    <t>09:52:06.003059</t>
-  </si>
-  <si>
-    <t>09:16:20.377258</t>
-  </si>
-  <si>
-    <t>08:48:50.182507</t>
-  </si>
-  <si>
-    <t>08:29:29.550114</t>
-  </si>
-  <si>
-    <t>08:35:13.982388</t>
-  </si>
-  <si>
-    <t>10:10:15.101848</t>
-  </si>
-  <si>
-    <t>09:48:49.946329</t>
-  </si>
-  <si>
-    <t>10:08:44.520399</t>
-  </si>
-  <si>
-    <t>08:19:11.917253</t>
-  </si>
-  <si>
-    <t>09:27:51.652836</t>
-  </si>
-  <si>
-    <t>10:49:55.920627</t>
-  </si>
-  <si>
-    <t>10:31:49.023671</t>
-  </si>
-  <si>
-    <t>15:25:20.537370</t>
-  </si>
-  <si>
-    <t>13:47:14.930206</t>
-  </si>
-  <si>
-    <t>14:52:17.728796</t>
-  </si>
-  <si>
-    <t>16:37:36.969114</t>
-  </si>
-  <si>
-    <t>16:07:22.117116</t>
-  </si>
-  <si>
-    <t>16:04:54.245005</t>
-  </si>
-  <si>
-    <t>16:08:01.247051</t>
-  </si>
-  <si>
-    <t>16:01:44.690168</t>
-  </si>
-  <si>
-    <t>14:49:18.088736</t>
-  </si>
-  <si>
-    <t>15:41:09.588406</t>
-  </si>
-  <si>
-    <t>15:34:00.225563</t>
-  </si>
-  <si>
-    <t>13:52:39.415273</t>
-  </si>
-  <si>
-    <t>15:53:20.567292</t>
-  </si>
-  <si>
-    <t>15:34:41.597058</t>
-  </si>
-  <si>
-    <t>16:52:12.667709</t>
-  </si>
-  <si>
-    <t>15:22:53.345618</t>
-  </si>
-  <si>
-    <t>15:05:34.224952</t>
-  </si>
-  <si>
-    <t>15:33:53.946082</t>
-  </si>
-  <si>
-    <t>15:06:37.393391</t>
-  </si>
-  <si>
-    <t>15:55:07.757574</t>
-  </si>
-  <si>
-    <t>15:51:50.480464</t>
-  </si>
-  <si>
-    <t>16:22:11.431654</t>
-  </si>
-  <si>
-    <t>16:01:06.738260</t>
-  </si>
-  <si>
-    <t>16:27:26.479138</t>
-  </si>
-  <si>
-    <t>15:43:25.100229</t>
-  </si>
-  <si>
-    <t>16:37:36.696803</t>
-  </si>
-  <si>
-    <t>15:37:08.559844</t>
-  </si>
-  <si>
-    <t>16:25:06.925333</t>
-  </si>
-  <si>
-    <t>16:04:26.674929</t>
-  </si>
-  <si>
-    <t>16:39:25.556714</t>
-  </si>
-  <si>
-    <t>15:49:11.610937</t>
-  </si>
-  <si>
-    <t>16:57:46.741410</t>
-  </si>
-  <si>
-    <t>16:32:23.081405</t>
-  </si>
-  <si>
-    <t>15:47:59.440474</t>
-  </si>
-  <si>
-    <t>16:25:14.539824</t>
-  </si>
-  <si>
-    <t>15:46:34.032743</t>
-  </si>
-  <si>
-    <t>16:08:28.662275</t>
-  </si>
-  <si>
-    <t>15:40:09.729715</t>
-  </si>
-  <si>
-    <t>16:07:47.361327</t>
-  </si>
-  <si>
-    <t>16:22:11.819024</t>
-  </si>
-  <si>
-    <t>11:57:02.788936</t>
-  </si>
-  <si>
-    <t>16:24:37.857669</t>
-  </si>
-  <si>
-    <t>16:21:24.983794</t>
-  </si>
-  <si>
-    <t>16:12:17.543272</t>
-  </si>
-  <si>
-    <t>16:22:25.412569</t>
-  </si>
-  <si>
-    <t>16:30:02.107360</t>
-  </si>
-  <si>
-    <t>15:52:47.890462</t>
-  </si>
-  <si>
-    <t>15:28:44.705740</t>
-  </si>
-  <si>
-    <t>14:56:09.807046</t>
-  </si>
-  <si>
-    <t>16:03:35.609692</t>
-  </si>
-  <si>
-    <t>14:41:19.822568</t>
-  </si>
-  <si>
-    <t>15:03:30.781108</t>
-  </si>
-  <si>
-    <t>15:27:04.900309</t>
-  </si>
-  <si>
-    <t>15:40:10.026856</t>
-  </si>
-  <si>
-    <t>13:43:04.827074</t>
-  </si>
-  <si>
-    <t>15:51:20.781645</t>
-  </si>
-  <si>
-    <t>15:26:50.684076</t>
-  </si>
-  <si>
-    <t>17:09:42.676444</t>
-  </si>
-  <si>
-    <t>16:44:54.724297</t>
-  </si>
-  <si>
-    <t>15:18:55.178066</t>
-  </si>
-  <si>
-    <t>15:11:33.151773</t>
-  </si>
-  <si>
-    <t>16:37:16.609989</t>
-  </si>
-  <si>
-    <t>17:13:55.078944</t>
-  </si>
-  <si>
-    <t>15:12:49.992999</t>
-  </si>
-  <si>
-    <t>15:31:19.429401</t>
-  </si>
-  <si>
-    <t>15:56:25.834118</t>
-  </si>
-  <si>
-    <t>13:10:27.481895</t>
-  </si>
-  <si>
-    <t>15:38:21.509774</t>
-  </si>
-  <si>
-    <t>15:18:33.322676</t>
-  </si>
-  <si>
-    <t>16:12:57.660147</t>
-  </si>
-  <si>
-    <t>16:32:23.023785</t>
-  </si>
-  <si>
-    <t>16:09:34.177926</t>
-  </si>
-  <si>
-    <t>15:26:30.148804</t>
-  </si>
-  <si>
-    <t>15:09:24.163306</t>
-  </si>
-  <si>
-    <t>15:57:33.861840</t>
-  </si>
-  <si>
-    <t>16:47:47.632751</t>
-  </si>
-  <si>
-    <t>16:57:57.806829</t>
-  </si>
-  <si>
-    <t>15:29:38.808066</t>
-  </si>
-  <si>
-    <t>17:18:33.404750</t>
-  </si>
-  <si>
-    <t>14:34:27.737082</t>
-  </si>
-  <si>
-    <t>16:13:32.836211</t>
-  </si>
-  <si>
-    <t>15:13:13.285806</t>
-  </si>
-  <si>
-    <t>14:26:34.375094</t>
-  </si>
-  <si>
-    <t>14:02:45.232741</t>
-  </si>
-  <si>
-    <t>14:00:16.769886</t>
-  </si>
-  <si>
-    <t>14:07:22.922564</t>
-  </si>
-  <si>
-    <t>16:23:56.124289</t>
-  </si>
-  <si>
-    <t>16:02:33.494864</t>
-  </si>
-  <si>
-    <t>15:51:27.576961</t>
-  </si>
-  <si>
-    <t>15:47:26.284502</t>
-  </si>
-  <si>
-    <t>15:54:31.836313</t>
-  </si>
-  <si>
-    <t>15:51:11.920175</t>
-  </si>
-  <si>
-    <t>14:51:36.153922</t>
-  </si>
-  <si>
-    <t>14:38:53.032086</t>
-  </si>
-  <si>
-    <t>13:05:07.710349</t>
-  </si>
-  <si>
-    <t>15:39:07.324963</t>
-  </si>
-  <si>
-    <t>17:00:34.530992</t>
-  </si>
-  <si>
-    <t>16:43:29.316232</t>
-  </si>
-  <si>
-    <t>16:39:25.338195</t>
-  </si>
-  <si>
-    <t>16:12:56.466012</t>
-  </si>
-  <si>
-    <t>16:54:32.919611</t>
-  </si>
-  <si>
-    <t>16:45:23.811388</t>
-  </si>
-  <si>
-    <t>16:49:11.315120</t>
-  </si>
-  <si>
-    <t>16:44:46.116942</t>
-  </si>
-  <si>
-    <t>14:40:06.211911</t>
-  </si>
-  <si>
-    <t>16:40:35.934108</t>
-  </si>
-  <si>
-    <t>16:56:38.071017</t>
-  </si>
-  <si>
-    <t>15:13:13.194350</t>
-  </si>
-  <si>
-    <t>15:03:15.933216</t>
-  </si>
-  <si>
-    <t>15:29:25.383884</t>
-  </si>
-  <si>
-    <t>13:57:17.150280</t>
-  </si>
-  <si>
-    <t>13:23:01.790943</t>
-  </si>
-  <si>
-    <t>13:36:06.236442</t>
-  </si>
-  <si>
-    <t>13:45:36.228169</t>
-  </si>
-  <si>
-    <t>14:08:44.622333</t>
-  </si>
-  <si>
-    <t>13:49:12.059775</t>
-  </si>
-  <si>
-    <t>14:03:37.897116</t>
-  </si>
-  <si>
-    <t>13:06:55.161330</t>
-  </si>
-  <si>
-    <t>13:22:45.270910</t>
-  </si>
-  <si>
-    <t>13:20:01.541774</t>
-  </si>
-  <si>
-    <t>13:31:10.117006</t>
-  </si>
-  <si>
-    <t>14:06:40.475410</t>
-  </si>
-  <si>
-    <t>15:17:04.264202</t>
-  </si>
-  <si>
-    <t>13:20:39.257708</t>
-  </si>
-  <si>
-    <t>13:27:08.547357</t>
-  </si>
-  <si>
-    <t>13:33:28.824622</t>
-  </si>
-  <si>
-    <t>14:24:27.951946</t>
-  </si>
-  <si>
-    <t>13:23:20.458496</t>
-  </si>
-  <si>
-    <t>13:27:05.763437</t>
-  </si>
-  <si>
-    <t>13:03:58.346825</t>
-  </si>
-  <si>
-    <t>13:01:10.531526</t>
-  </si>
-  <si>
-    <t>13:41:33.875879</t>
-  </si>
-  <si>
-    <t>13:15:57.100593</t>
-  </si>
-  <si>
-    <t>13:49:56.996169</t>
-  </si>
-  <si>
-    <t>13:51:59.941380</t>
-  </si>
-  <si>
-    <t>13:43:33.138961</t>
-  </si>
-  <si>
-    <t>14:21:06.893104</t>
-  </si>
-  <si>
-    <t>14:20:42.716610</t>
+    <t>08:44:56.076311</t>
+  </si>
+  <si>
+    <t>09:08:49.292404</t>
+  </si>
+  <si>
+    <t>09:52:45.083304</t>
+  </si>
+  <si>
+    <t>08:57:43.323259</t>
+  </si>
+  <si>
+    <t>09:37:23.904527</t>
+  </si>
+  <si>
+    <t>09:32:45.169916</t>
+  </si>
+  <si>
+    <t>09:39:16.083556</t>
+  </si>
+  <si>
+    <t>08:59:35.650622</t>
+  </si>
+  <si>
+    <t>10:34:22.643148</t>
+  </si>
+  <si>
+    <t>09:12:38.513020</t>
+  </si>
+  <si>
+    <t>08:17:30.203128</t>
+  </si>
+  <si>
+    <t>08:54:00.106603</t>
+  </si>
+  <si>
+    <t>11:23:56.133169</t>
+  </si>
+  <si>
+    <t>09:37:43.986900</t>
+  </si>
+  <si>
+    <t>08:32:36.719135</t>
+  </si>
+  <si>
+    <t>09:04:41.948562</t>
+  </si>
+  <si>
+    <t>09:23:41.658449</t>
+  </si>
+  <si>
+    <t>07:58:32.421860</t>
+  </si>
+  <si>
+    <t>08:27:39.780082</t>
+  </si>
+  <si>
+    <t>09:14:37.614695</t>
+  </si>
+  <si>
+    <t>09:52:19.570949</t>
+  </si>
+  <si>
+    <t>08:49:54.606218</t>
+  </si>
+  <si>
+    <t>09:13:50.718943</t>
+  </si>
+  <si>
+    <t>08:19:00.309452</t>
+  </si>
+  <si>
+    <t>08:32:43.323930</t>
+  </si>
+  <si>
+    <t>09:18:10.892202</t>
+  </si>
+  <si>
+    <t>09:51:18.801731</t>
+  </si>
+  <si>
+    <t>09:27:58.973466</t>
+  </si>
+  <si>
+    <t>09:47:32.050979</t>
+  </si>
+  <si>
+    <t>09:07:39.708566</t>
+  </si>
+  <si>
+    <t>09:58:42.325393</t>
+  </si>
+  <si>
+    <t>09:09:18.472478</t>
+  </si>
+  <si>
+    <t>09:21:44.776232</t>
+  </si>
+  <si>
+    <t>09:40:42.382560</t>
+  </si>
+  <si>
+    <t>09:10:12.371691</t>
+  </si>
+  <si>
+    <t>09:15:31.925148</t>
+  </si>
+  <si>
+    <t>09:22:17.922378</t>
+  </si>
+  <si>
+    <t>08:45:22.090140</t>
+  </si>
+  <si>
+    <t>09:18:21.993818</t>
+  </si>
+  <si>
+    <t>08:40:30.871125</t>
+  </si>
+  <si>
+    <t>10:09:38.382796</t>
+  </si>
+  <si>
+    <t>09:36:13.492103</t>
+  </si>
+  <si>
+    <t>08:46:15.749895</t>
+  </si>
+  <si>
+    <t>10:22:58.861822</t>
+  </si>
+  <si>
+    <t>09:26:07.470848</t>
+  </si>
+  <si>
+    <t>08:29:21.167685</t>
+  </si>
+  <si>
+    <t>08:37:32.798012</t>
+  </si>
+  <si>
+    <t>09:23:01.346616</t>
+  </si>
+  <si>
+    <t>08:52:52.922852</t>
+  </si>
+  <si>
+    <t>09:47:20.842820</t>
+  </si>
+  <si>
+    <t>09:04:33.240444</t>
+  </si>
+  <si>
+    <t>09:08:17.452018</t>
+  </si>
+  <si>
+    <t>09:06:17.427420</t>
+  </si>
+  <si>
+    <t>09:09:02.039417</t>
+  </si>
+  <si>
+    <t>08:03:56.426603</t>
+  </si>
+  <si>
+    <t>09:51:14.088261</t>
+  </si>
+  <si>
+    <t>08:51:37.209285</t>
+  </si>
+  <si>
+    <t>08:50:11.227424</t>
+  </si>
+  <si>
+    <t>09:01:21.008147</t>
+  </si>
+  <si>
+    <t>08:50:34.510336</t>
+  </si>
+  <si>
+    <t>08:22:58.122847</t>
+  </si>
+  <si>
+    <t>09:02:51.464593</t>
+  </si>
+  <si>
+    <t>09:08:40.933270</t>
+  </si>
+  <si>
+    <t>09:42:38.649328</t>
+  </si>
+  <si>
+    <t>09:12:38.533968</t>
+  </si>
+  <si>
+    <t>09:59:33.804113</t>
+  </si>
+  <si>
+    <t>09:39:38.161252</t>
+  </si>
+  <si>
+    <t>08:58:59.642040</t>
+  </si>
+  <si>
+    <t>08:26:05.475840</t>
+  </si>
+  <si>
+    <t>09:54:58.804431</t>
+  </si>
+  <si>
+    <t>09:11:41.730844</t>
+  </si>
+  <si>
+    <t>09:21:05.552894</t>
+  </si>
+  <si>
+    <t>08:43:22.187975</t>
+  </si>
+  <si>
+    <t>08:35:37.132009</t>
+  </si>
+  <si>
+    <t>08:33:42.660763</t>
+  </si>
+  <si>
+    <t>09:28:21.103396</t>
+  </si>
+  <si>
+    <t>09:54:06.455440</t>
+  </si>
+  <si>
+    <t>08:20:21.987109</t>
+  </si>
+  <si>
+    <t>09:42:27.220395</t>
+  </si>
+  <si>
+    <t>09:06:19.518024</t>
+  </si>
+  <si>
+    <t>09:00:42.839631</t>
+  </si>
+  <si>
+    <t>09:29:26.160106</t>
+  </si>
+  <si>
+    <t>10:54:33.715440</t>
+  </si>
+  <si>
+    <t>09:21:12.775897</t>
+  </si>
+  <si>
+    <t>08:39:38.535644</t>
+  </si>
+  <si>
+    <t>09:51:41.838629</t>
+  </si>
+  <si>
+    <t>08:54:44.381955</t>
+  </si>
+  <si>
+    <t>08:20:40.283669</t>
+  </si>
+  <si>
+    <t>09:04:36.533064</t>
+  </si>
+  <si>
+    <t>09:21:49.170035</t>
+  </si>
+  <si>
+    <t>08:27:51.709500</t>
+  </si>
+  <si>
+    <t>08:34:23.783458</t>
+  </si>
+  <si>
+    <t>09:09:48.268254</t>
+  </si>
+  <si>
+    <t>09:19:48.712390</t>
+  </si>
+  <si>
+    <t>09:25:46.090387</t>
+  </si>
+  <si>
+    <t>09:57:11.191029</t>
+  </si>
+  <si>
+    <t>08:35:07.514437</t>
+  </si>
+  <si>
+    <t>08:43:44.052961</t>
+  </si>
+  <si>
+    <t>08:23:35.588806</t>
+  </si>
+  <si>
+    <t>08:08:35.701825</t>
+  </si>
+  <si>
+    <t>09:55:52.929607</t>
+  </si>
+  <si>
+    <t>08:38:42.301976</t>
+  </si>
+  <si>
+    <t>09:44:54.807011</t>
+  </si>
+  <si>
+    <t>08:41:22.741896</t>
+  </si>
+  <si>
+    <t>08:39:40.003041</t>
+  </si>
+  <si>
+    <t>09:29:09.542679</t>
+  </si>
+  <si>
+    <t>08:51:49.967029</t>
+  </si>
+  <si>
+    <t>09:36:59.826858</t>
+  </si>
+  <si>
+    <t>08:45:19.128855</t>
+  </si>
+  <si>
+    <t>09:54:40.692817</t>
+  </si>
+  <si>
+    <t>08:57:36.944221</t>
+  </si>
+  <si>
+    <t>09:40:58.928505</t>
+  </si>
+  <si>
+    <t>07:58:02.700748</t>
+  </si>
+  <si>
+    <t>09:19:45.063719</t>
+  </si>
+  <si>
+    <t>08:50:39.195865</t>
+  </si>
+  <si>
+    <t>09:16:36.053258</t>
+  </si>
+  <si>
+    <t>09:26:56.761882</t>
+  </si>
+  <si>
+    <t>09:23:56.106995</t>
+  </si>
+  <si>
+    <t>08:45:44.397556</t>
+  </si>
+  <si>
+    <t>09:12:52.073702</t>
+  </si>
+  <si>
+    <t>08:11:52.858113</t>
+  </si>
+  <si>
+    <t>08:15:38.687650</t>
+  </si>
+  <si>
+    <t>09:36:19.923965</t>
+  </si>
+  <si>
+    <t>09:52:34.306486</t>
+  </si>
+  <si>
+    <t>10:13:23.514701</t>
+  </si>
+  <si>
+    <t>09:31:28.729061</t>
+  </si>
+  <si>
+    <t>10:20:54.486005</t>
+  </si>
+  <si>
+    <t>10:05:32.484035</t>
+  </si>
+  <si>
+    <t>09:26:44.747326</t>
+  </si>
+  <si>
+    <t>08:18:55.144266</t>
+  </si>
+  <si>
+    <t>09:15:23.944976</t>
+  </si>
+  <si>
+    <t>09:02:45.684635</t>
+  </si>
+  <si>
+    <t>08:27:31.885898</t>
+  </si>
+  <si>
+    <t>08:39:01.660995</t>
+  </si>
+  <si>
+    <t>08:51:20.984742</t>
+  </si>
+  <si>
+    <t>08:59:35.453798</t>
+  </si>
+  <si>
+    <t>08:43:16.031683</t>
+  </si>
+  <si>
+    <t>08:19:39.364721</t>
+  </si>
+  <si>
+    <t>09:01:57.535919</t>
+  </si>
+  <si>
+    <t>09:08:39.199474</t>
+  </si>
+  <si>
+    <t>09:11:15.197159</t>
+  </si>
+  <si>
+    <t>08:43:01.199406</t>
+  </si>
+  <si>
+    <t>09:25:58.358052</t>
+  </si>
+  <si>
+    <t>09:07:44.560239</t>
+  </si>
+  <si>
+    <t>08:37:32.056130</t>
+  </si>
+  <si>
+    <t>08:59:10.190732</t>
+  </si>
+  <si>
+    <t>10:02:59.208925</t>
+  </si>
+  <si>
+    <t>08:20:15.813457</t>
+  </si>
+  <si>
+    <t>09:40:42.560745</t>
+  </si>
+  <si>
+    <t>08:28:55.575851</t>
+  </si>
+  <si>
+    <t>09:18:15.204226</t>
+  </si>
+  <si>
+    <t>08:37:37.739213</t>
+  </si>
+  <si>
+    <t>08:56:16.555276</t>
+  </si>
+  <si>
+    <t>09:00:59.799279</t>
+  </si>
+  <si>
+    <t>08:59:29.016096</t>
+  </si>
+  <si>
+    <t>09:50:20.921490</t>
+  </si>
+  <si>
+    <t>08:39:14.312994</t>
+  </si>
+  <si>
+    <t>08:43:00.982361</t>
+  </si>
+  <si>
+    <t>08:57:59.017024</t>
+  </si>
+  <si>
+    <t>09:23:04.879568</t>
+  </si>
+  <si>
+    <t>09:26:02.839941</t>
+  </si>
+  <si>
+    <t>08:50:53.767119</t>
+  </si>
+  <si>
+    <t>14:56:48.551892</t>
+  </si>
+  <si>
+    <t>14:31:16.288159</t>
+  </si>
+  <si>
+    <t>12:37:42.980959</t>
+  </si>
+  <si>
+    <t>15:15:02.049367</t>
+  </si>
+  <si>
+    <t>13:32:42.334638</t>
+  </si>
+  <si>
+    <t>16:11:15.787463</t>
+  </si>
+  <si>
+    <t>15:49:36.287865</t>
+  </si>
+  <si>
+    <t>16:52:06.182091</t>
+  </si>
+  <si>
+    <t>15:01:51.701482</t>
+  </si>
+  <si>
+    <t>15:37:04.978769</t>
+  </si>
+  <si>
+    <t>15:57:30.146861</t>
+  </si>
+  <si>
+    <t>16:37:55.066669</t>
+  </si>
+  <si>
+    <t>15:37:38.296958</t>
+  </si>
+  <si>
+    <t>16:16:45.213056</t>
+  </si>
+  <si>
+    <t>15:57:46.548797</t>
+  </si>
+  <si>
+    <t>14:08:33.598913</t>
+  </si>
+  <si>
+    <t>16:17:36.596458</t>
+  </si>
+  <si>
+    <t>16:05:58.922024</t>
+  </si>
+  <si>
+    <t>16:02:36.708826</t>
+  </si>
+  <si>
+    <t>16:11:57.351444</t>
+  </si>
+  <si>
+    <t>15:45:59.609826</t>
+  </si>
+  <si>
+    <t>16:11:00.429091</t>
+  </si>
+  <si>
+    <t>15:43:08.329165</t>
+  </si>
+  <si>
+    <t>16:25:42.983293</t>
+  </si>
+  <si>
+    <t>13:53:59.641435</t>
+  </si>
+  <si>
+    <t>16:22:41.934748</t>
+  </si>
+  <si>
+    <t>16:44:32.748570</t>
+  </si>
+  <si>
+    <t>15:46:34.518932</t>
+  </si>
+  <si>
+    <t>16:12:04.076299</t>
+  </si>
+  <si>
+    <t>14:55:45.414272</t>
+  </si>
+  <si>
+    <t>15:48:43.718448</t>
+  </si>
+  <si>
+    <t>15:22:56.779853</t>
+  </si>
+  <si>
+    <t>15:41:26.588900</t>
+  </si>
+  <si>
+    <t>15:20:40.386500</t>
+  </si>
+  <si>
+    <t>15:25:20.191888</t>
+  </si>
+  <si>
+    <t>14:10:05.946030</t>
+  </si>
+  <si>
+    <t>16:13:07.801141</t>
+  </si>
+  <si>
+    <t>15:22:54.071040</t>
+  </si>
+  <si>
+    <t>14:56:20.742050</t>
+  </si>
+  <si>
+    <t>16:10:04.770986</t>
+  </si>
+  <si>
+    <t>15:35:06.465479</t>
+  </si>
+  <si>
+    <t>15:45:35.907085</t>
+  </si>
+  <si>
+    <t>16:20:37.208572</t>
+  </si>
+  <si>
+    <t>14:29:32.526252</t>
+  </si>
+  <si>
+    <t>14:08:05.173239</t>
+  </si>
+  <si>
+    <t>16:49:12.397948</t>
+  </si>
+  <si>
+    <t>15:10:33.194496</t>
+  </si>
+  <si>
+    <t>17:12:38.129997</t>
+  </si>
+  <si>
+    <t>16:14:49.799784</t>
+  </si>
+  <si>
+    <t>16:28:46.603028</t>
+  </si>
+  <si>
+    <t>15:50:25.660996</t>
+  </si>
+  <si>
+    <t>15:38:37.219034</t>
+  </si>
+  <si>
+    <t>15:59:18.638005</t>
+  </si>
+  <si>
+    <t>16:00:16.740426</t>
+  </si>
+  <si>
+    <t>16:34:01.337617</t>
+  </si>
+  <si>
+    <t>16:14:33.945909</t>
+  </si>
+  <si>
+    <t>17:12:35.006567</t>
+  </si>
+  <si>
+    <t>14:12:45.164454</t>
+  </si>
+  <si>
+    <t>16:15:08.257386</t>
+  </si>
+  <si>
+    <t>14:59:43.087952</t>
+  </si>
+  <si>
+    <t>16:23:00.778690</t>
+  </si>
+  <si>
+    <t>15:16:27.293934</t>
+  </si>
+  <si>
+    <t>15:57:23.777005</t>
+  </si>
+  <si>
+    <t>16:17:38.917337</t>
+  </si>
+  <si>
+    <t>15:58:15.156174</t>
+  </si>
+  <si>
+    <t>14:19:12.079218</t>
+  </si>
+  <si>
+    <t>14:51:18.447781</t>
+  </si>
+  <si>
+    <t>13:25:46.326851</t>
+  </si>
+  <si>
+    <t>14:57:13.159927</t>
+  </si>
+  <si>
+    <t>16:05:49.634636</t>
+  </si>
+  <si>
+    <t>16:20:35.283434</t>
+  </si>
+  <si>
+    <t>15:07:17.203680</t>
+  </si>
+  <si>
+    <t>15:32:39.944421</t>
+  </si>
+  <si>
+    <t>17:23:55.853172</t>
+  </si>
+  <si>
+    <t>13:28:36.781595</t>
+  </si>
+  <si>
+    <t>16:41:01.740378</t>
+  </si>
+  <si>
+    <t>15:19:00.792986</t>
+  </si>
+  <si>
+    <t>14:38:09.978796</t>
+  </si>
+  <si>
+    <t>16:44:01.551357</t>
+  </si>
+  <si>
+    <t>16:51:27.988951</t>
+  </si>
+  <si>
+    <t>16:01:13.953039</t>
+  </si>
+  <si>
+    <t>15:37:43.933627</t>
+  </si>
+  <si>
+    <t>14:41:55.414467</t>
+  </si>
+  <si>
+    <t>16:18:52.990154</t>
+  </si>
+  <si>
+    <t>17:06:39.315469</t>
+  </si>
+  <si>
+    <t>14:46:08.514190</t>
+  </si>
+  <si>
+    <t>16:55:04.633951</t>
+  </si>
+  <si>
+    <t>17:44:44.705757</t>
+  </si>
+  <si>
+    <t>14:56:53.631465</t>
+  </si>
+  <si>
+    <t>16:27:51.731083</t>
+  </si>
+  <si>
+    <t>17:08:57.310311</t>
+  </si>
+  <si>
+    <t>16:43:49.774427</t>
+  </si>
+  <si>
+    <t>14:39:53.003591</t>
+  </si>
+  <si>
+    <t>14:06:45.393542</t>
+  </si>
+  <si>
+    <t>16:09:21.944538</t>
+  </si>
+  <si>
+    <t>16:21:08.478138</t>
+  </si>
+  <si>
+    <t>14:04:32.506537</t>
+  </si>
+  <si>
+    <t>16:31:31.009412</t>
+  </si>
+  <si>
+    <t>15:19:20.325896</t>
+  </si>
+  <si>
+    <t>16:35:36.279088</t>
+  </si>
+  <si>
+    <t>15:28:33.283616</t>
+  </si>
+  <si>
+    <t>16:45:35.021299</t>
+  </si>
+  <si>
+    <t>16:10:49.933871</t>
+  </si>
+  <si>
+    <t>17:14:23.049060</t>
+  </si>
+  <si>
+    <t>15:06:13.401665</t>
+  </si>
+  <si>
+    <t>15:54:52.475895</t>
+  </si>
+  <si>
+    <t>15:00:48.389638</t>
+  </si>
+  <si>
+    <t>16:20:46.945450</t>
+  </si>
+  <si>
+    <t>14:17:19.577304</t>
+  </si>
+  <si>
+    <t>13:46:34.693942</t>
+  </si>
+  <si>
+    <t>14:31:46.916249</t>
+  </si>
+  <si>
+    <t>14:43:49.625929</t>
+  </si>
+  <si>
+    <t>14:27:34.979268</t>
+  </si>
+  <si>
+    <t>13:50:45.677050</t>
+  </si>
+  <si>
+    <t>14:14:34.594951</t>
+  </si>
+  <si>
+    <t>14:47:46.709468</t>
+  </si>
+  <si>
+    <t>14:39:34.705616</t>
+  </si>
+  <si>
+    <t>15:27:12.330372</t>
+  </si>
+  <si>
+    <t>13:52:06.671633</t>
+  </si>
+  <si>
+    <t>13:59:25.251118</t>
+  </si>
+  <si>
+    <t>13:19:25.317076</t>
+  </si>
+  <si>
+    <t>13:34:32.715759</t>
+  </si>
+  <si>
+    <t>12:53:32.991516</t>
+  </si>
+  <si>
+    <t>13:26:27.849009</t>
+  </si>
+  <si>
+    <t>14:41:35.209338</t>
+  </si>
+  <si>
+    <t>14:11:45.325363</t>
+  </si>
+  <si>
+    <t>14:57:43.596891</t>
+  </si>
+  <si>
+    <t>13:42:41.943625</t>
+  </si>
+  <si>
+    <t>13:40:07.276655</t>
+  </si>
+  <si>
+    <t>13:21:45.532112</t>
+  </si>
+  <si>
+    <t>13:32:56.169286</t>
+  </si>
+  <si>
+    <t>14:12:51.609662</t>
+  </si>
+  <si>
+    <t>14:34:26.507658</t>
+  </si>
+  <si>
+    <t>14:17:47.452204</t>
+  </si>
+  <si>
+    <t>14:13:47.066164</t>
+  </si>
+  <si>
+    <t>13:26:18.970153</t>
+  </si>
+  <si>
+    <t>14:16:19.205757</t>
+  </si>
+  <si>
+    <t>14:59:34.612468</t>
   </si>
   <si>
     <t>Commercial</t>
@@ -1323,7 +1323,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>10.62493565731922</v>
+        <v>25.64894717740552</v>
       </c>
       <c r="D2" t="s">
         <v>304</v>
@@ -1340,7 +1340,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>14.53904241283856</v>
+        <v>8.69537900683539</v>
       </c>
       <c r="D3" t="s">
         <v>304</v>
@@ -1357,7 +1357,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>19.03117611864149</v>
+        <v>15.07390635251245</v>
       </c>
       <c r="D4" t="s">
         <v>304</v>
@@ -1374,7 +1374,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>30.8477610505668</v>
+        <v>24.04700950792275</v>
       </c>
       <c r="D5" t="s">
         <v>304</v>
@@ -1391,7 +1391,7 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>24.2608643358399</v>
+        <v>17.53865851798879</v>
       </c>
       <c r="D6" t="s">
         <v>304</v>
@@ -1408,7 +1408,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>18.34349260006124</v>
+        <v>18.64950227855184</v>
       </c>
       <c r="D7" t="s">
         <v>304</v>
@@ -1425,7 +1425,7 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>33.49782131788171</v>
+        <v>35.7874968056983</v>
       </c>
       <c r="D8" t="s">
         <v>304</v>
@@ -1442,7 +1442,7 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>10.34801307998227</v>
+        <v>11.4712729259623</v>
       </c>
       <c r="D9" t="s">
         <v>304</v>
@@ -1459,7 +1459,7 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>15.74748372490442</v>
+        <v>5.189705016439719</v>
       </c>
       <c r="D10" t="s">
         <v>304</v>
@@ -1476,7 +1476,7 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>19.40651519611782</v>
+        <v>8.553803418938388</v>
       </c>
       <c r="D11" t="s">
         <v>304</v>
@@ -1493,7 +1493,7 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>13.72697722506443</v>
+        <v>11.05894427208481</v>
       </c>
       <c r="D12" t="s">
         <v>304</v>
@@ -1510,7 +1510,7 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>27.81016108599564</v>
+        <v>18.68040824889137</v>
       </c>
       <c r="D13" t="s">
         <v>304</v>
@@ -1527,7 +1527,7 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>8.045866853592816</v>
+        <v>22.26092233502204</v>
       </c>
       <c r="D14" t="s">
         <v>304</v>
@@ -1544,7 +1544,7 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>27.25161208362785</v>
+        <v>30.29498665606152</v>
       </c>
       <c r="D15" t="s">
         <v>304</v>
@@ -1561,7 +1561,7 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>18.1614724988786</v>
+        <v>15.45022242110749</v>
       </c>
       <c r="D16" t="s">
         <v>304</v>
@@ -1578,7 +1578,7 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>13.0865675123585</v>
+        <v>20.41244441746118</v>
       </c>
       <c r="D17" t="s">
         <v>304</v>
@@ -1595,7 +1595,7 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>6.808453769648169</v>
+        <v>15.77107055888309</v>
       </c>
       <c r="D18" t="s">
         <v>304</v>
@@ -1612,7 +1612,7 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>15.01687362743495</v>
+        <v>24.35798641915008</v>
       </c>
       <c r="D19" t="s">
         <v>304</v>
@@ -1629,7 +1629,7 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>23.74391111178679</v>
+        <v>25.08316042007836</v>
       </c>
       <c r="D20" t="s">
         <v>304</v>
@@ -1646,7 +1646,7 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>30.47604789936897</v>
+        <v>19.1919593729599</v>
       </c>
       <c r="D21" t="s">
         <v>304</v>
@@ -1663,7 +1663,7 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>27.94913904904104</v>
+        <v>12.69103771029879</v>
       </c>
       <c r="D22" t="s">
         <v>304</v>
@@ -1680,7 +1680,7 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>16.32061889088802</v>
+        <v>16.22365080033379</v>
       </c>
       <c r="D23" t="s">
         <v>304</v>
@@ -1697,7 +1697,7 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>17.23479101740962</v>
+        <v>16.64314065685874</v>
       </c>
       <c r="D24" t="s">
         <v>304</v>
@@ -1714,7 +1714,7 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>24.04311866230719</v>
+        <v>19.80153385910189</v>
       </c>
       <c r="D25" t="s">
         <v>304</v>
@@ -1731,7 +1731,7 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>18.09280927175337</v>
+        <v>9.786833860802219</v>
       </c>
       <c r="D26" t="s">
         <v>304</v>
@@ -1748,7 +1748,7 @@
         <v>29</v>
       </c>
       <c r="C27">
-        <v>31.10484867144665</v>
+        <v>15.32126163202147</v>
       </c>
       <c r="D27" t="s">
         <v>304</v>
@@ -1765,7 +1765,7 @@
         <v>30</v>
       </c>
       <c r="C28">
-        <v>24.98524520509623</v>
+        <v>29.42399504993038</v>
       </c>
       <c r="D28" t="s">
         <v>304</v>
@@ -1782,7 +1782,7 @@
         <v>31</v>
       </c>
       <c r="C29">
-        <v>12.11432262919</v>
+        <v>32.85929513772472</v>
       </c>
       <c r="D29" t="s">
         <v>304</v>
@@ -1799,7 +1799,7 @@
         <v>32</v>
       </c>
       <c r="C30">
-        <v>14.53912193751514</v>
+        <v>19.70722939678171</v>
       </c>
       <c r="D30" t="s">
         <v>304</v>
@@ -1816,7 +1816,7 @@
         <v>33</v>
       </c>
       <c r="C31">
-        <v>27.87309749295849</v>
+        <v>15.18861461846694</v>
       </c>
       <c r="D31" t="s">
         <v>304</v>
@@ -1833,7 +1833,7 @@
         <v>34</v>
       </c>
       <c r="C32">
-        <v>9.881917889059366</v>
+        <v>9.159880558489974</v>
       </c>
       <c r="D32" t="s">
         <v>304</v>
@@ -1850,7 +1850,7 @@
         <v>35</v>
       </c>
       <c r="C33">
-        <v>9.130352381493477</v>
+        <v>32.35567884280525</v>
       </c>
       <c r="D33" t="s">
         <v>304</v>
@@ -1867,7 +1867,7 @@
         <v>36</v>
       </c>
       <c r="C34">
-        <v>25.8202232380225</v>
+        <v>28.3793788858196</v>
       </c>
       <c r="D34" t="s">
         <v>304</v>
@@ -1884,7 +1884,7 @@
         <v>37</v>
       </c>
       <c r="C35">
-        <v>7.226849043446798</v>
+        <v>8.331495912564986</v>
       </c>
       <c r="D35" t="s">
         <v>304</v>
@@ -1901,7 +1901,7 @@
         <v>38</v>
       </c>
       <c r="C36">
-        <v>6.93059005787077</v>
+        <v>20.48964433248239</v>
       </c>
       <c r="D36" t="s">
         <v>304</v>
@@ -1918,7 +1918,7 @@
         <v>39</v>
       </c>
       <c r="C37">
-        <v>22.55618663016778</v>
+        <v>20.00814885739897</v>
       </c>
       <c r="D37" t="s">
         <v>304</v>
@@ -1935,7 +1935,7 @@
         <v>40</v>
       </c>
       <c r="C38">
-        <v>19.93163627751165</v>
+        <v>14.91671238005315</v>
       </c>
       <c r="D38" t="s">
         <v>304</v>
@@ -1952,7 +1952,7 @@
         <v>41</v>
       </c>
       <c r="C39">
-        <v>27.72841404203791</v>
+        <v>24.32641991752113</v>
       </c>
       <c r="D39" t="s">
         <v>304</v>
@@ -1969,7 +1969,7 @@
         <v>42</v>
       </c>
       <c r="C40">
-        <v>21.4847869989073</v>
+        <v>12.87516836434972</v>
       </c>
       <c r="D40" t="s">
         <v>304</v>
@@ -1986,7 +1986,7 @@
         <v>43</v>
       </c>
       <c r="C41">
-        <v>27.66110842834475</v>
+        <v>10.31650882092271</v>
       </c>
       <c r="D41" t="s">
         <v>304</v>
@@ -2003,7 +2003,7 @@
         <v>44</v>
       </c>
       <c r="C42">
-        <v>24.12663160588597</v>
+        <v>17.4531787701833</v>
       </c>
       <c r="D42" t="s">
         <v>304</v>
@@ -2020,7 +2020,7 @@
         <v>45</v>
       </c>
       <c r="C43">
-        <v>28.60169848622517</v>
+        <v>20.9510958357323</v>
       </c>
       <c r="D43" t="s">
         <v>304</v>
@@ -2037,7 +2037,7 @@
         <v>46</v>
       </c>
       <c r="C44">
-        <v>30.77226080809823</v>
+        <v>30.09932282202822</v>
       </c>
       <c r="D44" t="s">
         <v>304</v>
@@ -2054,7 +2054,7 @@
         <v>47</v>
       </c>
       <c r="C45">
-        <v>23.49154807065849</v>
+        <v>45.7371220361884</v>
       </c>
       <c r="D45" t="s">
         <v>304</v>
@@ -2071,7 +2071,7 @@
         <v>48</v>
       </c>
       <c r="C46">
-        <v>27.45581758198285</v>
+        <v>6.123475044245216</v>
       </c>
       <c r="D46" t="s">
         <v>304</v>
@@ -2088,7 +2088,7 @@
         <v>49</v>
       </c>
       <c r="C47">
-        <v>14.56865662280463</v>
+        <v>20.61385698818949</v>
       </c>
       <c r="D47" t="s">
         <v>304</v>
@@ -2105,7 +2105,7 @@
         <v>50</v>
       </c>
       <c r="C48">
-        <v>17.09033880690174</v>
+        <v>24.65298438753486</v>
       </c>
       <c r="D48" t="s">
         <v>304</v>
@@ -2122,7 +2122,7 @@
         <v>51</v>
       </c>
       <c r="C49">
-        <v>10.70041894559732</v>
+        <v>33.03498745531098</v>
       </c>
       <c r="D49" t="s">
         <v>304</v>
@@ -2139,7 +2139,7 @@
         <v>52</v>
       </c>
       <c r="C50">
-        <v>31.09941691614317</v>
+        <v>11.95204577532084</v>
       </c>
       <c r="D50" t="s">
         <v>304</v>
@@ -2156,7 +2156,7 @@
         <v>53</v>
       </c>
       <c r="C51">
-        <v>20.45046643647282</v>
+        <v>16.16896093973493</v>
       </c>
       <c r="D51" t="s">
         <v>304</v>
@@ -2173,7 +2173,7 @@
         <v>54</v>
       </c>
       <c r="C52">
-        <v>38.83230897755572</v>
+        <v>8.398046501994507</v>
       </c>
       <c r="D52" t="s">
         <v>304</v>
@@ -2190,7 +2190,7 @@
         <v>55</v>
       </c>
       <c r="C53">
-        <v>15.78638346610647</v>
+        <v>18.56490226119628</v>
       </c>
       <c r="D53" t="s">
         <v>304</v>
@@ -2207,7 +2207,7 @@
         <v>56</v>
       </c>
       <c r="C54">
-        <v>61.98732984790269</v>
+        <v>17.09099202516259</v>
       </c>
       <c r="D54" t="s">
         <v>304</v>
@@ -2224,7 +2224,7 @@
         <v>57</v>
       </c>
       <c r="C55">
-        <v>15.37259552442258</v>
+        <v>19.40287860212054</v>
       </c>
       <c r="D55" t="s">
         <v>304</v>
@@ -2241,7 +2241,7 @@
         <v>58</v>
       </c>
       <c r="C56">
-        <v>14.01222896303962</v>
+        <v>21.7074463168917</v>
       </c>
       <c r="D56" t="s">
         <v>304</v>
@@ -2258,7 +2258,7 @@
         <v>59</v>
       </c>
       <c r="C57">
-        <v>17.5501328376184</v>
+        <v>26.36478160405575</v>
       </c>
       <c r="D57" t="s">
         <v>304</v>
@@ -2275,7 +2275,7 @@
         <v>60</v>
       </c>
       <c r="C58">
-        <v>11.35138118941616</v>
+        <v>23.57751978515208</v>
       </c>
       <c r="D58" t="s">
         <v>304</v>
@@ -2292,7 +2292,7 @@
         <v>61</v>
       </c>
       <c r="C59">
-        <v>18.73081348290066</v>
+        <v>21.91354396256821</v>
       </c>
       <c r="D59" t="s">
         <v>304</v>
@@ -2309,7 +2309,7 @@
         <v>62</v>
       </c>
       <c r="C60">
-        <v>24.94746492115626</v>
+        <v>13.91693967044074</v>
       </c>
       <c r="D60" t="s">
         <v>304</v>
@@ -2326,7 +2326,7 @@
         <v>63</v>
       </c>
       <c r="C61">
-        <v>23.12923626574663</v>
+        <v>15.12251312629735</v>
       </c>
       <c r="D61" t="s">
         <v>304</v>
@@ -2343,7 +2343,7 @@
         <v>64</v>
       </c>
       <c r="C62">
-        <v>9.165336182346795</v>
+        <v>20.08226658020972</v>
       </c>
       <c r="D62" t="s">
         <v>304</v>
@@ -2360,7 +2360,7 @@
         <v>65</v>
       </c>
       <c r="C63">
-        <v>10.85869190112578</v>
+        <v>33.02014764340967</v>
       </c>
       <c r="D63" t="s">
         <v>304</v>
@@ -2377,7 +2377,7 @@
         <v>66</v>
       </c>
       <c r="C64">
-        <v>15.67239897731105</v>
+        <v>18.94530935157381</v>
       </c>
       <c r="D64" t="s">
         <v>304</v>
@@ -2394,7 +2394,7 @@
         <v>67</v>
       </c>
       <c r="C65">
-        <v>58.33940314627879</v>
+        <v>17.2182914932079</v>
       </c>
       <c r="D65" t="s">
         <v>304</v>
@@ -2411,7 +2411,7 @@
         <v>68</v>
       </c>
       <c r="C66">
-        <v>12.84348807917135</v>
+        <v>11.23604893746763</v>
       </c>
       <c r="D66" t="s">
         <v>304</v>
@@ -2428,7 +2428,7 @@
         <v>69</v>
       </c>
       <c r="C67">
-        <v>35.93149085447277</v>
+        <v>20.3718167000806</v>
       </c>
       <c r="D67" t="s">
         <v>304</v>
@@ -2445,7 +2445,7 @@
         <v>70</v>
       </c>
       <c r="C68">
-        <v>17.01966012221579</v>
+        <v>20.02469402057949</v>
       </c>
       <c r="D68" t="s">
         <v>304</v>
@@ -2462,7 +2462,7 @@
         <v>71</v>
       </c>
       <c r="C69">
-        <v>11.96353108238856</v>
+        <v>51.46260130288224</v>
       </c>
       <c r="D69" t="s">
         <v>304</v>
@@ -2479,7 +2479,7 @@
         <v>72</v>
       </c>
       <c r="C70">
-        <v>16.51654970882473</v>
+        <v>12.59694326983675</v>
       </c>
       <c r="D70" t="s">
         <v>304</v>
@@ -2496,7 +2496,7 @@
         <v>73</v>
       </c>
       <c r="C71">
-        <v>23.30139278455457</v>
+        <v>25.01956403346357</v>
       </c>
       <c r="D71" t="s">
         <v>304</v>
@@ -2513,7 +2513,7 @@
         <v>74</v>
       </c>
       <c r="C72">
-        <v>15.83030467880147</v>
+        <v>28.84973082982488</v>
       </c>
       <c r="D72" t="s">
         <v>304</v>
@@ -2530,7 +2530,7 @@
         <v>75</v>
       </c>
       <c r="C73">
-        <v>17.28897262664552</v>
+        <v>26.48905104003878</v>
       </c>
       <c r="D73" t="s">
         <v>304</v>
@@ -2547,7 +2547,7 @@
         <v>76</v>
       </c>
       <c r="C74">
-        <v>26.5314260972011</v>
+        <v>28.89264447755732</v>
       </c>
       <c r="D74" t="s">
         <v>304</v>
@@ -2564,7 +2564,7 @@
         <v>77</v>
       </c>
       <c r="C75">
-        <v>21.62268043601733</v>
+        <v>48.18204542672005</v>
       </c>
       <c r="D75" t="s">
         <v>304</v>
@@ -2581,7 +2581,7 @@
         <v>78</v>
       </c>
       <c r="C76">
-        <v>25.48228966006809</v>
+        <v>24.4148178835197</v>
       </c>
       <c r="D76" t="s">
         <v>304</v>
@@ -2598,7 +2598,7 @@
         <v>79</v>
       </c>
       <c r="C77">
-        <v>25.48312128176573</v>
+        <v>14.57640117447283</v>
       </c>
       <c r="D77" t="s">
         <v>304</v>
@@ -2615,7 +2615,7 @@
         <v>80</v>
       </c>
       <c r="C78">
-        <v>23.07694526178345</v>
+        <v>20.42604952603678</v>
       </c>
       <c r="D78" t="s">
         <v>304</v>
@@ -2632,7 +2632,7 @@
         <v>81</v>
       </c>
       <c r="C79">
-        <v>25.89656059707141</v>
+        <v>27.36768116542062</v>
       </c>
       <c r="D79" t="s">
         <v>304</v>
@@ -2649,7 +2649,7 @@
         <v>82</v>
       </c>
       <c r="C80">
-        <v>37.21777639246964</v>
+        <v>28.29771527872879</v>
       </c>
       <c r="D80" t="s">
         <v>304</v>
@@ -2666,7 +2666,7 @@
         <v>83</v>
       </c>
       <c r="C81">
-        <v>23.33764403411857</v>
+        <v>7.860207504707619</v>
       </c>
       <c r="D81" t="s">
         <v>304</v>
@@ -2683,7 +2683,7 @@
         <v>84</v>
       </c>
       <c r="C82">
-        <v>19.0379747843074</v>
+        <v>16.61205502484095</v>
       </c>
       <c r="D82" t="s">
         <v>304</v>
@@ -2700,7 +2700,7 @@
         <v>85</v>
       </c>
       <c r="C83">
-        <v>23.23810696728879</v>
+        <v>20.06879006712706</v>
       </c>
       <c r="D83" t="s">
         <v>304</v>
@@ -2717,7 +2717,7 @@
         <v>86</v>
       </c>
       <c r="C84">
-        <v>21.00165019461683</v>
+        <v>27.57598514977213</v>
       </c>
       <c r="D84" t="s">
         <v>304</v>
@@ -2734,7 +2734,7 @@
         <v>87</v>
       </c>
       <c r="C85">
-        <v>16.05173288332218</v>
+        <v>12.58245738987267</v>
       </c>
       <c r="D85" t="s">
         <v>304</v>
@@ -2751,7 +2751,7 @@
         <v>88</v>
       </c>
       <c r="C86">
-        <v>15.48883675624109</v>
+        <v>17.32765572808212</v>
       </c>
       <c r="D86" t="s">
         <v>304</v>
@@ -2768,7 +2768,7 @@
         <v>89</v>
       </c>
       <c r="C87">
-        <v>18.66517413307471</v>
+        <v>41.32857078679724</v>
       </c>
       <c r="D87" t="s">
         <v>304</v>
@@ -2785,7 +2785,7 @@
         <v>90</v>
       </c>
       <c r="C88">
-        <v>15.41059767968722</v>
+        <v>25.1952677047797</v>
       </c>
       <c r="D88" t="s">
         <v>304</v>
@@ -2802,7 +2802,7 @@
         <v>91</v>
       </c>
       <c r="C89">
-        <v>16.36465116810723</v>
+        <v>26.6503940272694</v>
       </c>
       <c r="D89" t="s">
         <v>304</v>
@@ -2819,7 +2819,7 @@
         <v>92</v>
       </c>
       <c r="C90">
-        <v>11.34083688774837</v>
+        <v>28.04476681130969</v>
       </c>
       <c r="D90" t="s">
         <v>304</v>
@@ -2836,7 +2836,7 @@
         <v>93</v>
       </c>
       <c r="C91">
-        <v>15.95189824110598</v>
+        <v>31.46252051967017</v>
       </c>
       <c r="D91" t="s">
         <v>304</v>
@@ -2853,7 +2853,7 @@
         <v>94</v>
       </c>
       <c r="C92">
-        <v>18.68652127800559</v>
+        <v>26.06264200742348</v>
       </c>
       <c r="D92" t="s">
         <v>304</v>
@@ -2870,7 +2870,7 @@
         <v>95</v>
       </c>
       <c r="C93">
-        <v>26.36116783772735</v>
+        <v>14.90115369791407</v>
       </c>
       <c r="D93" t="s">
         <v>304</v>
@@ -2887,7 +2887,7 @@
         <v>96</v>
       </c>
       <c r="C94">
-        <v>28.27117887622528</v>
+        <v>19.97343328348679</v>
       </c>
       <c r="D94" t="s">
         <v>304</v>
@@ -2904,7 +2904,7 @@
         <v>97</v>
       </c>
       <c r="C95">
-        <v>18.81309927475954</v>
+        <v>30.70890768606276</v>
       </c>
       <c r="D95" t="s">
         <v>304</v>
@@ -2921,7 +2921,7 @@
         <v>98</v>
       </c>
       <c r="C96">
-        <v>17.59062650780177</v>
+        <v>37.27499494448268</v>
       </c>
       <c r="D96" t="s">
         <v>304</v>
@@ -2938,7 +2938,7 @@
         <v>99</v>
       </c>
       <c r="C97">
-        <v>24.11815927884378</v>
+        <v>6.339934780984704</v>
       </c>
       <c r="D97" t="s">
         <v>304</v>
@@ -2955,7 +2955,7 @@
         <v>100</v>
       </c>
       <c r="C98">
-        <v>13.01639041027249</v>
+        <v>42.76590315183917</v>
       </c>
       <c r="D98" t="s">
         <v>304</v>
@@ -2972,7 +2972,7 @@
         <v>101</v>
       </c>
       <c r="C99">
-        <v>26.26251635594033</v>
+        <v>25.61744067782984</v>
       </c>
       <c r="D99" t="s">
         <v>304</v>
@@ -2989,7 +2989,7 @@
         <v>102</v>
       </c>
       <c r="C100">
-        <v>40.47517002260965</v>
+        <v>14.60923203317112</v>
       </c>
       <c r="D100" t="s">
         <v>304</v>
@@ -3006,7 +3006,7 @@
         <v>103</v>
       </c>
       <c r="C101">
-        <v>12.71051215698959</v>
+        <v>33.99857118959041</v>
       </c>
       <c r="D101" t="s">
         <v>304</v>
@@ -3023,7 +3023,7 @@
         <v>104</v>
       </c>
       <c r="C102">
-        <v>34.04360724646395</v>
+        <v>49.17277081913121</v>
       </c>
       <c r="D102" t="s">
         <v>304</v>
@@ -3040,7 +3040,7 @@
         <v>105</v>
       </c>
       <c r="C103">
-        <v>17.67654570654814</v>
+        <v>14.94616089403192</v>
       </c>
       <c r="D103" t="s">
         <v>304</v>
@@ -3057,7 +3057,7 @@
         <v>106</v>
       </c>
       <c r="C104">
-        <v>23.82822901222921</v>
+        <v>14.00859298360176</v>
       </c>
       <c r="D104" t="s">
         <v>304</v>
@@ -3074,7 +3074,7 @@
         <v>107</v>
       </c>
       <c r="C105">
-        <v>20.86891122968841</v>
+        <v>17.94585694741779</v>
       </c>
       <c r="D105" t="s">
         <v>304</v>
@@ -3091,7 +3091,7 @@
         <v>108</v>
       </c>
       <c r="C106">
-        <v>19.00073304138813</v>
+        <v>16.7496316103117</v>
       </c>
       <c r="D106" t="s">
         <v>304</v>
@@ -3108,7 +3108,7 @@
         <v>109</v>
       </c>
       <c r="C107">
-        <v>15.89298901892042</v>
+        <v>19.74072238815298</v>
       </c>
       <c r="D107" t="s">
         <v>304</v>
@@ -3125,7 +3125,7 @@
         <v>110</v>
       </c>
       <c r="C108">
-        <v>23.3179021622914</v>
+        <v>16.26789929970087</v>
       </c>
       <c r="D108" t="s">
         <v>304</v>
@@ -3142,7 +3142,7 @@
         <v>111</v>
       </c>
       <c r="C109">
-        <v>41.48411200679593</v>
+        <v>17.92456438631755</v>
       </c>
       <c r="D109" t="s">
         <v>304</v>
@@ -3159,7 +3159,7 @@
         <v>112</v>
       </c>
       <c r="C110">
-        <v>6.99642286039988</v>
+        <v>32.36753983891856</v>
       </c>
       <c r="D110" t="s">
         <v>304</v>
@@ -3176,7 +3176,7 @@
         <v>113</v>
       </c>
       <c r="C111">
-        <v>14.52056611603424</v>
+        <v>21.07028214173625</v>
       </c>
       <c r="D111" t="s">
         <v>304</v>
@@ -3193,7 +3193,7 @@
         <v>114</v>
       </c>
       <c r="C112">
-        <v>15.81584543024387</v>
+        <v>22.41860738863994</v>
       </c>
       <c r="D112" t="s">
         <v>304</v>
@@ -3210,7 +3210,7 @@
         <v>115</v>
       </c>
       <c r="C113">
-        <v>25.25006182424985</v>
+        <v>37.69327237464072</v>
       </c>
       <c r="D113" t="s">
         <v>304</v>
@@ -3227,7 +3227,7 @@
         <v>116</v>
       </c>
       <c r="C114">
-        <v>27.35794570195632</v>
+        <v>20.17254336778786</v>
       </c>
       <c r="D114" t="s">
         <v>304</v>
@@ -3244,7 +3244,7 @@
         <v>117</v>
       </c>
       <c r="C115">
-        <v>24.78914510742175</v>
+        <v>15.56651800093922</v>
       </c>
       <c r="D115" t="s">
         <v>304</v>
@@ -3261,7 +3261,7 @@
         <v>118</v>
       </c>
       <c r="C116">
-        <v>45.73457545084599</v>
+        <v>12.23138917147372</v>
       </c>
       <c r="D116" t="s">
         <v>304</v>
@@ -3278,7 +3278,7 @@
         <v>119</v>
       </c>
       <c r="C117">
-        <v>25.79415711972669</v>
+        <v>18.84303989000736</v>
       </c>
       <c r="D117" t="s">
         <v>304</v>
@@ -3295,7 +3295,7 @@
         <v>120</v>
       </c>
       <c r="C118">
-        <v>24.8339791758865</v>
+        <v>20.49830823232253</v>
       </c>
       <c r="D118" t="s">
         <v>304</v>
@@ -3312,7 +3312,7 @@
         <v>121</v>
       </c>
       <c r="C119">
-        <v>27.80068508649166</v>
+        <v>26.52183905931097</v>
       </c>
       <c r="D119" t="s">
         <v>304</v>
@@ -3329,7 +3329,7 @@
         <v>122</v>
       </c>
       <c r="C120">
-        <v>20.07004237487905</v>
+        <v>18.42793734381708</v>
       </c>
       <c r="D120" t="s">
         <v>304</v>
@@ -3346,7 +3346,7 @@
         <v>123</v>
       </c>
       <c r="C121">
-        <v>17.59465748689423</v>
+        <v>19.16990583175201</v>
       </c>
       <c r="D121" t="s">
         <v>304</v>
@@ -3363,7 +3363,7 @@
         <v>124</v>
       </c>
       <c r="C122">
-        <v>23.60840946307616</v>
+        <v>4.663555172109691</v>
       </c>
       <c r="D122" t="s">
         <v>304</v>
@@ -3380,7 +3380,7 @@
         <v>125</v>
       </c>
       <c r="C123">
-        <v>18.92670937023706</v>
+        <v>17.73826579165437</v>
       </c>
       <c r="D123" t="s">
         <v>304</v>
@@ -3397,7 +3397,7 @@
         <v>126</v>
       </c>
       <c r="C124">
-        <v>42.34288618313565</v>
+        <v>14.05583650194345</v>
       </c>
       <c r="D124" t="s">
         <v>304</v>
@@ -3414,7 +3414,7 @@
         <v>127</v>
       </c>
       <c r="C125">
-        <v>29.35563653493786</v>
+        <v>21.03753547190164</v>
       </c>
       <c r="D125" t="s">
         <v>304</v>
@@ -3431,7 +3431,7 @@
         <v>128</v>
       </c>
       <c r="C126">
-        <v>22.33788755626832</v>
+        <v>20.0777000098273</v>
       </c>
       <c r="D126" t="s">
         <v>304</v>
@@ -3448,7 +3448,7 @@
         <v>129</v>
       </c>
       <c r="C127">
-        <v>33.32831488425382</v>
+        <v>14.64383635921379</v>
       </c>
       <c r="D127" t="s">
         <v>304</v>
@@ -3465,7 +3465,7 @@
         <v>130</v>
       </c>
       <c r="C128">
-        <v>36.15677871293529</v>
+        <v>17.70898244069507</v>
       </c>
       <c r="D128" t="s">
         <v>304</v>
@@ -3482,7 +3482,7 @@
         <v>131</v>
       </c>
       <c r="C129">
-        <v>11.27171528817062</v>
+        <v>16.71589513418865</v>
       </c>
       <c r="D129" t="s">
         <v>304</v>
@@ -3499,7 +3499,7 @@
         <v>132</v>
       </c>
       <c r="C130">
-        <v>20.4364046852866</v>
+        <v>38.90503525477293</v>
       </c>
       <c r="D130" t="s">
         <v>304</v>
@@ -3516,7 +3516,7 @@
         <v>133</v>
       </c>
       <c r="C131">
-        <v>7.70248355875105</v>
+        <v>11.86915602803096</v>
       </c>
       <c r="D131" t="s">
         <v>304</v>
@@ -3533,7 +3533,7 @@
         <v>134</v>
       </c>
       <c r="C132">
-        <v>8.747754235894991</v>
+        <v>29.55914814038621</v>
       </c>
       <c r="D132" t="s">
         <v>304</v>
@@ -3550,7 +3550,7 @@
         <v>135</v>
       </c>
       <c r="C133">
-        <v>35.55187005862443</v>
+        <v>17.78346358718495</v>
       </c>
       <c r="D133" t="s">
         <v>304</v>
@@ -3567,7 +3567,7 @@
         <v>136</v>
       </c>
       <c r="C134">
-        <v>44.10204044658585</v>
+        <v>29.24811617973975</v>
       </c>
       <c r="D134" t="s">
         <v>304</v>
@@ -3584,7 +3584,7 @@
         <v>137</v>
       </c>
       <c r="C135">
-        <v>28.69738015408864</v>
+        <v>11.06594453419051</v>
       </c>
       <c r="D135" t="s">
         <v>304</v>
@@ -3601,7 +3601,7 @@
         <v>138</v>
       </c>
       <c r="C136">
-        <v>31.41740202724541</v>
+        <v>30.81793414393798</v>
       </c>
       <c r="D136" t="s">
         <v>304</v>
@@ -3618,7 +3618,7 @@
         <v>139</v>
       </c>
       <c r="C137">
-        <v>14.67411085162247</v>
+        <v>23.60203314982794</v>
       </c>
       <c r="D137" t="s">
         <v>304</v>
@@ -3635,7 +3635,7 @@
         <v>140</v>
       </c>
       <c r="C138">
-        <v>9.205155346615568</v>
+        <v>60.50288785818249</v>
       </c>
       <c r="D138" t="s">
         <v>304</v>
@@ -3652,7 +3652,7 @@
         <v>141</v>
       </c>
       <c r="C139">
-        <v>23.48560461037517</v>
+        <v>34.96608343821278</v>
       </c>
       <c r="D139" t="s">
         <v>304</v>
@@ -3669,7 +3669,7 @@
         <v>142</v>
       </c>
       <c r="C140">
-        <v>32.38257263542334</v>
+        <v>55.53112742775838</v>
       </c>
       <c r="D140" t="s">
         <v>304</v>
@@ -3686,7 +3686,7 @@
         <v>143</v>
       </c>
       <c r="C141">
-        <v>10.63658980793478</v>
+        <v>26.1365499567512</v>
       </c>
       <c r="D141" t="s">
         <v>304</v>
@@ -3703,7 +3703,7 @@
         <v>144</v>
       </c>
       <c r="C142">
-        <v>28.70771338822617</v>
+        <v>18.09362020136095</v>
       </c>
       <c r="D142" t="s">
         <v>304</v>
@@ -3720,7 +3720,7 @@
         <v>145</v>
       </c>
       <c r="C143">
-        <v>20.85217543431645</v>
+        <v>13.81730059486681</v>
       </c>
       <c r="D143" t="s">
         <v>304</v>
@@ -3737,7 +3737,7 @@
         <v>146</v>
       </c>
       <c r="C144">
-        <v>25.28022030157284</v>
+        <v>25.0980882141244</v>
       </c>
       <c r="D144" t="s">
         <v>304</v>
@@ -3754,7 +3754,7 @@
         <v>147</v>
       </c>
       <c r="C145">
-        <v>8.438613035009134</v>
+        <v>27.34948119966934</v>
       </c>
       <c r="D145" t="s">
         <v>304</v>
@@ -3771,7 +3771,7 @@
         <v>148</v>
       </c>
       <c r="C146">
-        <v>10.93713299650084</v>
+        <v>16.06673804274836</v>
       </c>
       <c r="D146" t="s">
         <v>304</v>
@@ -3788,7 +3788,7 @@
         <v>149</v>
       </c>
       <c r="C147">
-        <v>8.447418539254301</v>
+        <v>6.39936335168135</v>
       </c>
       <c r="D147" t="s">
         <v>304</v>
@@ -3805,7 +3805,7 @@
         <v>150</v>
       </c>
       <c r="C148">
-        <v>23.39977455948967</v>
+        <v>18.02166271710824</v>
       </c>
       <c r="D148" t="s">
         <v>304</v>
@@ -3822,7 +3822,7 @@
         <v>151</v>
       </c>
       <c r="C149">
-        <v>15.22802478708599</v>
+        <v>17.40478206999373</v>
       </c>
       <c r="D149" t="s">
         <v>304</v>
@@ -3839,7 +3839,7 @@
         <v>152</v>
       </c>
       <c r="C150">
-        <v>15.4932751703656</v>
+        <v>17.00333664700383</v>
       </c>
       <c r="D150" t="s">
         <v>304</v>
@@ -3856,7 +3856,7 @@
         <v>153</v>
       </c>
       <c r="C151">
-        <v>37.39287900030744</v>
+        <v>23.62447938533273</v>
       </c>
       <c r="D151" t="s">
         <v>304</v>
@@ -3873,7 +3873,7 @@
         <v>154</v>
       </c>
       <c r="C152">
-        <v>7.528279869383995</v>
+        <v>20.70541181199798</v>
       </c>
       <c r="D152" t="s">
         <v>304</v>
@@ -3890,7 +3890,7 @@
         <v>155</v>
       </c>
       <c r="C153">
-        <v>4.092004047624144</v>
+        <v>26.9522725272393</v>
       </c>
       <c r="D153" t="s">
         <v>304</v>
@@ -3907,7 +3907,7 @@
         <v>156</v>
       </c>
       <c r="C154">
-        <v>29.17644733618263</v>
+        <v>10.99486338457997</v>
       </c>
       <c r="D154" t="s">
         <v>304</v>
@@ -3924,7 +3924,7 @@
         <v>157</v>
       </c>
       <c r="C155">
-        <v>44.84200979253303</v>
+        <v>22.72023320176077</v>
       </c>
       <c r="D155" t="s">
         <v>304</v>
@@ -3941,7 +3941,7 @@
         <v>158</v>
       </c>
       <c r="C156">
-        <v>21.60465343122022</v>
+        <v>24.16567257270309</v>
       </c>
       <c r="D156" t="s">
         <v>304</v>
@@ -3958,7 +3958,7 @@
         <v>159</v>
       </c>
       <c r="C157">
-        <v>27.9603050377529</v>
+        <v>1.775167669850669</v>
       </c>
       <c r="D157" t="s">
         <v>304</v>
@@ -3975,7 +3975,7 @@
         <v>160</v>
       </c>
       <c r="C158">
-        <v>16.66074163939609</v>
+        <v>14.64775480612471</v>
       </c>
       <c r="D158" t="s">
         <v>304</v>
@@ -3992,7 +3992,7 @@
         <v>161</v>
       </c>
       <c r="C159">
-        <v>14.61750983511925</v>
+        <v>25.92332841626756</v>
       </c>
       <c r="D159" t="s">
         <v>304</v>
@@ -4009,7 +4009,7 @@
         <v>162</v>
       </c>
       <c r="C160">
-        <v>8.42149414153331</v>
+        <v>24.09200944229104</v>
       </c>
       <c r="D160" t="s">
         <v>304</v>
@@ -4026,7 +4026,7 @@
         <v>163</v>
       </c>
       <c r="C161">
-        <v>6.207601463823918</v>
+        <v>18.25825529280372</v>
       </c>
       <c r="D161" t="s">
         <v>304</v>
@@ -4043,7 +4043,7 @@
         <v>164</v>
       </c>
       <c r="C162">
-        <v>13.48525826056262</v>
+        <v>24.8129030856811</v>
       </c>
       <c r="D162" t="s">
         <v>304</v>
@@ -4060,7 +4060,7 @@
         <v>165</v>
       </c>
       <c r="C163">
-        <v>22.86218281040264</v>
+        <v>10.41361450413135</v>
       </c>
       <c r="D163" t="s">
         <v>304</v>
@@ -4077,7 +4077,7 @@
         <v>166</v>
       </c>
       <c r="C164">
-        <v>32.59726228214207</v>
+        <v>29.95795863855866</v>
       </c>
       <c r="D164" t="s">
         <v>304</v>
@@ -4094,7 +4094,7 @@
         <v>167</v>
       </c>
       <c r="C165">
-        <v>11.04790763442308</v>
+        <v>16.73848596145456</v>
       </c>
       <c r="D165" t="s">
         <v>304</v>
@@ -4111,7 +4111,7 @@
         <v>168</v>
       </c>
       <c r="C166">
-        <v>9.006780819278081</v>
+        <v>10.6058628272609</v>
       </c>
       <c r="D166" t="s">
         <v>304</v>
@@ -4128,7 +4128,7 @@
         <v>169</v>
       </c>
       <c r="C167">
-        <v>9.574985740083164</v>
+        <v>27.7142412007634</v>
       </c>
       <c r="D167" t="s">
         <v>304</v>
@@ -4145,7 +4145,7 @@
         <v>170</v>
       </c>
       <c r="C168">
-        <v>13.48415945651964</v>
+        <v>8.186140260567996</v>
       </c>
       <c r="D168" t="s">
         <v>304</v>
@@ -4162,7 +4162,7 @@
         <v>171</v>
       </c>
       <c r="C169">
-        <v>25.7148302269656</v>
+        <v>22.2709788732374</v>
       </c>
       <c r="D169" t="s">
         <v>304</v>
@@ -4179,7 +4179,7 @@
         <v>172</v>
       </c>
       <c r="C170">
-        <v>8.843028963294127</v>
+        <v>16.53576336833358</v>
       </c>
       <c r="D170" t="s">
         <v>304</v>
@@ -4196,7 +4196,7 @@
         <v>173</v>
       </c>
       <c r="C171">
-        <v>18.92113173265926</v>
+        <v>32.80253030497468</v>
       </c>
       <c r="D171" t="s">
         <v>304</v>
@@ -4213,7 +4213,7 @@
         <v>174</v>
       </c>
       <c r="C172">
-        <v>22.7530478195799</v>
+        <v>35.15164915606238</v>
       </c>
       <c r="D172" t="s">
         <v>304</v>
@@ -4230,7 +4230,7 @@
         <v>175</v>
       </c>
       <c r="C173">
-        <v>19.41567118518433</v>
+        <v>33.04269731109975</v>
       </c>
       <c r="D173" t="s">
         <v>304</v>
@@ -4247,7 +4247,7 @@
         <v>176</v>
       </c>
       <c r="C174">
-        <v>35.52644359947976</v>
+        <v>31.65868503171264</v>
       </c>
       <c r="D174" t="s">
         <v>304</v>
@@ -4264,7 +4264,7 @@
         <v>177</v>
       </c>
       <c r="C175">
-        <v>24.21986252981093</v>
+        <v>9.723947087360518</v>
       </c>
       <c r="D175" t="s">
         <v>304</v>
@@ -4281,7 +4281,7 @@
         <v>178</v>
       </c>
       <c r="C176">
-        <v>24.70699515450568</v>
+        <v>14.14747313607843</v>
       </c>
       <c r="D176" t="s">
         <v>304</v>
@@ -4298,7 +4298,7 @@
         <v>179</v>
       </c>
       <c r="C177">
-        <v>16.123292989719</v>
+        <v>11.68394274289163</v>
       </c>
       <c r="D177" t="s">
         <v>304</v>
@@ -4315,7 +4315,7 @@
         <v>180</v>
       </c>
       <c r="C178">
-        <v>18.26081647343402</v>
+        <v>28.16732535002705</v>
       </c>
       <c r="D178" t="s">
         <v>304</v>
@@ -4332,7 +4332,7 @@
         <v>181</v>
       </c>
       <c r="C179">
-        <v>8.592414240090983</v>
+        <v>8.810112706712218</v>
       </c>
       <c r="D179" t="s">
         <v>304</v>
@@ -4349,7 +4349,7 @@
         <v>182</v>
       </c>
       <c r="C180">
-        <v>16.05784043671934</v>
+        <v>5.633350564866687</v>
       </c>
       <c r="D180" t="s">
         <v>304</v>
@@ -4366,7 +4366,7 @@
         <v>183</v>
       </c>
       <c r="C181">
-        <v>39.20815857680611</v>
+        <v>15.81903819473322</v>
       </c>
       <c r="D181" t="s">
         <v>304</v>
@@ -4383,7 +4383,7 @@
         <v>184</v>
       </c>
       <c r="C182">
-        <v>16.67707989439672</v>
+        <v>11.08361477829521</v>
       </c>
       <c r="D182" t="s">
         <v>304</v>
@@ -4400,7 +4400,7 @@
         <v>185</v>
       </c>
       <c r="C183">
-        <v>34.80246184246583</v>
+        <v>9.992010803001172</v>
       </c>
       <c r="D183" t="s">
         <v>304</v>
@@ -4417,7 +4417,7 @@
         <v>186</v>
       </c>
       <c r="C184">
-        <v>19.7713887485088</v>
+        <v>38.37381940238274</v>
       </c>
       <c r="D184" t="s">
         <v>304</v>
@@ -4434,7 +4434,7 @@
         <v>187</v>
       </c>
       <c r="C185">
-        <v>9.19672231981804</v>
+        <v>12.39891209244437</v>
       </c>
       <c r="D185" t="s">
         <v>304</v>
@@ -4451,7 +4451,7 @@
         <v>188</v>
       </c>
       <c r="C186">
-        <v>7.725712953477673</v>
+        <v>37.21967685981924</v>
       </c>
       <c r="D186" t="s">
         <v>304</v>
@@ -4468,7 +4468,7 @@
         <v>189</v>
       </c>
       <c r="C187">
-        <v>10.89879903326749</v>
+        <v>13.78766184630229</v>
       </c>
       <c r="D187" t="s">
         <v>304</v>
@@ -4485,7 +4485,7 @@
         <v>190</v>
       </c>
       <c r="C188">
-        <v>12.00772339920441</v>
+        <v>22.04287985132095</v>
       </c>
       <c r="D188" t="s">
         <v>304</v>
@@ -4502,7 +4502,7 @@
         <v>191</v>
       </c>
       <c r="C189">
-        <v>13.70181989544516</v>
+        <v>20.3783491945002</v>
       </c>
       <c r="D189" t="s">
         <v>304</v>
@@ -4519,7 +4519,7 @@
         <v>192</v>
       </c>
       <c r="C190">
-        <v>16.9531192968081</v>
+        <v>21.0239283046652</v>
       </c>
       <c r="D190" t="s">
         <v>304</v>
@@ -4536,7 +4536,7 @@
         <v>193</v>
       </c>
       <c r="C191">
-        <v>20.89122566743846</v>
+        <v>20.2511605970695</v>
       </c>
       <c r="D191" t="s">
         <v>304</v>
@@ -4553,7 +4553,7 @@
         <v>194</v>
       </c>
       <c r="C192">
-        <v>7.980540708727673</v>
+        <v>26.56305713961689</v>
       </c>
       <c r="D192" t="s">
         <v>304</v>
@@ -4570,7 +4570,7 @@
         <v>195</v>
       </c>
       <c r="C193">
-        <v>34.77966491552526</v>
+        <v>15.97975889296862</v>
       </c>
       <c r="D193" t="s">
         <v>304</v>
@@ -4587,7 +4587,7 @@
         <v>196</v>
       </c>
       <c r="C194">
-        <v>16.82110710283577</v>
+        <v>21.23557215755814</v>
       </c>
       <c r="D194" t="s">
         <v>304</v>
@@ -4604,7 +4604,7 @@
         <v>197</v>
       </c>
       <c r="C195">
-        <v>14.24900098159739</v>
+        <v>35.25039911057009</v>
       </c>
       <c r="D195" t="s">
         <v>304</v>
@@ -4621,7 +4621,7 @@
         <v>198</v>
       </c>
       <c r="C196">
-        <v>16.15034813585293</v>
+        <v>33.10368448304069</v>
       </c>
       <c r="D196" t="s">
         <v>304</v>
@@ -4638,7 +4638,7 @@
         <v>199</v>
       </c>
       <c r="C197">
-        <v>16.37124780092634</v>
+        <v>22.61551964967792</v>
       </c>
       <c r="D197" t="s">
         <v>304</v>
@@ -4655,7 +4655,7 @@
         <v>200</v>
       </c>
       <c r="C198">
-        <v>1.886329141436159</v>
+        <v>21.21515915270055</v>
       </c>
       <c r="D198" t="s">
         <v>304</v>
@@ -4672,7 +4672,7 @@
         <v>201</v>
       </c>
       <c r="C199">
-        <v>23.14944336749897</v>
+        <v>19.37945418768609</v>
       </c>
       <c r="D199" t="s">
         <v>304</v>
@@ -4689,7 +4689,7 @@
         <v>202</v>
       </c>
       <c r="C200">
-        <v>32.83221709067684</v>
+        <v>13.71374369280855</v>
       </c>
       <c r="D200" t="s">
         <v>304</v>
@@ -4706,7 +4706,7 @@
         <v>203</v>
       </c>
       <c r="C201">
-        <v>36.777435632056</v>
+        <v>10.91740556161999</v>
       </c>
       <c r="D201" t="s">
         <v>304</v>
@@ -4723,7 +4723,7 @@
         <v>204</v>
       </c>
       <c r="C202">
-        <v>10.61088382458664</v>
+        <v>5.652954613421997</v>
       </c>
       <c r="D202" t="s">
         <v>304</v>
@@ -4740,7 +4740,7 @@
         <v>205</v>
       </c>
       <c r="C203">
-        <v>12.90445690883481</v>
+        <v>35.11748257757435</v>
       </c>
       <c r="D203" t="s">
         <v>304</v>
@@ -4757,7 +4757,7 @@
         <v>206</v>
       </c>
       <c r="C204">
-        <v>19.93220564121952</v>
+        <v>16.64736645158112</v>
       </c>
       <c r="D204" t="s">
         <v>304</v>
@@ -4774,7 +4774,7 @@
         <v>207</v>
       </c>
       <c r="C205">
-        <v>18.42015535944907</v>
+        <v>14.86973060562642</v>
       </c>
       <c r="D205" t="s">
         <v>304</v>
@@ -4791,7 +4791,7 @@
         <v>208</v>
       </c>
       <c r="C206">
-        <v>35.45095567666166</v>
+        <v>13.56811854266579</v>
       </c>
       <c r="D206" t="s">
         <v>304</v>
@@ -4808,7 +4808,7 @@
         <v>209</v>
       </c>
       <c r="C207">
-        <v>16.20174503292933</v>
+        <v>36.29766155834651</v>
       </c>
       <c r="D207" t="s">
         <v>304</v>
@@ -4825,7 +4825,7 @@
         <v>210</v>
       </c>
       <c r="C208">
-        <v>26.03301178278312</v>
+        <v>22.40569124841384</v>
       </c>
       <c r="D208" t="s">
         <v>304</v>
@@ -4842,7 +4842,7 @@
         <v>211</v>
       </c>
       <c r="C209">
-        <v>10.51122933035107</v>
+        <v>7.784732097963715</v>
       </c>
       <c r="D209" t="s">
         <v>304</v>
@@ -4859,7 +4859,7 @@
         <v>212</v>
       </c>
       <c r="C210">
-        <v>39.50364309708677</v>
+        <v>19.30621930242956</v>
       </c>
       <c r="D210" t="s">
         <v>304</v>
@@ -4876,7 +4876,7 @@
         <v>213</v>
       </c>
       <c r="C211">
-        <v>33.23830495222376</v>
+        <v>29.42148730529291</v>
       </c>
       <c r="D211" t="s">
         <v>304</v>
@@ -4893,7 +4893,7 @@
         <v>214</v>
       </c>
       <c r="C212">
-        <v>24.86090950196292</v>
+        <v>4.336956657626862</v>
       </c>
       <c r="D212" t="s">
         <v>304</v>
@@ -4910,7 +4910,7 @@
         <v>215</v>
       </c>
       <c r="C213">
-        <v>28.27777442296039</v>
+        <v>23.88509588997985</v>
       </c>
       <c r="D213" t="s">
         <v>304</v>
@@ -4927,7 +4927,7 @@
         <v>216</v>
       </c>
       <c r="C214">
-        <v>11.45666054442607</v>
+        <v>31.24201745066899</v>
       </c>
       <c r="D214" t="s">
         <v>304</v>
@@ -4944,7 +4944,7 @@
         <v>217</v>
       </c>
       <c r="C215">
-        <v>14.83810658938209</v>
+        <v>20.68789025884614</v>
       </c>
       <c r="D215" t="s">
         <v>304</v>
@@ -4961,7 +4961,7 @@
         <v>218</v>
       </c>
       <c r="C216">
-        <v>19.59760335350455</v>
+        <v>20.45721830936395</v>
       </c>
       <c r="D216" t="s">
         <v>304</v>
@@ -4978,7 +4978,7 @@
         <v>219</v>
       </c>
       <c r="C217">
-        <v>16.66764206255984</v>
+        <v>23.25111453570605</v>
       </c>
       <c r="D217" t="s">
         <v>304</v>
@@ -4995,7 +4995,7 @@
         <v>220</v>
       </c>
       <c r="C218">
-        <v>12.25117218798787</v>
+        <v>17.36073112331891</v>
       </c>
       <c r="D218" t="s">
         <v>304</v>
@@ -5012,7 +5012,7 @@
         <v>221</v>
       </c>
       <c r="C219">
-        <v>50.91753108815861</v>
+        <v>16.55363793056632</v>
       </c>
       <c r="D219" t="s">
         <v>304</v>
@@ -5029,7 +5029,7 @@
         <v>222</v>
       </c>
       <c r="C220">
-        <v>29.67390965717471</v>
+        <v>21.74241993325638</v>
       </c>
       <c r="D220" t="s">
         <v>304</v>
@@ -5046,7 +5046,7 @@
         <v>223</v>
       </c>
       <c r="C221">
-        <v>15.61617092307429</v>
+        <v>17.65838957055163</v>
       </c>
       <c r="D221" t="s">
         <v>304</v>
@@ -5063,7 +5063,7 @@
         <v>224</v>
       </c>
       <c r="C222">
-        <v>23.83971291849285</v>
+        <v>19.04394056092832</v>
       </c>
       <c r="D222" t="s">
         <v>304</v>
@@ -5080,7 +5080,7 @@
         <v>225</v>
       </c>
       <c r="C223">
-        <v>30.79887760383424</v>
+        <v>4.405955734221374</v>
       </c>
       <c r="D223" t="s">
         <v>304</v>
@@ -5097,7 +5097,7 @@
         <v>226</v>
       </c>
       <c r="C224">
-        <v>18.30996361313898</v>
+        <v>27.87007191476977</v>
       </c>
       <c r="D224" t="s">
         <v>304</v>
@@ -5114,7 +5114,7 @@
         <v>227</v>
       </c>
       <c r="C225">
-        <v>25.32943539395758</v>
+        <v>15.40116098102613</v>
       </c>
       <c r="D225" t="s">
         <v>304</v>
@@ -5131,7 +5131,7 @@
         <v>228</v>
       </c>
       <c r="C226">
-        <v>16.1607588644939</v>
+        <v>15.58357485344087</v>
       </c>
       <c r="D226" t="s">
         <v>304</v>
@@ -5148,7 +5148,7 @@
         <v>229</v>
       </c>
       <c r="C227">
-        <v>25.27992166607756</v>
+        <v>27.33112306172675</v>
       </c>
       <c r="D227" t="s">
         <v>304</v>
@@ -5165,7 +5165,7 @@
         <v>230</v>
       </c>
       <c r="C228">
-        <v>28.90335355275123</v>
+        <v>14.67106404055786</v>
       </c>
       <c r="D228" t="s">
         <v>304</v>
@@ -5182,7 +5182,7 @@
         <v>231</v>
       </c>
       <c r="C229">
-        <v>37.73804602782551</v>
+        <v>10.8075801486712</v>
       </c>
       <c r="D229" t="s">
         <v>304</v>
@@ -5199,7 +5199,7 @@
         <v>232</v>
       </c>
       <c r="C230">
-        <v>9.725709970526639</v>
+        <v>19.27442303254859</v>
       </c>
       <c r="D230" t="s">
         <v>304</v>
@@ -5216,7 +5216,7 @@
         <v>233</v>
       </c>
       <c r="C231">
-        <v>7.07670455108433</v>
+        <v>12.57311707417051</v>
       </c>
       <c r="D231" t="s">
         <v>304</v>
@@ -5233,7 +5233,7 @@
         <v>234</v>
       </c>
       <c r="C232">
-        <v>30.57098755074322</v>
+        <v>24.30792666303686</v>
       </c>
       <c r="D232" t="s">
         <v>304</v>
@@ -5250,7 +5250,7 @@
         <v>235</v>
       </c>
       <c r="C233">
-        <v>5.888158173825069</v>
+        <v>31.17148386331451</v>
       </c>
       <c r="D233" t="s">
         <v>304</v>
@@ -5267,7 +5267,7 @@
         <v>236</v>
       </c>
       <c r="C234">
-        <v>13.99216704545223</v>
+        <v>32.03985031971209</v>
       </c>
       <c r="D234" t="s">
         <v>304</v>
@@ -5284,7 +5284,7 @@
         <v>237</v>
       </c>
       <c r="C235">
-        <v>13.29980475472433</v>
+        <v>17.87903435714063</v>
       </c>
       <c r="D235" t="s">
         <v>304</v>
@@ -5301,7 +5301,7 @@
         <v>238</v>
       </c>
       <c r="C236">
-        <v>19.52931097771944</v>
+        <v>24.02413369354377</v>
       </c>
       <c r="D236" t="s">
         <v>304</v>
@@ -5318,7 +5318,7 @@
         <v>239</v>
       </c>
       <c r="C237">
-        <v>14.64738432514337</v>
+        <v>20.22793497709965</v>
       </c>
       <c r="D237" t="s">
         <v>304</v>
@@ -5335,7 +5335,7 @@
         <v>240</v>
       </c>
       <c r="C238">
-        <v>34.52599842700541</v>
+        <v>21.78309156128422</v>
       </c>
       <c r="D238" t="s">
         <v>304</v>
@@ -5352,7 +5352,7 @@
         <v>241</v>
       </c>
       <c r="C239">
-        <v>15.29340201257467</v>
+        <v>43.30602838615576</v>
       </c>
       <c r="D239" t="s">
         <v>304</v>
@@ -5369,7 +5369,7 @@
         <v>242</v>
       </c>
       <c r="C240">
-        <v>26.86420673090552</v>
+        <v>16.4128598258582</v>
       </c>
       <c r="D240" t="s">
         <v>304</v>
@@ -5386,7 +5386,7 @@
         <v>243</v>
       </c>
       <c r="C241">
-        <v>43.41360515533797</v>
+        <v>19.80998787029955</v>
       </c>
       <c r="D241" t="s">
         <v>304</v>
@@ -5403,7 +5403,7 @@
         <v>244</v>
       </c>
       <c r="C242">
-        <v>19.50286467799332</v>
+        <v>19.97703972686834</v>
       </c>
       <c r="D242" t="s">
         <v>304</v>
@@ -5420,7 +5420,7 @@
         <v>245</v>
       </c>
       <c r="C243">
-        <v>8.241017222968937</v>
+        <v>34.90029996822075</v>
       </c>
       <c r="D243" t="s">
         <v>304</v>
@@ -5437,7 +5437,7 @@
         <v>246</v>
       </c>
       <c r="C244">
-        <v>12.37092185442942</v>
+        <v>33.35499294173356</v>
       </c>
       <c r="D244" t="s">
         <v>304</v>
@@ -5454,7 +5454,7 @@
         <v>247</v>
       </c>
       <c r="C245">
-        <v>15.97437749325184</v>
+        <v>7.720011947548917</v>
       </c>
       <c r="D245" t="s">
         <v>304</v>
@@ -5471,7 +5471,7 @@
         <v>248</v>
       </c>
       <c r="C246">
-        <v>21.12207969027967</v>
+        <v>33.14061211226086</v>
       </c>
       <c r="D246" t="s">
         <v>304</v>
@@ -5488,7 +5488,7 @@
         <v>249</v>
       </c>
       <c r="C247">
-        <v>20.82694875752226</v>
+        <v>39.11779651302174</v>
       </c>
       <c r="D247" t="s">
         <v>304</v>
@@ -5505,7 +5505,7 @@
         <v>250</v>
       </c>
       <c r="C248">
-        <v>37.73257250733452</v>
+        <v>7.48786457325968</v>
       </c>
       <c r="D248" t="s">
         <v>304</v>
@@ -5522,7 +5522,7 @@
         <v>251</v>
       </c>
       <c r="C249">
-        <v>13.35992689725525</v>
+        <v>9.698614695840327</v>
       </c>
       <c r="D249" t="s">
         <v>304</v>
@@ -5539,7 +5539,7 @@
         <v>252</v>
       </c>
       <c r="C250">
-        <v>23.97643838374998</v>
+        <v>23.85465956005803</v>
       </c>
       <c r="D250" t="s">
         <v>304</v>
@@ -5556,7 +5556,7 @@
         <v>253</v>
       </c>
       <c r="C251">
-        <v>6.116117099007724</v>
+        <v>13.71295077752543</v>
       </c>
       <c r="D251" t="s">
         <v>304</v>
@@ -5573,7 +5573,7 @@
         <v>254</v>
       </c>
       <c r="C252">
-        <v>32.9836569076617</v>
+        <v>17.26135936023993</v>
       </c>
       <c r="D252" t="s">
         <v>304</v>
@@ -5590,7 +5590,7 @@
         <v>255</v>
       </c>
       <c r="C253">
-        <v>25.52112242723786</v>
+        <v>22.44070652706283</v>
       </c>
       <c r="D253" t="s">
         <v>304</v>
@@ -5607,7 +5607,7 @@
         <v>256</v>
       </c>
       <c r="C254">
-        <v>9.565414660565365</v>
+        <v>26.99039792771658</v>
       </c>
       <c r="D254" t="s">
         <v>304</v>
@@ -5624,7 +5624,7 @@
         <v>257</v>
       </c>
       <c r="C255">
-        <v>14.63655194977224</v>
+        <v>36.54722137605775</v>
       </c>
       <c r="D255" t="s">
         <v>304</v>
@@ -5641,7 +5641,7 @@
         <v>258</v>
       </c>
       <c r="C256">
-        <v>53.74020890391687</v>
+        <v>6.079347770157932</v>
       </c>
       <c r="D256" t="s">
         <v>304</v>
@@ -5658,7 +5658,7 @@
         <v>259</v>
       </c>
       <c r="C257">
-        <v>19.20085738366911</v>
+        <v>23.5011498799506</v>
       </c>
       <c r="D257" t="s">
         <v>304</v>
@@ -5675,7 +5675,7 @@
         <v>260</v>
       </c>
       <c r="C258">
-        <v>16.15178120598388</v>
+        <v>22.43841975291482</v>
       </c>
       <c r="D258" t="s">
         <v>304</v>
@@ -5692,7 +5692,7 @@
         <v>261</v>
       </c>
       <c r="C259">
-        <v>47.3980412742282</v>
+        <v>9.478438246875731</v>
       </c>
       <c r="D259" t="s">
         <v>304</v>
@@ -5709,7 +5709,7 @@
         <v>262</v>
       </c>
       <c r="C260">
-        <v>17.11897828542594</v>
+        <v>23.77318603244927</v>
       </c>
       <c r="D260" t="s">
         <v>304</v>
@@ -5726,7 +5726,7 @@
         <v>263</v>
       </c>
       <c r="C261">
-        <v>18.08984745068927</v>
+        <v>21.16719434688074</v>
       </c>
       <c r="D261" t="s">
         <v>304</v>
@@ -5743,7 +5743,7 @@
         <v>264</v>
       </c>
       <c r="C262">
-        <v>31.26454700985945</v>
+        <v>11.46557837342986</v>
       </c>
       <c r="D262" t="s">
         <v>304</v>
@@ -5760,7 +5760,7 @@
         <v>265</v>
       </c>
       <c r="C263">
-        <v>31.07036168228689</v>
+        <v>16.9539703956834</v>
       </c>
       <c r="D263" t="s">
         <v>304</v>
@@ -5777,7 +5777,7 @@
         <v>266</v>
       </c>
       <c r="C264">
-        <v>12.07234462876633</v>
+        <v>9.888574115116459</v>
       </c>
       <c r="D264" t="s">
         <v>304</v>
@@ -5794,7 +5794,7 @@
         <v>267</v>
       </c>
       <c r="C265">
-        <v>2.374958159636821</v>
+        <v>14.42335905485323</v>
       </c>
       <c r="D265" t="s">
         <v>304</v>
@@ -5811,7 +5811,7 @@
         <v>268</v>
       </c>
       <c r="C266">
-        <v>18.88993687178898</v>
+        <v>22.08204883216095</v>
       </c>
       <c r="D266" t="s">
         <v>304</v>
@@ -5828,7 +5828,7 @@
         <v>269</v>
       </c>
       <c r="C267">
-        <v>8.107679804429791</v>
+        <v>15.23835406909421</v>
       </c>
       <c r="D267" t="s">
         <v>304</v>
@@ -5845,7 +5845,7 @@
         <v>270</v>
       </c>
       <c r="C268">
-        <v>20.5861785062093</v>
+        <v>9.540657823141906</v>
       </c>
       <c r="D268" t="s">
         <v>304</v>
@@ -5862,7 +5862,7 @@
         <v>271</v>
       </c>
       <c r="C269">
-        <v>10.94655444221075</v>
+        <v>17.84811308622037</v>
       </c>
       <c r="D269" t="s">
         <v>304</v>
@@ -5879,7 +5879,7 @@
         <v>272</v>
       </c>
       <c r="C270">
-        <v>8.485270969209292</v>
+        <v>14.87843784447342</v>
       </c>
       <c r="D270" t="s">
         <v>304</v>
@@ -5896,7 +5896,7 @@
         <v>273</v>
       </c>
       <c r="C271">
-        <v>13.52832987823081</v>
+        <v>19.86851212686078</v>
       </c>
       <c r="D271" t="s">
         <v>304</v>
@@ -5913,7 +5913,7 @@
         <v>274</v>
       </c>
       <c r="C272">
-        <v>8.352078350238699</v>
+        <v>18.90736951060813</v>
       </c>
       <c r="D272" t="s">
         <v>304</v>
@@ -5930,7 +5930,7 @@
         <v>275</v>
       </c>
       <c r="C273">
-        <v>18.16341630407823</v>
+        <v>15.27577803725111</v>
       </c>
       <c r="D273" t="s">
         <v>305</v>
@@ -5947,7 +5947,7 @@
         <v>276</v>
       </c>
       <c r="C274">
-        <v>23.2889742722624</v>
+        <v>24.54248793065025</v>
       </c>
       <c r="D274" t="s">
         <v>305</v>
@@ -5964,7 +5964,7 @@
         <v>277</v>
       </c>
       <c r="C275">
-        <v>8.404391553778723</v>
+        <v>14.95700484670022</v>
       </c>
       <c r="D275" t="s">
         <v>305</v>
@@ -5981,7 +5981,7 @@
         <v>278</v>
       </c>
       <c r="C276">
-        <v>26.15568188324406</v>
+        <v>13.77306879227697</v>
       </c>
       <c r="D276" t="s">
         <v>305</v>
@@ -5998,7 +5998,7 @@
         <v>279</v>
       </c>
       <c r="C277">
-        <v>33.85015633913745</v>
+        <v>13.59666727042588</v>
       </c>
       <c r="D277" t="s">
         <v>305</v>
@@ -6015,7 +6015,7 @@
         <v>280</v>
       </c>
       <c r="C278">
-        <v>6.479619559377943</v>
+        <v>23.94103326722317</v>
       </c>
       <c r="D278" t="s">
         <v>305</v>
@@ -6032,7 +6032,7 @@
         <v>281</v>
       </c>
       <c r="C279">
-        <v>29.19411595500844</v>
+        <v>10.41380463595615</v>
       </c>
       <c r="D279" t="s">
         <v>305</v>
@@ -6049,7 +6049,7 @@
         <v>282</v>
       </c>
       <c r="C280">
-        <v>22.64724648323896</v>
+        <v>18.52196569172499</v>
       </c>
       <c r="D280" t="s">
         <v>305</v>
@@ -6066,7 +6066,7 @@
         <v>283</v>
       </c>
       <c r="C281">
-        <v>16.20067923570972</v>
+        <v>27.53281310421751</v>
       </c>
       <c r="D281" t="s">
         <v>305</v>
@@ -6083,7 +6083,7 @@
         <v>284</v>
       </c>
       <c r="C282">
-        <v>38.3820337876036</v>
+        <v>22.38447340635172</v>
       </c>
       <c r="D282" t="s">
         <v>305</v>
@@ -6100,7 +6100,7 @@
         <v>285</v>
       </c>
       <c r="C283">
-        <v>52.87725486972754</v>
+        <v>7.709311032309616</v>
       </c>
       <c r="D283" t="s">
         <v>305</v>
@@ -6117,7 +6117,7 @@
         <v>286</v>
       </c>
       <c r="C284">
-        <v>17.82944257357285</v>
+        <v>22.35337650756361</v>
       </c>
       <c r="D284" t="s">
         <v>305</v>
@@ -6134,7 +6134,7 @@
         <v>287</v>
       </c>
       <c r="C285">
-        <v>11.37644090186875</v>
+        <v>12.89742494529197</v>
       </c>
       <c r="D285" t="s">
         <v>305</v>
@@ -6151,7 +6151,7 @@
         <v>288</v>
       </c>
       <c r="C286">
-        <v>9.82839257569103</v>
+        <v>7.368459020190331</v>
       </c>
       <c r="D286" t="s">
         <v>305</v>
@@ -6168,7 +6168,7 @@
         <v>289</v>
       </c>
       <c r="C287">
-        <v>19.24759991582781</v>
+        <v>8.63635084801855</v>
       </c>
       <c r="D287" t="s">
         <v>305</v>
@@ -6185,7 +6185,7 @@
         <v>290</v>
       </c>
       <c r="C288">
-        <v>25.4164617280421</v>
+        <v>19.25520033340243</v>
       </c>
       <c r="D288" t="s">
         <v>305</v>
@@ -6202,7 +6202,7 @@
         <v>291</v>
       </c>
       <c r="C289">
-        <v>28.23010329802429</v>
+        <v>32.26192554396834</v>
       </c>
       <c r="D289" t="s">
         <v>305</v>
@@ -6219,7 +6219,7 @@
         <v>292</v>
       </c>
       <c r="C290">
-        <v>46.30334327644062</v>
+        <v>17.5242987033594</v>
       </c>
       <c r="D290" t="s">
         <v>305</v>
@@ -6236,7 +6236,7 @@
         <v>293</v>
       </c>
       <c r="C291">
-        <v>27.70912746751741</v>
+        <v>9.531728776527913</v>
       </c>
       <c r="D291" t="s">
         <v>305</v>
@@ -6253,7 +6253,7 @@
         <v>294</v>
       </c>
       <c r="C292">
-        <v>27.18128535288749</v>
+        <v>11.13790166297348</v>
       </c>
       <c r="D292" t="s">
         <v>305</v>
@@ -6270,7 +6270,7 @@
         <v>295</v>
       </c>
       <c r="C293">
-        <v>12.83985412354536</v>
+        <v>17.15653944246657</v>
       </c>
       <c r="D293" t="s">
         <v>305</v>
@@ -6287,7 +6287,7 @@
         <v>296</v>
       </c>
       <c r="C294">
-        <v>15.71064615382864</v>
+        <v>47.67117698911917</v>
       </c>
       <c r="D294" t="s">
         <v>305</v>
@@ -6304,7 +6304,7 @@
         <v>297</v>
       </c>
       <c r="C295">
-        <v>25.16792312164694</v>
+        <v>24.73042871195502</v>
       </c>
       <c r="D295" t="s">
         <v>305</v>
@@ -6321,7 +6321,7 @@
         <v>298</v>
       </c>
       <c r="C296">
-        <v>11.58101563697543</v>
+        <v>58.54799188611444</v>
       </c>
       <c r="D296" t="s">
         <v>305</v>
@@ -6338,7 +6338,7 @@
         <v>299</v>
       </c>
       <c r="C297">
-        <v>14.81654321915341</v>
+        <v>28.4465670877616</v>
       </c>
       <c r="D297" t="s">
         <v>305</v>
@@ -6355,7 +6355,7 @@
         <v>300</v>
       </c>
       <c r="C298">
-        <v>22.1488808914482</v>
+        <v>52.09073091732892</v>
       </c>
       <c r="D298" t="s">
         <v>305</v>
@@ -6372,7 +6372,7 @@
         <v>301</v>
       </c>
       <c r="C299">
-        <v>33.48184847750397</v>
+        <v>27.36332623560546</v>
       </c>
       <c r="D299" t="s">
         <v>305</v>
@@ -6389,7 +6389,7 @@
         <v>302</v>
       </c>
       <c r="C300">
-        <v>15.49447972837646</v>
+        <v>10.56634989511021</v>
       </c>
       <c r="D300" t="s">
         <v>305</v>
@@ -6406,7 +6406,7 @@
         <v>303</v>
       </c>
       <c r="C301">
-        <v>21.6099808595602</v>
+        <v>31.98614624218054</v>
       </c>
       <c r="D301" t="s">
         <v>305</v>

</xml_diff>

<commit_message>
EV charging implementation and load flows
new all analysis done in excel
</commit_message>
<xml_diff>
--- a/EVbehaviour.xlsx
+++ b/EVbehaviour.xlsx
@@ -28,904 +28,904 @@
     <t>Time of Day</t>
   </si>
   <si>
-    <t>08:54:39.592169</t>
-  </si>
-  <si>
-    <t>08:49:43.060807</t>
-  </si>
-  <si>
-    <t>08:29:47.228658</t>
-  </si>
-  <si>
-    <t>09:30:02.234787</t>
-  </si>
-  <si>
-    <t>09:18:20.735672</t>
-  </si>
-  <si>
-    <t>09:07:54.818432</t>
-  </si>
-  <si>
-    <t>09:47:30.299007</t>
-  </si>
-  <si>
-    <t>09:28:31.044949</t>
-  </si>
-  <si>
-    <t>09:09:06.393013</t>
-  </si>
-  <si>
-    <t>08:36:49.861243</t>
-  </si>
-  <si>
-    <t>09:58:02.747126</t>
-  </si>
-  <si>
-    <t>08:34:41.736145</t>
-  </si>
-  <si>
-    <t>08:57:31.207979</t>
-  </si>
-  <si>
-    <t>08:32:07.590603</t>
-  </si>
-  <si>
-    <t>10:22:40.564528</t>
-  </si>
-  <si>
-    <t>09:39:52.463691</t>
-  </si>
-  <si>
-    <t>08:13:06.785650</t>
-  </si>
-  <si>
-    <t>09:55:48.235327</t>
-  </si>
-  <si>
-    <t>09:03:57.504976</t>
-  </si>
-  <si>
-    <t>09:32:02.896655</t>
-  </si>
-  <si>
-    <t>08:48:00.663896</t>
-  </si>
-  <si>
-    <t>09:17:10.847971</t>
-  </si>
-  <si>
-    <t>10:15:16.999403</t>
-  </si>
-  <si>
-    <t>09:18:07.882279</t>
-  </si>
-  <si>
-    <t>08:53:05.246968</t>
-  </si>
-  <si>
-    <t>09:21:30.463905</t>
-  </si>
-  <si>
-    <t>09:09:00.813692</t>
-  </si>
-  <si>
-    <t>08:17:48.297945</t>
-  </si>
-  <si>
-    <t>08:32:59.021935</t>
-  </si>
-  <si>
-    <t>09:37:41.374741</t>
-  </si>
-  <si>
-    <t>07:57:26.352662</t>
-  </si>
-  <si>
-    <t>08:25:56.596202</t>
-  </si>
-  <si>
-    <t>08:15:02.164131</t>
-  </si>
-  <si>
-    <t>09:35:11.887004</t>
-  </si>
-  <si>
-    <t>08:32:12.843084</t>
-  </si>
-  <si>
-    <t>08:59:30.832153</t>
-  </si>
-  <si>
-    <t>09:12:04.829903</t>
-  </si>
-  <si>
-    <t>08:45:00.699737</t>
-  </si>
-  <si>
-    <t>09:20:52.256206</t>
-  </si>
-  <si>
-    <t>08:58:07.203992</t>
-  </si>
-  <si>
-    <t>09:00:29.078099</t>
-  </si>
-  <si>
-    <t>09:48:29.664968</t>
-  </si>
-  <si>
-    <t>09:05:46.988042</t>
-  </si>
-  <si>
-    <t>08:54:13.244231</t>
-  </si>
-  <si>
-    <t>08:54:07.987990</t>
-  </si>
-  <si>
-    <t>08:28:37.885003</t>
-  </si>
-  <si>
-    <t>08:01:51.539692</t>
-  </si>
-  <si>
-    <t>08:52:06.443389</t>
-  </si>
-  <si>
-    <t>08:33:17.104134</t>
-  </si>
-  <si>
-    <t>08:39:36.513326</t>
-  </si>
-  <si>
-    <t>09:25:34.749937</t>
-  </si>
-  <si>
-    <t>09:22:37.567165</t>
-  </si>
-  <si>
-    <t>08:53:51.507828</t>
-  </si>
-  <si>
-    <t>10:54:13.929165</t>
-  </si>
-  <si>
-    <t>08:54:47.722561</t>
-  </si>
-  <si>
-    <t>09:14:58.428644</t>
-  </si>
-  <si>
-    <t>09:12:13.823723</t>
-  </si>
-  <si>
-    <t>09:40:12.148769</t>
-  </si>
-  <si>
-    <t>10:20:28.988336</t>
-  </si>
-  <si>
-    <t>08:56:09.394249</t>
-  </si>
-  <si>
-    <t>10:14:23.086915</t>
-  </si>
-  <si>
-    <t>09:05:10.927808</t>
-  </si>
-  <si>
-    <t>08:40:42.899350</t>
-  </si>
-  <si>
-    <t>08:44:57.532045</t>
-  </si>
-  <si>
-    <t>09:21:19.996318</t>
-  </si>
-  <si>
-    <t>08:01:25.826931</t>
-  </si>
-  <si>
-    <t>08:52:19.848230</t>
-  </si>
-  <si>
-    <t>08:53:59.869670</t>
-  </si>
-  <si>
-    <t>08:29:11.544270</t>
-  </si>
-  <si>
-    <t>08:59:18.366680</t>
-  </si>
-  <si>
-    <t>08:36:36.092530</t>
-  </si>
-  <si>
-    <t>09:33:04.994371</t>
-  </si>
-  <si>
-    <t>09:48:03.948453</t>
-  </si>
-  <si>
-    <t>08:38:16.965407</t>
-  </si>
-  <si>
-    <t>08:20:24.141887</t>
-  </si>
-  <si>
-    <t>08:37:00.062404</t>
-  </si>
-  <si>
-    <t>09:49:20.416540</t>
-  </si>
-  <si>
-    <t>09:02:58.899739</t>
-  </si>
-  <si>
-    <t>09:11:37.881799</t>
-  </si>
-  <si>
-    <t>08:07:00.291838</t>
-  </si>
-  <si>
-    <t>09:38:00.197924</t>
-  </si>
-  <si>
-    <t>09:23:39.570286</t>
-  </si>
-  <si>
-    <t>08:48:38.722976</t>
-  </si>
-  <si>
-    <t>09:00:50.924328</t>
-  </si>
-  <si>
-    <t>08:57:48.097782</t>
-  </si>
-  <si>
-    <t>09:17:10.146292</t>
-  </si>
-  <si>
-    <t>10:03:56.203155</t>
-  </si>
-  <si>
-    <t>09:14:13.487679</t>
-  </si>
-  <si>
-    <t>08:36:53.291483</t>
-  </si>
-  <si>
-    <t>09:39:15.346811</t>
-  </si>
-  <si>
-    <t>08:54:01.111360</t>
-  </si>
-  <si>
-    <t>09:33:44.043123</t>
-  </si>
-  <si>
-    <t>08:21:24.594790</t>
-  </si>
-  <si>
-    <t>08:17:54.405016</t>
-  </si>
-  <si>
-    <t>09:01:13.460695</t>
-  </si>
-  <si>
-    <t>08:43:45.237182</t>
-  </si>
-  <si>
-    <t>08:45:03.664945</t>
-  </si>
-  <si>
-    <t>10:08:08.134456</t>
-  </si>
-  <si>
-    <t>10:37:20.056857</t>
-  </si>
-  <si>
-    <t>08:24:57.308945</t>
-  </si>
-  <si>
-    <t>09:35:23.340767</t>
-  </si>
-  <si>
-    <t>08:41:32.609052</t>
-  </si>
-  <si>
-    <t>09:14:22.527821</t>
-  </si>
-  <si>
-    <t>08:32:22.274882</t>
-  </si>
-  <si>
-    <t>09:23:41.536545</t>
-  </si>
-  <si>
-    <t>09:03:06.970192</t>
-  </si>
-  <si>
-    <t>08:51:51.538216</t>
-  </si>
-  <si>
-    <t>09:41:25.374807</t>
-  </si>
-  <si>
-    <t>09:16:47.388362</t>
-  </si>
-  <si>
-    <t>10:03:24.530715</t>
-  </si>
-  <si>
-    <t>08:43:03.898921</t>
-  </si>
-  <si>
-    <t>09:00:59.342543</t>
-  </si>
-  <si>
-    <t>08:22:12.396584</t>
-  </si>
-  <si>
-    <t>09:26:21.899549</t>
-  </si>
-  <si>
-    <t>08:20:01.441538</t>
-  </si>
-  <si>
-    <t>09:32:44.157149</t>
-  </si>
-  <si>
-    <t>09:17:08.064366</t>
-  </si>
-  <si>
-    <t>09:20:02.226146</t>
-  </si>
-  <si>
-    <t>08:42:51.080042</t>
-  </si>
-  <si>
-    <t>08:19:12.000106</t>
-  </si>
-  <si>
-    <t>08:21:43.822561</t>
-  </si>
-  <si>
-    <t>10:07:02.630566</t>
-  </si>
-  <si>
-    <t>08:31:49.943268</t>
-  </si>
-  <si>
-    <t>08:21:19.126860</t>
-  </si>
-  <si>
-    <t>08:25:12.822850</t>
-  </si>
-  <si>
-    <t>08:38:19.823181</t>
-  </si>
-  <si>
-    <t>09:26:23.257366</t>
-  </si>
-  <si>
-    <t>08:53:21.341732</t>
-  </si>
-  <si>
-    <t>09:05:17.595409</t>
-  </si>
-  <si>
-    <t>08:46:43.826745</t>
-  </si>
-  <si>
-    <t>09:18:09.286606</t>
-  </si>
-  <si>
-    <t>09:08:43.401801</t>
-  </si>
-  <si>
-    <t>09:07:31.689706</t>
-  </si>
-  <si>
-    <t>10:45:50.390158</t>
-  </si>
-  <si>
-    <t>09:12:00.888751</t>
-  </si>
-  <si>
-    <t>09:54:29.836462</t>
-  </si>
-  <si>
-    <t>09:32:51.453188</t>
-  </si>
-  <si>
-    <t>09:15:41.178619</t>
-  </si>
-  <si>
-    <t>08:53:35.956275</t>
-  </si>
-  <si>
-    <t>08:59:53.162332</t>
-  </si>
-  <si>
-    <t>08:55:10.812460</t>
-  </si>
-  <si>
-    <t>07:57:07.978992</t>
-  </si>
-  <si>
-    <t>08:41:49.440619</t>
-  </si>
-  <si>
-    <t>08:44:12.668569</t>
-  </si>
-  <si>
-    <t>08:09:08.736595</t>
-  </si>
-  <si>
-    <t>10:23:26.974313</t>
-  </si>
-  <si>
-    <t>08:29:37.875220</t>
-  </si>
-  <si>
-    <t>08:34:44.219548</t>
-  </si>
-  <si>
-    <t>09:12:02.416313</t>
-  </si>
-  <si>
-    <t>09:21:07.507986</t>
-  </si>
-  <si>
-    <t>10:12:23.655988</t>
-  </si>
-  <si>
-    <t>09:07:58.244792</t>
-  </si>
-  <si>
-    <t>08:30:12.649329</t>
-  </si>
-  <si>
-    <t>08:29:28.163370</t>
-  </si>
-  <si>
-    <t>09:00:25.340379</t>
-  </si>
-  <si>
-    <t>09:41:06.554991</t>
-  </si>
-  <si>
-    <t>08:45:12.029511</t>
-  </si>
-  <si>
-    <t>09:05:44.932580</t>
-  </si>
-  <si>
-    <t>08:41:26.430389</t>
-  </si>
-  <si>
-    <t>09:19:21.692044</t>
-  </si>
-  <si>
-    <t>10:23:48.317141</t>
-  </si>
-  <si>
-    <t>09:22:03.425966</t>
-  </si>
-  <si>
-    <t>11:10:37.987008</t>
-  </si>
-  <si>
-    <t>14:53:15.763025</t>
-  </si>
-  <si>
-    <t>15:53:04.357438</t>
-  </si>
-  <si>
-    <t>15:50:13.944183</t>
-  </si>
-  <si>
-    <t>15:40:11.748185</t>
-  </si>
-  <si>
-    <t>16:26:15.025659</t>
-  </si>
-  <si>
-    <t>14:27:43.319576</t>
-  </si>
-  <si>
-    <t>14:28:57.791292</t>
-  </si>
-  <si>
-    <t>16:59:44.626608</t>
-  </si>
-  <si>
-    <t>14:33:17.292435</t>
-  </si>
-  <si>
-    <t>17:04:33.514744</t>
-  </si>
-  <si>
-    <t>16:41:52.227263</t>
-  </si>
-  <si>
-    <t>15:22:44.708165</t>
-  </si>
-  <si>
-    <t>15:39:37.127687</t>
-  </si>
-  <si>
-    <t>13:32:07.186508</t>
-  </si>
-  <si>
-    <t>12:27:16.526950</t>
-  </si>
-  <si>
-    <t>17:03:37.147709</t>
-  </si>
-  <si>
-    <t>16:16:14.204616</t>
-  </si>
-  <si>
-    <t>16:23:33.419600</t>
-  </si>
-  <si>
-    <t>12:19:12.102264</t>
-  </si>
-  <si>
-    <t>13:35:12.962089</t>
-  </si>
-  <si>
-    <t>17:05:48.068319</t>
-  </si>
-  <si>
-    <t>15:11:05.967448</t>
-  </si>
-  <si>
-    <t>15:33:10.434708</t>
-  </si>
-  <si>
-    <t>17:04:16.925825</t>
-  </si>
-  <si>
-    <t>12:47:46.310400</t>
-  </si>
-  <si>
-    <t>16:07:22.512665</t>
-  </si>
-  <si>
-    <t>14:09:24.595633</t>
-  </si>
-  <si>
-    <t>17:19:15.953990</t>
-  </si>
-  <si>
-    <t>13:32:59.069341</t>
-  </si>
-  <si>
-    <t>15:10:35.256766</t>
-  </si>
-  <si>
-    <t>14:28:40.873041</t>
-  </si>
-  <si>
-    <t>16:46:39.813526</t>
-  </si>
-  <si>
-    <t>16:59:06.126022</t>
-  </si>
-  <si>
-    <t>15:43:57.999753</t>
-  </si>
-  <si>
-    <t>15:38:26.440462</t>
-  </si>
-  <si>
-    <t>15:37:01.393377</t>
-  </si>
-  <si>
-    <t>15:53:06.821927</t>
-  </si>
-  <si>
-    <t>14:59:10.601788</t>
-  </si>
-  <si>
-    <t>14:01:08.395174</t>
-  </si>
-  <si>
-    <t>15:46:08.729421</t>
-  </si>
-  <si>
-    <t>17:02:09.516942</t>
-  </si>
-  <si>
-    <t>14:53:21.041956</t>
-  </si>
-  <si>
-    <t>16:18:47.278428</t>
-  </si>
-  <si>
-    <t>15:06:27.209018</t>
-  </si>
-  <si>
-    <t>16:16:30.394535</t>
-  </si>
-  <si>
-    <t>15:20:08.196329</t>
-  </si>
-  <si>
-    <t>15:39:21.329701</t>
-  </si>
-  <si>
-    <t>12:03:24.934819</t>
-  </si>
-  <si>
-    <t>14:54:59.353865</t>
-  </si>
-  <si>
-    <t>16:22:12.339712</t>
-  </si>
-  <si>
-    <t>16:49:51.252504</t>
-  </si>
-  <si>
-    <t>15:39:09.096549</t>
-  </si>
-  <si>
-    <t>16:38:54.535723</t>
-  </si>
-  <si>
-    <t>15:58:14.486771</t>
-  </si>
-  <si>
-    <t>17:26:15.843454</t>
-  </si>
-  <si>
-    <t>16:40:52.941984</t>
-  </si>
-  <si>
-    <t>15:12:56.313788</t>
-  </si>
-  <si>
-    <t>15:50:21.343068</t>
-  </si>
-  <si>
-    <t>13:51:30.269253</t>
-  </si>
-  <si>
-    <t>15:55:50.190011</t>
-  </si>
-  <si>
-    <t>16:40:59.761827</t>
-  </si>
-  <si>
-    <t>12:51:58.759854</t>
-  </si>
-  <si>
-    <t>16:28:32.457688</t>
-  </si>
-  <si>
-    <t>15:15:25.165546</t>
-  </si>
-  <si>
-    <t>16:43:40.341126</t>
-  </si>
-  <si>
-    <t>13:45:56.684469</t>
-  </si>
-  <si>
-    <t>12:26:16.427863</t>
-  </si>
-  <si>
-    <t>16:44:30.417153</t>
-  </si>
-  <si>
-    <t>15:51:10.536091</t>
-  </si>
-  <si>
-    <t>16:35:30.833991</t>
-  </si>
-  <si>
-    <t>15:20:49.988242</t>
-  </si>
-  <si>
-    <t>12:56:52.573613</t>
-  </si>
-  <si>
-    <t>16:01:18.952971</t>
-  </si>
-  <si>
-    <t>15:54:37.079531</t>
-  </si>
-  <si>
-    <t>16:19:42.576679</t>
-  </si>
-  <si>
-    <t>14:41:47.927653</t>
-  </si>
-  <si>
-    <t>16:44:12.036780</t>
-  </si>
-  <si>
-    <t>16:19:25.648838</t>
-  </si>
-  <si>
-    <t>14:45:33.567576</t>
-  </si>
-  <si>
-    <t>15:06:15.419455</t>
-  </si>
-  <si>
-    <t>16:09:03.815213</t>
-  </si>
-  <si>
-    <t>15:17:15.333745</t>
-  </si>
-  <si>
-    <t>14:10:34.925163</t>
-  </si>
-  <si>
-    <t>14:59:53.021659</t>
-  </si>
-  <si>
-    <t>15:45:07.228601</t>
-  </si>
-  <si>
-    <t>15:37:08.206663</t>
-  </si>
-  <si>
-    <t>15:43:03.920368</t>
-  </si>
-  <si>
-    <t>15:34:14.056459</t>
-  </si>
-  <si>
-    <t>13:13:33.993979</t>
-  </si>
-  <si>
-    <t>16:30:08.482890</t>
-  </si>
-  <si>
-    <t>12:02:20.908677</t>
-  </si>
-  <si>
-    <t>15:22:03.977995</t>
-  </si>
-  <si>
-    <t>15:40:11.838707</t>
-  </si>
-  <si>
-    <t>17:33:32.327413</t>
-  </si>
-  <si>
-    <t>16:11:31.016491</t>
-  </si>
-  <si>
-    <t>14:32:09.126945</t>
-  </si>
-  <si>
-    <t>16:32:18.837883</t>
-  </si>
-  <si>
-    <t>14:52:16.691542</t>
-  </si>
-  <si>
-    <t>16:08:48.698585</t>
-  </si>
-  <si>
-    <t>14:22:44.166553</t>
-  </si>
-  <si>
-    <t>14:58:04.157603</t>
-  </si>
-  <si>
-    <t>16:16:00.434654</t>
-  </si>
-  <si>
-    <t>15:39:23.359678</t>
-  </si>
-  <si>
-    <t>15:25:55.779215</t>
-  </si>
-  <si>
-    <t>15:20:38.440910</t>
-  </si>
-  <si>
-    <t>15:45:13.256055</t>
-  </si>
-  <si>
-    <t>16:24:27.108258</t>
-  </si>
-  <si>
-    <t>13:33:48.314235</t>
-  </si>
-  <si>
-    <t>13:47:18.440977</t>
-  </si>
-  <si>
-    <t>14:53:55.528825</t>
-  </si>
-  <si>
-    <t>14:22:55.198570</t>
-  </si>
-  <si>
-    <t>13:34:56.284674</t>
-  </si>
-  <si>
-    <t>14:21:37.652803</t>
-  </si>
-  <si>
-    <t>13:03:06.921308</t>
-  </si>
-  <si>
-    <t>14:05:33.103010</t>
-  </si>
-  <si>
-    <t>13:37:15.720786</t>
-  </si>
-  <si>
-    <t>14:05:13.137944</t>
-  </si>
-  <si>
-    <t>13:08:52.197222</t>
-  </si>
-  <si>
-    <t>14:12:49.067069</t>
-  </si>
-  <si>
-    <t>14:23:30.161060</t>
-  </si>
-  <si>
-    <t>13:42:41.286655</t>
-  </si>
-  <si>
-    <t>14:37:05.494547</t>
-  </si>
-  <si>
-    <t>14:22:33.829556</t>
-  </si>
-  <si>
-    <t>13:37:11.362577</t>
-  </si>
-  <si>
-    <t>15:27:34.856577</t>
-  </si>
-  <si>
-    <t>13:48:46.612887</t>
-  </si>
-  <si>
-    <t>12:38:21.833045</t>
-  </si>
-  <si>
-    <t>13:29:51.800939</t>
-  </si>
-  <si>
-    <t>13:57:59.357536</t>
-  </si>
-  <si>
-    <t>13:41:00.064081</t>
-  </si>
-  <si>
-    <t>14:44:47.126199</t>
-  </si>
-  <si>
-    <t>14:00:29.208678</t>
-  </si>
-  <si>
-    <t>13:52:29.859850</t>
-  </si>
-  <si>
-    <t>14:25:34.133170</t>
-  </si>
-  <si>
-    <t>14:15:30.396481</t>
-  </si>
-  <si>
-    <t>14:24:59.178375</t>
-  </si>
-  <si>
-    <t>13:45:02.643511</t>
+    <t>10:00:30.964361</t>
+  </si>
+  <si>
+    <t>08:38:28.304690</t>
+  </si>
+  <si>
+    <t>08:37:30.051338</t>
+  </si>
+  <si>
+    <t>09:35:52.583326</t>
+  </si>
+  <si>
+    <t>08:42:57.308795</t>
+  </si>
+  <si>
+    <t>10:05:19.270131</t>
+  </si>
+  <si>
+    <t>09:21:45.409564</t>
+  </si>
+  <si>
+    <t>08:44:11.732088</t>
+  </si>
+  <si>
+    <t>08:49:31.038316</t>
+  </si>
+  <si>
+    <t>09:20:17.335968</t>
+  </si>
+  <si>
+    <t>08:29:52.197331</t>
+  </si>
+  <si>
+    <t>08:14:06.425661</t>
+  </si>
+  <si>
+    <t>10:51:16.439821</t>
+  </si>
+  <si>
+    <t>08:40:52.709524</t>
+  </si>
+  <si>
+    <t>09:27:39.317710</t>
+  </si>
+  <si>
+    <t>08:29:39.532590</t>
+  </si>
+  <si>
+    <t>09:02:58.237195</t>
+  </si>
+  <si>
+    <t>08:37:12.348780</t>
+  </si>
+  <si>
+    <t>09:14:08.830680</t>
+  </si>
+  <si>
+    <t>08:41:35.217476</t>
+  </si>
+  <si>
+    <t>08:40:24.290702</t>
+  </si>
+  <si>
+    <t>10:00:58.194239</t>
+  </si>
+  <si>
+    <t>08:40:27.093418</t>
+  </si>
+  <si>
+    <t>09:31:08.581755</t>
+  </si>
+  <si>
+    <t>09:08:05.807467</t>
+  </si>
+  <si>
+    <t>09:39:57.387629</t>
+  </si>
+  <si>
+    <t>08:52:36.767967</t>
+  </si>
+  <si>
+    <t>08:34:06.159185</t>
+  </si>
+  <si>
+    <t>08:38:13.557532</t>
+  </si>
+  <si>
+    <t>08:51:21.881896</t>
+  </si>
+  <si>
+    <t>08:46:37.178219</t>
+  </si>
+  <si>
+    <t>09:12:47.483278</t>
+  </si>
+  <si>
+    <t>08:25:03.464828</t>
+  </si>
+  <si>
+    <t>10:13:09.282822</t>
+  </si>
+  <si>
+    <t>10:25:31.371755</t>
+  </si>
+  <si>
+    <t>10:25:17.970541</t>
+  </si>
+  <si>
+    <t>08:44:30.095671</t>
+  </si>
+  <si>
+    <t>09:37:21.093046</t>
+  </si>
+  <si>
+    <t>09:07:39.032031</t>
+  </si>
+  <si>
+    <t>11:06:15.349304</t>
+  </si>
+  <si>
+    <t>09:03:46.379927</t>
+  </si>
+  <si>
+    <t>09:02:00.912547</t>
+  </si>
+  <si>
+    <t>09:12:15.034528</t>
+  </si>
+  <si>
+    <t>09:05:16.231835</t>
+  </si>
+  <si>
+    <t>09:22:55.229482</t>
+  </si>
+  <si>
+    <t>08:52:10.068570</t>
+  </si>
+  <si>
+    <t>09:43:26.377778</t>
+  </si>
+  <si>
+    <t>09:02:34.882281</t>
+  </si>
+  <si>
+    <t>10:10:21.230338</t>
+  </si>
+  <si>
+    <t>11:20:15.409694</t>
+  </si>
+  <si>
+    <t>08:56:26.418825</t>
+  </si>
+  <si>
+    <t>08:58:03.444375</t>
+  </si>
+  <si>
+    <t>09:12:58.848106</t>
+  </si>
+  <si>
+    <t>09:25:56.384214</t>
+  </si>
+  <si>
+    <t>10:22:49.720308</t>
+  </si>
+  <si>
+    <t>09:04:47.438824</t>
+  </si>
+  <si>
+    <t>09:30:14.242506</t>
+  </si>
+  <si>
+    <t>09:26:00.864508</t>
+  </si>
+  <si>
+    <t>08:47:42.321098</t>
+  </si>
+  <si>
+    <t>10:23:44.691154</t>
+  </si>
+  <si>
+    <t>08:21:21.373930</t>
+  </si>
+  <si>
+    <t>09:07:25.643298</t>
+  </si>
+  <si>
+    <t>09:23:51.485220</t>
+  </si>
+  <si>
+    <t>09:19:00.821300</t>
+  </si>
+  <si>
+    <t>08:56:14.996482</t>
+  </si>
+  <si>
+    <t>08:57:25.857747</t>
+  </si>
+  <si>
+    <t>08:35:07.758985</t>
+  </si>
+  <si>
+    <t>09:58:27.158445</t>
+  </si>
+  <si>
+    <t>09:12:41.549918</t>
+  </si>
+  <si>
+    <t>08:57:28.177873</t>
+  </si>
+  <si>
+    <t>08:31:47.011410</t>
+  </si>
+  <si>
+    <t>08:21:23.507195</t>
+  </si>
+  <si>
+    <t>09:46:30.435068</t>
+  </si>
+  <si>
+    <t>08:49:00.853566</t>
+  </si>
+  <si>
+    <t>08:34:11.609567</t>
+  </si>
+  <si>
+    <t>09:57:15.931461</t>
+  </si>
+  <si>
+    <t>11:14:51.855830</t>
+  </si>
+  <si>
+    <t>09:35:59.301791</t>
+  </si>
+  <si>
+    <t>10:44:09.462280</t>
+  </si>
+  <si>
+    <t>08:49:02.468040</t>
+  </si>
+  <si>
+    <t>09:26:12.381001</t>
+  </si>
+  <si>
+    <t>08:51:47.708999</t>
+  </si>
+  <si>
+    <t>08:48:57.489360</t>
+  </si>
+  <si>
+    <t>08:46:47.117021</t>
+  </si>
+  <si>
+    <t>08:28:12.142086</t>
+  </si>
+  <si>
+    <t>08:50:50.817787</t>
+  </si>
+  <si>
+    <t>09:50:05.463224</t>
+  </si>
+  <si>
+    <t>08:56:13.322115</t>
+  </si>
+  <si>
+    <t>08:36:15.103638</t>
+  </si>
+  <si>
+    <t>09:01:47.495397</t>
+  </si>
+  <si>
+    <t>09:13:51.415006</t>
+  </si>
+  <si>
+    <t>09:02:54.141679</t>
+  </si>
+  <si>
+    <t>10:08:06.901931</t>
+  </si>
+  <si>
+    <t>08:50:14.515549</t>
+  </si>
+  <si>
+    <t>08:27:43.765997</t>
+  </si>
+  <si>
+    <t>08:56:51.119557</t>
+  </si>
+  <si>
+    <t>08:05:34.841653</t>
+  </si>
+  <si>
+    <t>08:56:21.410222</t>
+  </si>
+  <si>
+    <t>09:17:48.498373</t>
+  </si>
+  <si>
+    <t>09:34:08.117214</t>
+  </si>
+  <si>
+    <t>08:40:53.659430</t>
+  </si>
+  <si>
+    <t>08:33:45.828607</t>
+  </si>
+  <si>
+    <t>08:54:01.577597</t>
+  </si>
+  <si>
+    <t>09:23:50.518245</t>
+  </si>
+  <si>
+    <t>07:57:53.989575</t>
+  </si>
+  <si>
+    <t>09:57:57.825414</t>
+  </si>
+  <si>
+    <t>08:59:05.336866</t>
+  </si>
+  <si>
+    <t>08:48:31.534938</t>
+  </si>
+  <si>
+    <t>08:34:32.488865</t>
+  </si>
+  <si>
+    <t>08:55:53.662363</t>
+  </si>
+  <si>
+    <t>12:00:02.707908</t>
+  </si>
+  <si>
+    <t>08:57:45.537264</t>
+  </si>
+  <si>
+    <t>08:58:21.985528</t>
+  </si>
+  <si>
+    <t>09:16:46.384256</t>
+  </si>
+  <si>
+    <t>08:54:52.131118</t>
+  </si>
+  <si>
+    <t>09:32:37.540596</t>
+  </si>
+  <si>
+    <t>08:40:22.547043</t>
+  </si>
+  <si>
+    <t>09:40:39.852843</t>
+  </si>
+  <si>
+    <t>10:38:38.765243</t>
+  </si>
+  <si>
+    <t>09:17:58.131436</t>
+  </si>
+  <si>
+    <t>09:16:51.529126</t>
+  </si>
+  <si>
+    <t>08:26:39.957607</t>
+  </si>
+  <si>
+    <t>09:10:14.471454</t>
+  </si>
+  <si>
+    <t>09:25:29.368144</t>
+  </si>
+  <si>
+    <t>10:11:36.725310</t>
+  </si>
+  <si>
+    <t>09:00:35.778192</t>
+  </si>
+  <si>
+    <t>10:01:21.416367</t>
+  </si>
+  <si>
+    <t>08:45:29.870287</t>
+  </si>
+  <si>
+    <t>09:12:44.676688</t>
+  </si>
+  <si>
+    <t>08:22:56.855846</t>
+  </si>
+  <si>
+    <t>09:21:27.374370</t>
+  </si>
+  <si>
+    <t>09:05:23.248565</t>
+  </si>
+  <si>
+    <t>09:27:45.182139</t>
+  </si>
+  <si>
+    <t>09:48:19.543735</t>
+  </si>
+  <si>
+    <t>10:09:09.488087</t>
+  </si>
+  <si>
+    <t>08:17:31.058695</t>
+  </si>
+  <si>
+    <t>09:05:22.278144</t>
+  </si>
+  <si>
+    <t>08:17:17.073580</t>
+  </si>
+  <si>
+    <t>09:10:38.915071</t>
+  </si>
+  <si>
+    <t>10:04:45.899974</t>
+  </si>
+  <si>
+    <t>07:47:52.296279</t>
+  </si>
+  <si>
+    <t>08:31:17.047727</t>
+  </si>
+  <si>
+    <t>09:22:36.121406</t>
+  </si>
+  <si>
+    <t>10:30:52.660172</t>
+  </si>
+  <si>
+    <t>08:17:59.391624</t>
+  </si>
+  <si>
+    <t>09:10:59.470900</t>
+  </si>
+  <si>
+    <t>09:00:20.667100</t>
+  </si>
+  <si>
+    <t>09:33:03.739876</t>
+  </si>
+  <si>
+    <t>08:37:21.843004</t>
+  </si>
+  <si>
+    <t>09:12:16.057694</t>
+  </si>
+  <si>
+    <t>10:08:57.282437</t>
+  </si>
+  <si>
+    <t>08:33:38.844982</t>
+  </si>
+  <si>
+    <t>09:07:56.211572</t>
+  </si>
+  <si>
+    <t>10:15:41.256827</t>
+  </si>
+  <si>
+    <t>10:40:34.744349</t>
+  </si>
+  <si>
+    <t>10:06:15.308113</t>
+  </si>
+  <si>
+    <t>08:34:53.304494</t>
+  </si>
+  <si>
+    <t>08:38:31.052754</t>
+  </si>
+  <si>
+    <t>10:18:17.511736</t>
+  </si>
+  <si>
+    <t>11:06:21.226774</t>
+  </si>
+  <si>
+    <t>08:56:08.679719</t>
+  </si>
+  <si>
+    <t>08:24:54.819193</t>
+  </si>
+  <si>
+    <t>14:41:34.490409</t>
+  </si>
+  <si>
+    <t>13:51:21.795206</t>
+  </si>
+  <si>
+    <t>13:33:54.538206</t>
+  </si>
+  <si>
+    <t>15:52:19.289937</t>
+  </si>
+  <si>
+    <t>16:31:58.739052</t>
+  </si>
+  <si>
+    <t>16:45:30.238908</t>
+  </si>
+  <si>
+    <t>15:30:53.956274</t>
+  </si>
+  <si>
+    <t>16:26:38.198790</t>
+  </si>
+  <si>
+    <t>16:01:13.682687</t>
+  </si>
+  <si>
+    <t>16:19:55.474169</t>
+  </si>
+  <si>
+    <t>16:27:45.844688</t>
+  </si>
+  <si>
+    <t>15:09:39.908520</t>
+  </si>
+  <si>
+    <t>14:48:55.401790</t>
+  </si>
+  <si>
+    <t>16:03:19.167907</t>
+  </si>
+  <si>
+    <t>16:46:00.530482</t>
+  </si>
+  <si>
+    <t>16:16:12.767184</t>
+  </si>
+  <si>
+    <t>16:03:26.940764</t>
+  </si>
+  <si>
+    <t>15:10:33.631905</t>
+  </si>
+  <si>
+    <t>16:48:59.352780</t>
+  </si>
+  <si>
+    <t>15:48:41.690851</t>
+  </si>
+  <si>
+    <t>16:02:01.464133</t>
+  </si>
+  <si>
+    <t>16:45:47.901937</t>
+  </si>
+  <si>
+    <t>14:47:16.210373</t>
+  </si>
+  <si>
+    <t>16:08:58.229522</t>
+  </si>
+  <si>
+    <t>13:45:32.083279</t>
+  </si>
+  <si>
+    <t>16:19:57.689322</t>
+  </si>
+  <si>
+    <t>15:30:50.403354</t>
+  </si>
+  <si>
+    <t>13:13:35.542147</t>
+  </si>
+  <si>
+    <t>16:07:24.180223</t>
+  </si>
+  <si>
+    <t>16:11:15.950642</t>
+  </si>
+  <si>
+    <t>16:26:09.173412</t>
+  </si>
+  <si>
+    <t>13:36:14.272924</t>
+  </si>
+  <si>
+    <t>15:36:05.620386</t>
+  </si>
+  <si>
+    <t>14:46:16.745767</t>
+  </si>
+  <si>
+    <t>14:24:26.308424</t>
+  </si>
+  <si>
+    <t>16:42:36.644292</t>
+  </si>
+  <si>
+    <t>16:45:39.427635</t>
+  </si>
+  <si>
+    <t>14:24:15.912842</t>
+  </si>
+  <si>
+    <t>14:48:13.913234</t>
+  </si>
+  <si>
+    <t>15:30:50.555874</t>
+  </si>
+  <si>
+    <t>16:09:25.312980</t>
+  </si>
+  <si>
+    <t>15:19:58.097579</t>
+  </si>
+  <si>
+    <t>16:17:59.178956</t>
+  </si>
+  <si>
+    <t>16:38:31.198919</t>
+  </si>
+  <si>
+    <t>16:01:03.288790</t>
+  </si>
+  <si>
+    <t>16:22:04.207964</t>
+  </si>
+  <si>
+    <t>16:44:19.009087</t>
+  </si>
+  <si>
+    <t>16:02:22.202999</t>
+  </si>
+  <si>
+    <t>16:27:23.514169</t>
+  </si>
+  <si>
+    <t>16:04:54.734842</t>
+  </si>
+  <si>
+    <t>14:57:46.095560</t>
+  </si>
+  <si>
+    <t>13:46:57.018857</t>
+  </si>
+  <si>
+    <t>15:27:36.944699</t>
+  </si>
+  <si>
+    <t>14:49:59.178139</t>
+  </si>
+  <si>
+    <t>15:39:19.314664</t>
+  </si>
+  <si>
+    <t>16:35:57.189014</t>
+  </si>
+  <si>
+    <t>14:41:23.656242</t>
+  </si>
+  <si>
+    <t>15:00:37.837304</t>
+  </si>
+  <si>
+    <t>15:33:49.581467</t>
+  </si>
+  <si>
+    <t>17:04:02.181886</t>
+  </si>
+  <si>
+    <t>14:53:54.989183</t>
+  </si>
+  <si>
+    <t>16:51:33.590148</t>
+  </si>
+  <si>
+    <t>16:31:28.333430</t>
+  </si>
+  <si>
+    <t>14:49:09.087566</t>
+  </si>
+  <si>
+    <t>14:17:57.462687</t>
+  </si>
+  <si>
+    <t>15:13:27.167280</t>
+  </si>
+  <si>
+    <t>15:34:06.025196</t>
+  </si>
+  <si>
+    <t>16:04:20.531977</t>
+  </si>
+  <si>
+    <t>13:18:20.960807</t>
+  </si>
+  <si>
+    <t>15:17:09.540292</t>
+  </si>
+  <si>
+    <t>17:29:54.429638</t>
+  </si>
+  <si>
+    <t>15:40:43.447855</t>
+  </si>
+  <si>
+    <t>16:42:57.492599</t>
+  </si>
+  <si>
+    <t>15:04:36.178703</t>
+  </si>
+  <si>
+    <t>16:28:26.211407</t>
+  </si>
+  <si>
+    <t>14:19:07.429319</t>
+  </si>
+  <si>
+    <t>16:26:56.225579</t>
+  </si>
+  <si>
+    <t>16:18:20.502891</t>
+  </si>
+  <si>
+    <t>14:17:34.694534</t>
+  </si>
+  <si>
+    <t>16:26:11.650378</t>
+  </si>
+  <si>
+    <t>14:53:41.322220</t>
+  </si>
+  <si>
+    <t>14:04:45.563187</t>
+  </si>
+  <si>
+    <t>14:49:26.378715</t>
+  </si>
+  <si>
+    <t>15:39:13.879002</t>
+  </si>
+  <si>
+    <t>14:44:46.785327</t>
+  </si>
+  <si>
+    <t>15:10:11.474427</t>
+  </si>
+  <si>
+    <t>15:20:15.453949</t>
+  </si>
+  <si>
+    <t>15:05:30.056946</t>
+  </si>
+  <si>
+    <t>14:50:14.926761</t>
+  </si>
+  <si>
+    <t>15:51:23.394608</t>
+  </si>
+  <si>
+    <t>13:06:25.111250</t>
+  </si>
+  <si>
+    <t>15:30:52.527493</t>
+  </si>
+  <si>
+    <t>15:23:44.182373</t>
+  </si>
+  <si>
+    <t>16:24:24.945294</t>
+  </si>
+  <si>
+    <t>14:51:13.211167</t>
+  </si>
+  <si>
+    <t>15:31:37.487879</t>
+  </si>
+  <si>
+    <t>15:33:13.673610</t>
+  </si>
+  <si>
+    <t>15:26:02.282315</t>
+  </si>
+  <si>
+    <t>15:53:51.235173</t>
+  </si>
+  <si>
+    <t>11:41:39.549800</t>
+  </si>
+  <si>
+    <t>13:20:55.337412</t>
+  </si>
+  <si>
+    <t>15:55:41.833876</t>
+  </si>
+  <si>
+    <t>15:25:32.721348</t>
+  </si>
+  <si>
+    <t>16:38:17.564993</t>
+  </si>
+  <si>
+    <t>16:18:37.808219</t>
+  </si>
+  <si>
+    <t>14:23:13.625393</t>
+  </si>
+  <si>
+    <t>15:27:37.779668</t>
+  </si>
+  <si>
+    <t>15:20:35.782434</t>
+  </si>
+  <si>
+    <t>13:33:56.027360</t>
+  </si>
+  <si>
+    <t>14:06:38.904246</t>
+  </si>
+  <si>
+    <t>14:03:41.824753</t>
+  </si>
+  <si>
+    <t>13:42:59.791446</t>
+  </si>
+  <si>
+    <t>14:08:19.343845</t>
+  </si>
+  <si>
+    <t>12:52:27.627663</t>
+  </si>
+  <si>
+    <t>13:35:25.068268</t>
+  </si>
+  <si>
+    <t>15:16:16.195438</t>
+  </si>
+  <si>
+    <t>13:54:22.253538</t>
+  </si>
+  <si>
+    <t>13:36:41.192594</t>
+  </si>
+  <si>
+    <t>14:18:39.698332</t>
+  </si>
+  <si>
+    <t>13:04:03.334194</t>
+  </si>
+  <si>
+    <t>14:15:28.893551</t>
+  </si>
+  <si>
+    <t>14:12:35.668594</t>
+  </si>
+  <si>
+    <t>13:45:26.900841</t>
+  </si>
+  <si>
+    <t>13:26:57.439848</t>
+  </si>
+  <si>
+    <t>13:26:42.769165</t>
+  </si>
+  <si>
+    <t>14:28:13.905771</t>
+  </si>
+  <si>
+    <t>14:11:26.651513</t>
+  </si>
+  <si>
+    <t>13:42:52.825449</t>
+  </si>
+  <si>
+    <t>13:29:14.858966</t>
+  </si>
+  <si>
+    <t>15:28:50.262434</t>
+  </si>
+  <si>
+    <t>13:39:49.965673</t>
+  </si>
+  <si>
+    <t>14:11:02.719554</t>
+  </si>
+  <si>
+    <t>14:24:00.751998</t>
+  </si>
+  <si>
+    <t>13:56:01.952985</t>
+  </si>
+  <si>
+    <t>14:42:26.363843</t>
+  </si>
+  <si>
+    <t>13:08:43.357157</t>
+  </si>
+  <si>
+    <t>13:51:15.743648</t>
+  </si>
+  <si>
+    <t>14:08:19.800181</t>
   </si>
   <si>
     <t>Commercial</t>
@@ -1323,7 +1323,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>43.78711989497639</v>
+        <v>39.75282767225426</v>
       </c>
       <c r="D2" t="s">
         <v>304</v>
@@ -1340,7 +1340,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>16.99208002040279</v>
+        <v>11.63501624739779</v>
       </c>
       <c r="D3" t="s">
         <v>304</v>
@@ -1357,7 +1357,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>22.66012091022734</v>
+        <v>34.55552298750682</v>
       </c>
       <c r="D4" t="s">
         <v>304</v>
@@ -1374,7 +1374,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>40.28852634154036</v>
+        <v>24.739988150454</v>
       </c>
       <c r="D5" t="s">
         <v>304</v>
@@ -1391,7 +1391,7 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>13.66108718675138</v>
+        <v>32.97621928302043</v>
       </c>
       <c r="D6" t="s">
         <v>304</v>
@@ -1408,7 +1408,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>22.11392960100872</v>
+        <v>6.496411979989462</v>
       </c>
       <c r="D7" t="s">
         <v>304</v>
@@ -1425,7 +1425,7 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>41.19928302076933</v>
+        <v>31.38754319129147</v>
       </c>
       <c r="D8" t="s">
         <v>304</v>
@@ -1442,7 +1442,7 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>6.50947837766534</v>
+        <v>24.77197053992895</v>
       </c>
       <c r="D9" t="s">
         <v>304</v>
@@ -1459,7 +1459,7 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>15.9248010367347</v>
+        <v>60.06758961228982</v>
       </c>
       <c r="D10" t="s">
         <v>304</v>
@@ -1476,7 +1476,7 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>21.38000043317331</v>
+        <v>21.33646766384987</v>
       </c>
       <c r="D11" t="s">
         <v>304</v>
@@ -1493,7 +1493,7 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>14.24595529213899</v>
+        <v>18.96437862601704</v>
       </c>
       <c r="D12" t="s">
         <v>304</v>
@@ -1510,7 +1510,7 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>23.48188671774098</v>
+        <v>19.25521693217853</v>
       </c>
       <c r="D13" t="s">
         <v>304</v>
@@ -1527,7 +1527,7 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>28.40242930986945</v>
+        <v>17.66706165354791</v>
       </c>
       <c r="D14" t="s">
         <v>304</v>
@@ -1544,7 +1544,7 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>14.498209317183</v>
+        <v>47.5968675584817</v>
       </c>
       <c r="D15" t="s">
         <v>304</v>
@@ -1561,7 +1561,7 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>23.15144206427138</v>
+        <v>23.77403410638029</v>
       </c>
       <c r="D16" t="s">
         <v>304</v>
@@ -1578,7 +1578,7 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>24.52849296701112</v>
+        <v>11.94875463897461</v>
       </c>
       <c r="D17" t="s">
         <v>304</v>
@@ -1595,7 +1595,7 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>6.657691236516028</v>
+        <v>12.85643668215286</v>
       </c>
       <c r="D18" t="s">
         <v>304</v>
@@ -1612,7 +1612,7 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>35.12244266875043</v>
+        <v>3.434374563660322</v>
       </c>
       <c r="D19" t="s">
         <v>304</v>
@@ -1629,7 +1629,7 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>9.353171053420709</v>
+        <v>14.73081257644077</v>
       </c>
       <c r="D20" t="s">
         <v>304</v>
@@ -1646,7 +1646,7 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>31.25083308679562</v>
+        <v>17.07430361412992</v>
       </c>
       <c r="D21" t="s">
         <v>304</v>
@@ -1663,7 +1663,7 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>16.69958105232745</v>
+        <v>15.95164220458062</v>
       </c>
       <c r="D22" t="s">
         <v>304</v>
@@ -1680,7 +1680,7 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>22.83985160107458</v>
+        <v>32.70851391811062</v>
       </c>
       <c r="D23" t="s">
         <v>304</v>
@@ -1697,7 +1697,7 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>14.57931819663941</v>
+        <v>20.14840612296792</v>
       </c>
       <c r="D24" t="s">
         <v>304</v>
@@ -1714,7 +1714,7 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>15.5810633796226</v>
+        <v>26.65326206564041</v>
       </c>
       <c r="D25" t="s">
         <v>304</v>
@@ -1731,7 +1731,7 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>17.04615293336105</v>
+        <v>9.331167312641018</v>
       </c>
       <c r="D26" t="s">
         <v>304</v>
@@ -1748,7 +1748,7 @@
         <v>29</v>
       </c>
       <c r="C27">
-        <v>29.37501571766105</v>
+        <v>19.68173385882358</v>
       </c>
       <c r="D27" t="s">
         <v>304</v>
@@ -1765,7 +1765,7 @@
         <v>30</v>
       </c>
       <c r="C28">
-        <v>14.69637305612901</v>
+        <v>18.23304133736695</v>
       </c>
       <c r="D28" t="s">
         <v>304</v>
@@ -1782,7 +1782,7 @@
         <v>31</v>
       </c>
       <c r="C29">
-        <v>14.16537782039902</v>
+        <v>19.64827652188851</v>
       </c>
       <c r="D29" t="s">
         <v>304</v>
@@ -1799,7 +1799,7 @@
         <v>32</v>
       </c>
       <c r="C30">
-        <v>56.00898115694567</v>
+        <v>35.14069960129709</v>
       </c>
       <c r="D30" t="s">
         <v>304</v>
@@ -1816,7 +1816,7 @@
         <v>33</v>
       </c>
       <c r="C31">
-        <v>14.66257932497644</v>
+        <v>16.57932558678754</v>
       </c>
       <c r="D31" t="s">
         <v>304</v>
@@ -1833,7 +1833,7 @@
         <v>34</v>
       </c>
       <c r="C32">
-        <v>22.64688657185408</v>
+        <v>31.56030507413216</v>
       </c>
       <c r="D32" t="s">
         <v>304</v>
@@ -1850,7 +1850,7 @@
         <v>35</v>
       </c>
       <c r="C33">
-        <v>14.80510882958378</v>
+        <v>32.65998178940805</v>
       </c>
       <c r="D33" t="s">
         <v>304</v>
@@ -1867,7 +1867,7 @@
         <v>36</v>
       </c>
       <c r="C34">
-        <v>24.75012407598234</v>
+        <v>18.24611634619961</v>
       </c>
       <c r="D34" t="s">
         <v>304</v>
@@ -1884,7 +1884,7 @@
         <v>37</v>
       </c>
       <c r="C35">
-        <v>25.20556222727948</v>
+        <v>17.43375372610785</v>
       </c>
       <c r="D35" t="s">
         <v>304</v>
@@ -1901,7 +1901,7 @@
         <v>38</v>
       </c>
       <c r="C36">
-        <v>16.46217074590631</v>
+        <v>16.18139507470108</v>
       </c>
       <c r="D36" t="s">
         <v>304</v>
@@ -1918,7 +1918,7 @@
         <v>39</v>
       </c>
       <c r="C37">
-        <v>12.37584338344357</v>
+        <v>18.10662573412203</v>
       </c>
       <c r="D37" t="s">
         <v>304</v>
@@ -1935,7 +1935,7 @@
         <v>40</v>
       </c>
       <c r="C38">
-        <v>11.69472095265817</v>
+        <v>18.84046734587332</v>
       </c>
       <c r="D38" t="s">
         <v>304</v>
@@ -1952,7 +1952,7 @@
         <v>41</v>
       </c>
       <c r="C39">
-        <v>14.30221765652393</v>
+        <v>18.15323438996595</v>
       </c>
       <c r="D39" t="s">
         <v>304</v>
@@ -1969,7 +1969,7 @@
         <v>42</v>
       </c>
       <c r="C40">
-        <v>17.38399037422348</v>
+        <v>21.34120464929596</v>
       </c>
       <c r="D40" t="s">
         <v>304</v>
@@ -1986,7 +1986,7 @@
         <v>43</v>
       </c>
       <c r="C41">
-        <v>22.20831032323336</v>
+        <v>23.62675113246726</v>
       </c>
       <c r="D41" t="s">
         <v>304</v>
@@ -2003,7 +2003,7 @@
         <v>44</v>
       </c>
       <c r="C42">
-        <v>41.1803750091964</v>
+        <v>13.65117594167655</v>
       </c>
       <c r="D42" t="s">
         <v>304</v>
@@ -2020,7 +2020,7 @@
         <v>45</v>
       </c>
       <c r="C43">
-        <v>17.71099829863962</v>
+        <v>27.33075293007668</v>
       </c>
       <c r="D43" t="s">
         <v>304</v>
@@ -2037,7 +2037,7 @@
         <v>46</v>
       </c>
       <c r="C44">
-        <v>12.41376044302176</v>
+        <v>18.5524598680059</v>
       </c>
       <c r="D44" t="s">
         <v>304</v>
@@ -2054,7 +2054,7 @@
         <v>47</v>
       </c>
       <c r="C45">
-        <v>7.964387158936823</v>
+        <v>13.72602970707087</v>
       </c>
       <c r="D45" t="s">
         <v>304</v>
@@ -2071,7 +2071,7 @@
         <v>48</v>
       </c>
       <c r="C46">
-        <v>12.15001610013392</v>
+        <v>12.63236312177266</v>
       </c>
       <c r="D46" t="s">
         <v>304</v>
@@ -2088,7 +2088,7 @@
         <v>49</v>
       </c>
       <c r="C47">
-        <v>25.94869309235003</v>
+        <v>24.61213193693454</v>
       </c>
       <c r="D47" t="s">
         <v>304</v>
@@ -2105,7 +2105,7 @@
         <v>50</v>
       </c>
       <c r="C48">
-        <v>28.96001047105388</v>
+        <v>22.19856187849478</v>
       </c>
       <c r="D48" t="s">
         <v>304</v>
@@ -2122,7 +2122,7 @@
         <v>51</v>
       </c>
       <c r="C49">
-        <v>17.04997207629495</v>
+        <v>14.99075397055716</v>
       </c>
       <c r="D49" t="s">
         <v>304</v>
@@ -2139,7 +2139,7 @@
         <v>52</v>
       </c>
       <c r="C50">
-        <v>18.58585601859796</v>
+        <v>18.64265219411157</v>
       </c>
       <c r="D50" t="s">
         <v>304</v>
@@ -2156,7 +2156,7 @@
         <v>53</v>
       </c>
       <c r="C51">
-        <v>24.17623124919326</v>
+        <v>13.53226917612093</v>
       </c>
       <c r="D51" t="s">
         <v>304</v>
@@ -2173,7 +2173,7 @@
         <v>54</v>
       </c>
       <c r="C52">
-        <v>5.98057079720772</v>
+        <v>11.80081657680509</v>
       </c>
       <c r="D52" t="s">
         <v>304</v>
@@ -2190,7 +2190,7 @@
         <v>55</v>
       </c>
       <c r="C53">
-        <v>22.36276037942849</v>
+        <v>16.90915415557402</v>
       </c>
       <c r="D53" t="s">
         <v>304</v>
@@ -2207,7 +2207,7 @@
         <v>56</v>
       </c>
       <c r="C54">
-        <v>18.77683355596584</v>
+        <v>9.127117361204213</v>
       </c>
       <c r="D54" t="s">
         <v>304</v>
@@ -2224,7 +2224,7 @@
         <v>57</v>
       </c>
       <c r="C55">
-        <v>17.68480878171676</v>
+        <v>22.18751478027392</v>
       </c>
       <c r="D55" t="s">
         <v>304</v>
@@ -2241,7 +2241,7 @@
         <v>58</v>
       </c>
       <c r="C56">
-        <v>13.01717685711657</v>
+        <v>8.29714017486388</v>
       </c>
       <c r="D56" t="s">
         <v>304</v>
@@ -2258,7 +2258,7 @@
         <v>59</v>
       </c>
       <c r="C57">
-        <v>17.35292843610177</v>
+        <v>19.96717838436411</v>
       </c>
       <c r="D57" t="s">
         <v>304</v>
@@ -2275,7 +2275,7 @@
         <v>60</v>
       </c>
       <c r="C58">
-        <v>15.30594913708336</v>
+        <v>13.33632395390435</v>
       </c>
       <c r="D58" t="s">
         <v>304</v>
@@ -2292,7 +2292,7 @@
         <v>61</v>
       </c>
       <c r="C59">
-        <v>20.98068317341368</v>
+        <v>13.21304155235663</v>
       </c>
       <c r="D59" t="s">
         <v>304</v>
@@ -2309,7 +2309,7 @@
         <v>62</v>
       </c>
       <c r="C60">
-        <v>31.74555914398153</v>
+        <v>15.36427085243445</v>
       </c>
       <c r="D60" t="s">
         <v>304</v>
@@ -2326,7 +2326,7 @@
         <v>63</v>
       </c>
       <c r="C61">
-        <v>14.45312286444667</v>
+        <v>7.410781428728184</v>
       </c>
       <c r="D61" t="s">
         <v>304</v>
@@ -2343,7 +2343,7 @@
         <v>64</v>
       </c>
       <c r="C62">
-        <v>9.135970361253493</v>
+        <v>4.239985331143055</v>
       </c>
       <c r="D62" t="s">
         <v>304</v>
@@ -2360,7 +2360,7 @@
         <v>65</v>
       </c>
       <c r="C63">
-        <v>21.0353197178887</v>
+        <v>8.239187542291642</v>
       </c>
       <c r="D63" t="s">
         <v>304</v>
@@ -2377,7 +2377,7 @@
         <v>66</v>
       </c>
       <c r="C64">
-        <v>18.04417015440717</v>
+        <v>8.20436767786931</v>
       </c>
       <c r="D64" t="s">
         <v>304</v>
@@ -2394,7 +2394,7 @@
         <v>67</v>
       </c>
       <c r="C65">
-        <v>25.31302457083119</v>
+        <v>11.4202485367123</v>
       </c>
       <c r="D65" t="s">
         <v>304</v>
@@ -2411,7 +2411,7 @@
         <v>68</v>
       </c>
       <c r="C66">
-        <v>29.55174155640773</v>
+        <v>33.4608028897243</v>
       </c>
       <c r="D66" t="s">
         <v>304</v>
@@ -2428,7 +2428,7 @@
         <v>69</v>
       </c>
       <c r="C67">
-        <v>9.477232818260825</v>
+        <v>36.51418885396012</v>
       </c>
       <c r="D67" t="s">
         <v>304</v>
@@ -2445,7 +2445,7 @@
         <v>70</v>
       </c>
       <c r="C68">
-        <v>31.80566132282319</v>
+        <v>21.38773048867002</v>
       </c>
       <c r="D68" t="s">
         <v>304</v>
@@ -2462,7 +2462,7 @@
         <v>71</v>
       </c>
       <c r="C69">
-        <v>13.82875309274939</v>
+        <v>4.647887312754136</v>
       </c>
       <c r="D69" t="s">
         <v>304</v>
@@ -2479,7 +2479,7 @@
         <v>72</v>
       </c>
       <c r="C70">
-        <v>18.25416754676143</v>
+        <v>19.33771392811508</v>
       </c>
       <c r="D70" t="s">
         <v>304</v>
@@ -2496,7 +2496,7 @@
         <v>73</v>
       </c>
       <c r="C71">
-        <v>14.46936679979641</v>
+        <v>25.54363610713394</v>
       </c>
       <c r="D71" t="s">
         <v>304</v>
@@ -2513,7 +2513,7 @@
         <v>74</v>
       </c>
       <c r="C72">
-        <v>12.16577354306041</v>
+        <v>8.103847750683599</v>
       </c>
       <c r="D72" t="s">
         <v>304</v>
@@ -2530,7 +2530,7 @@
         <v>75</v>
       </c>
       <c r="C73">
-        <v>14.34834060118048</v>
+        <v>20.45017254705874</v>
       </c>
       <c r="D73" t="s">
         <v>304</v>
@@ -2547,7 +2547,7 @@
         <v>76</v>
       </c>
       <c r="C74">
-        <v>9.502011780274081</v>
+        <v>25.85760760894291</v>
       </c>
       <c r="D74" t="s">
         <v>304</v>
@@ -2564,7 +2564,7 @@
         <v>77</v>
       </c>
       <c r="C75">
-        <v>24.58016746468858</v>
+        <v>9.077950007798716</v>
       </c>
       <c r="D75" t="s">
         <v>304</v>
@@ -2581,7 +2581,7 @@
         <v>78</v>
       </c>
       <c r="C76">
-        <v>4.861851373940278</v>
+        <v>11.92351711643827</v>
       </c>
       <c r="D76" t="s">
         <v>304</v>
@@ -2598,7 +2598,7 @@
         <v>79</v>
       </c>
       <c r="C77">
-        <v>10.39132031092107</v>
+        <v>14.06069581784003</v>
       </c>
       <c r="D77" t="s">
         <v>304</v>
@@ -2615,7 +2615,7 @@
         <v>80</v>
       </c>
       <c r="C78">
-        <v>22.23831405687178</v>
+        <v>35.02259411750889</v>
       </c>
       <c r="D78" t="s">
         <v>304</v>
@@ -2632,7 +2632,7 @@
         <v>81</v>
       </c>
       <c r="C79">
-        <v>23.13776130713279</v>
+        <v>15.61809530819648</v>
       </c>
       <c r="D79" t="s">
         <v>304</v>
@@ -2649,7 +2649,7 @@
         <v>82</v>
       </c>
       <c r="C80">
-        <v>12.98531840897678</v>
+        <v>15.09928919663276</v>
       </c>
       <c r="D80" t="s">
         <v>304</v>
@@ -2666,7 +2666,7 @@
         <v>83</v>
       </c>
       <c r="C81">
-        <v>26.39806698404998</v>
+        <v>13.13888249145537</v>
       </c>
       <c r="D81" t="s">
         <v>304</v>
@@ -2683,7 +2683,7 @@
         <v>84</v>
       </c>
       <c r="C82">
-        <v>11.06982021580743</v>
+        <v>14.24736526350076</v>
       </c>
       <c r="D82" t="s">
         <v>304</v>
@@ -2700,7 +2700,7 @@
         <v>85</v>
       </c>
       <c r="C83">
-        <v>26.61469936213241</v>
+        <v>10.90535420204366</v>
       </c>
       <c r="D83" t="s">
         <v>304</v>
@@ -2717,7 +2717,7 @@
         <v>86</v>
       </c>
       <c r="C84">
-        <v>28.19698270812523</v>
+        <v>26.86457439323417</v>
       </c>
       <c r="D84" t="s">
         <v>304</v>
@@ -2734,7 +2734,7 @@
         <v>87</v>
       </c>
       <c r="C85">
-        <v>18.76306497759057</v>
+        <v>20.85487533273187</v>
       </c>
       <c r="D85" t="s">
         <v>304</v>
@@ -2751,7 +2751,7 @@
         <v>88</v>
       </c>
       <c r="C86">
-        <v>21.89690674465736</v>
+        <v>28.34617417072643</v>
       </c>
       <c r="D86" t="s">
         <v>304</v>
@@ -2768,7 +2768,7 @@
         <v>89</v>
       </c>
       <c r="C87">
-        <v>14.12473162692577</v>
+        <v>16.61583904560332</v>
       </c>
       <c r="D87" t="s">
         <v>304</v>
@@ -2785,7 +2785,7 @@
         <v>90</v>
       </c>
       <c r="C88">
-        <v>44.40598558097339</v>
+        <v>14.41009707245692</v>
       </c>
       <c r="D88" t="s">
         <v>304</v>
@@ -2802,7 +2802,7 @@
         <v>91</v>
       </c>
       <c r="C89">
-        <v>20.30549175545858</v>
+        <v>31.48259970308897</v>
       </c>
       <c r="D89" t="s">
         <v>304</v>
@@ -2819,7 +2819,7 @@
         <v>92</v>
       </c>
       <c r="C90">
-        <v>32.37215814010735</v>
+        <v>22.30792443225709</v>
       </c>
       <c r="D90" t="s">
         <v>304</v>
@@ -2836,7 +2836,7 @@
         <v>93</v>
       </c>
       <c r="C91">
-        <v>30.12348217734876</v>
+        <v>7.689136601367046</v>
       </c>
       <c r="D91" t="s">
         <v>304</v>
@@ -2853,7 +2853,7 @@
         <v>94</v>
       </c>
       <c r="C92">
-        <v>19.46165298841214</v>
+        <v>14.06604380756544</v>
       </c>
       <c r="D92" t="s">
         <v>304</v>
@@ -2870,7 +2870,7 @@
         <v>95</v>
       </c>
       <c r="C93">
-        <v>23.98082752670372</v>
+        <v>26.51974404735785</v>
       </c>
       <c r="D93" t="s">
         <v>304</v>
@@ -2887,7 +2887,7 @@
         <v>96</v>
       </c>
       <c r="C94">
-        <v>13.80638076153735</v>
+        <v>34.37459447521873</v>
       </c>
       <c r="D94" t="s">
         <v>304</v>
@@ -2904,7 +2904,7 @@
         <v>97</v>
       </c>
       <c r="C95">
-        <v>11.13684865807006</v>
+        <v>10.8354418474537</v>
       </c>
       <c r="D95" t="s">
         <v>304</v>
@@ -2921,7 +2921,7 @@
         <v>98</v>
       </c>
       <c r="C96">
-        <v>6.943618627123872</v>
+        <v>13.39512286232253</v>
       </c>
       <c r="D96" t="s">
         <v>304</v>
@@ -2938,7 +2938,7 @@
         <v>99</v>
       </c>
       <c r="C97">
-        <v>20.47713832222561</v>
+        <v>13.05942214079835</v>
       </c>
       <c r="D97" t="s">
         <v>304</v>
@@ -2955,7 +2955,7 @@
         <v>100</v>
       </c>
       <c r="C98">
-        <v>19.23352274849253</v>
+        <v>15.67563005441571</v>
       </c>
       <c r="D98" t="s">
         <v>304</v>
@@ -2972,7 +2972,7 @@
         <v>101</v>
       </c>
       <c r="C99">
-        <v>23.58907686461502</v>
+        <v>18.92490202035714</v>
       </c>
       <c r="D99" t="s">
         <v>304</v>
@@ -2989,7 +2989,7 @@
         <v>102</v>
       </c>
       <c r="C100">
-        <v>11.03141678689421</v>
+        <v>11.40161924319125</v>
       </c>
       <c r="D100" t="s">
         <v>304</v>
@@ -3006,7 +3006,7 @@
         <v>103</v>
       </c>
       <c r="C101">
-        <v>18.78191509828078</v>
+        <v>26.32033053941438</v>
       </c>
       <c r="D101" t="s">
         <v>304</v>
@@ -3023,7 +3023,7 @@
         <v>104</v>
       </c>
       <c r="C102">
-        <v>43.00888690632764</v>
+        <v>41.09249050961649</v>
       </c>
       <c r="D102" t="s">
         <v>304</v>
@@ -3040,7 +3040,7 @@
         <v>105</v>
       </c>
       <c r="C103">
-        <v>16.42867794781776</v>
+        <v>17.44870753651668</v>
       </c>
       <c r="D103" t="s">
         <v>304</v>
@@ -3057,7 +3057,7 @@
         <v>106</v>
       </c>
       <c r="C104">
-        <v>36.21306939221109</v>
+        <v>32.23249251283274</v>
       </c>
       <c r="D104" t="s">
         <v>304</v>
@@ -3074,7 +3074,7 @@
         <v>107</v>
       </c>
       <c r="C105">
-        <v>21.29818179888811</v>
+        <v>18.26236329372335</v>
       </c>
       <c r="D105" t="s">
         <v>304</v>
@@ -3091,7 +3091,7 @@
         <v>108</v>
       </c>
       <c r="C106">
-        <v>19.79444087900691</v>
+        <v>27.77813618162413</v>
       </c>
       <c r="D106" t="s">
         <v>304</v>
@@ -3108,7 +3108,7 @@
         <v>109</v>
       </c>
       <c r="C107">
-        <v>45.71940421853503</v>
+        <v>16.69870998654716</v>
       </c>
       <c r="D107" t="s">
         <v>304</v>
@@ -3125,7 +3125,7 @@
         <v>110</v>
       </c>
       <c r="C108">
-        <v>20.53354149220211</v>
+        <v>12.97938730039484</v>
       </c>
       <c r="D108" t="s">
         <v>304</v>
@@ -3142,7 +3142,7 @@
         <v>111</v>
       </c>
       <c r="C109">
-        <v>16.59767069460728</v>
+        <v>22.57441012552878</v>
       </c>
       <c r="D109" t="s">
         <v>304</v>
@@ -3159,7 +3159,7 @@
         <v>112</v>
       </c>
       <c r="C110">
-        <v>6.895498939048585</v>
+        <v>25.52631329462972</v>
       </c>
       <c r="D110" t="s">
         <v>304</v>
@@ -3176,7 +3176,7 @@
         <v>113</v>
       </c>
       <c r="C111">
-        <v>12.49640237850093</v>
+        <v>7.79054965253431</v>
       </c>
       <c r="D111" t="s">
         <v>304</v>
@@ -3193,7 +3193,7 @@
         <v>114</v>
       </c>
       <c r="C112">
-        <v>15.49603815115292</v>
+        <v>11.74718062576074</v>
       </c>
       <c r="D112" t="s">
         <v>304</v>
@@ -3210,7 +3210,7 @@
         <v>115</v>
       </c>
       <c r="C113">
-        <v>21.57593547202928</v>
+        <v>18.70741796279677</v>
       </c>
       <c r="D113" t="s">
         <v>304</v>
@@ -3227,7 +3227,7 @@
         <v>116</v>
       </c>
       <c r="C114">
-        <v>7.713106268862177</v>
+        <v>14.83524015584971</v>
       </c>
       <c r="D114" t="s">
         <v>304</v>
@@ -3244,7 +3244,7 @@
         <v>117</v>
       </c>
       <c r="C115">
-        <v>13.90402261022821</v>
+        <v>11.34049758400011</v>
       </c>
       <c r="D115" t="s">
         <v>304</v>
@@ -3261,7 +3261,7 @@
         <v>118</v>
       </c>
       <c r="C116">
-        <v>23.73173652425413</v>
+        <v>19.19151089051474</v>
       </c>
       <c r="D116" t="s">
         <v>304</v>
@@ -3278,7 +3278,7 @@
         <v>119</v>
       </c>
       <c r="C117">
-        <v>29.89607977289688</v>
+        <v>22.66564392929899</v>
       </c>
       <c r="D117" t="s">
         <v>304</v>
@@ -3295,7 +3295,7 @@
         <v>120</v>
       </c>
       <c r="C118">
-        <v>19.82380611444545</v>
+        <v>8.753518568631909</v>
       </c>
       <c r="D118" t="s">
         <v>304</v>
@@ -3312,7 +3312,7 @@
         <v>121</v>
       </c>
       <c r="C119">
-        <v>10.54288852930751</v>
+        <v>13.73853977068961</v>
       </c>
       <c r="D119" t="s">
         <v>304</v>
@@ -3329,7 +3329,7 @@
         <v>122</v>
       </c>
       <c r="C120">
-        <v>25.49152872616158</v>
+        <v>31.85409924323869</v>
       </c>
       <c r="D120" t="s">
         <v>304</v>
@@ -3346,7 +3346,7 @@
         <v>123</v>
       </c>
       <c r="C121">
-        <v>25.66737939942529</v>
+        <v>47.10783004801149</v>
       </c>
       <c r="D121" t="s">
         <v>304</v>
@@ -3363,7 +3363,7 @@
         <v>124</v>
       </c>
       <c r="C122">
-        <v>17.20037750145424</v>
+        <v>17.63818923697551</v>
       </c>
       <c r="D122" t="s">
         <v>304</v>
@@ -3380,7 +3380,7 @@
         <v>125</v>
       </c>
       <c r="C123">
-        <v>14.54045715389801</v>
+        <v>20.90293108732524</v>
       </c>
       <c r="D123" t="s">
         <v>304</v>
@@ -3397,7 +3397,7 @@
         <v>126</v>
       </c>
       <c r="C124">
-        <v>25.18982002647243</v>
+        <v>18.27031902981777</v>
       </c>
       <c r="D124" t="s">
         <v>304</v>
@@ -3414,7 +3414,7 @@
         <v>127</v>
       </c>
       <c r="C125">
-        <v>12.80929019789212</v>
+        <v>25.76330783070583</v>
       </c>
       <c r="D125" t="s">
         <v>304</v>
@@ -3431,7 +3431,7 @@
         <v>128</v>
       </c>
       <c r="C126">
-        <v>12.15191778956942</v>
+        <v>24.00915132188906</v>
       </c>
       <c r="D126" t="s">
         <v>304</v>
@@ -3448,7 +3448,7 @@
         <v>129</v>
       </c>
       <c r="C127">
-        <v>21.10816740573726</v>
+        <v>21.88732781817072</v>
       </c>
       <c r="D127" t="s">
         <v>304</v>
@@ -3465,7 +3465,7 @@
         <v>130</v>
       </c>
       <c r="C128">
-        <v>26.49280022694809</v>
+        <v>20.46027284626058</v>
       </c>
       <c r="D128" t="s">
         <v>304</v>
@@ -3482,7 +3482,7 @@
         <v>131</v>
       </c>
       <c r="C129">
-        <v>15.82019416736566</v>
+        <v>15.02865787237961</v>
       </c>
       <c r="D129" t="s">
         <v>304</v>
@@ -3499,7 +3499,7 @@
         <v>132</v>
       </c>
       <c r="C130">
-        <v>16.08064675285509</v>
+        <v>30.9799674153045</v>
       </c>
       <c r="D130" t="s">
         <v>304</v>
@@ -3516,7 +3516,7 @@
         <v>133</v>
       </c>
       <c r="C131">
-        <v>19.24098171110747</v>
+        <v>20.07322097145438</v>
       </c>
       <c r="D131" t="s">
         <v>304</v>
@@ -3533,7 +3533,7 @@
         <v>134</v>
       </c>
       <c r="C132">
-        <v>19.7757079474375</v>
+        <v>13.30325502209162</v>
       </c>
       <c r="D132" t="s">
         <v>304</v>
@@ -3550,7 +3550,7 @@
         <v>135</v>
       </c>
       <c r="C133">
-        <v>20.30802324576531</v>
+        <v>13.48253250895793</v>
       </c>
       <c r="D133" t="s">
         <v>304</v>
@@ -3567,7 +3567,7 @@
         <v>136</v>
       </c>
       <c r="C134">
-        <v>17.02533000876285</v>
+        <v>13.5434581018192</v>
       </c>
       <c r="D134" t="s">
         <v>304</v>
@@ -3584,7 +3584,7 @@
         <v>137</v>
       </c>
       <c r="C135">
-        <v>19.54497946888951</v>
+        <v>22.17390093814451</v>
       </c>
       <c r="D135" t="s">
         <v>304</v>
@@ -3601,7 +3601,7 @@
         <v>138</v>
       </c>
       <c r="C136">
-        <v>20.55924345181377</v>
+        <v>23.57163466698348</v>
       </c>
       <c r="D136" t="s">
         <v>304</v>
@@ -3618,7 +3618,7 @@
         <v>139</v>
       </c>
       <c r="C137">
-        <v>5.991508347886981</v>
+        <v>15.41892887704962</v>
       </c>
       <c r="D137" t="s">
         <v>304</v>
@@ -3635,7 +3635,7 @@
         <v>140</v>
       </c>
       <c r="C138">
-        <v>26.91854893005443</v>
+        <v>11.14027799894071</v>
       </c>
       <c r="D138" t="s">
         <v>304</v>
@@ -3652,7 +3652,7 @@
         <v>141</v>
       </c>
       <c r="C139">
-        <v>19.44867063140447</v>
+        <v>12.63011971447525</v>
       </c>
       <c r="D139" t="s">
         <v>304</v>
@@ -3669,7 +3669,7 @@
         <v>142</v>
       </c>
       <c r="C140">
-        <v>25.40730942560812</v>
+        <v>17.37699916393521</v>
       </c>
       <c r="D140" t="s">
         <v>304</v>
@@ -3686,7 +3686,7 @@
         <v>143</v>
       </c>
       <c r="C141">
-        <v>13.84984223401127</v>
+        <v>29.19086456487894</v>
       </c>
       <c r="D141" t="s">
         <v>304</v>
@@ -3703,7 +3703,7 @@
         <v>144</v>
       </c>
       <c r="C142">
-        <v>21.53938473722307</v>
+        <v>22.25816131402396</v>
       </c>
       <c r="D142" t="s">
         <v>304</v>
@@ -3720,7 +3720,7 @@
         <v>145</v>
       </c>
       <c r="C143">
-        <v>13.96108654565839</v>
+        <v>23.04632462573222</v>
       </c>
       <c r="D143" t="s">
         <v>304</v>
@@ -3737,7 +3737,7 @@
         <v>146</v>
       </c>
       <c r="C144">
-        <v>10.09317483256969</v>
+        <v>16.56117991870034</v>
       </c>
       <c r="D144" t="s">
         <v>304</v>
@@ -3754,7 +3754,7 @@
         <v>147</v>
       </c>
       <c r="C145">
-        <v>20.3835134497252</v>
+        <v>16.83964968498543</v>
       </c>
       <c r="D145" t="s">
         <v>304</v>
@@ -3771,7 +3771,7 @@
         <v>148</v>
       </c>
       <c r="C146">
-        <v>33.43683908539101</v>
+        <v>26.51625815186107</v>
       </c>
       <c r="D146" t="s">
         <v>304</v>
@@ -3788,7 +3788,7 @@
         <v>149</v>
       </c>
       <c r="C147">
-        <v>14.58015736544747</v>
+        <v>16.73327889731875</v>
       </c>
       <c r="D147" t="s">
         <v>304</v>
@@ -3805,7 +3805,7 @@
         <v>150</v>
       </c>
       <c r="C148">
-        <v>17.61064379075329</v>
+        <v>11.65953690428239</v>
       </c>
       <c r="D148" t="s">
         <v>304</v>
@@ -3822,7 +3822,7 @@
         <v>151</v>
       </c>
       <c r="C149">
-        <v>23.40889943155172</v>
+        <v>16.9311112801306</v>
       </c>
       <c r="D149" t="s">
         <v>304</v>
@@ -3839,7 +3839,7 @@
         <v>152</v>
       </c>
       <c r="C150">
-        <v>18.43348311364208</v>
+        <v>42.89920632078297</v>
       </c>
       <c r="D150" t="s">
         <v>304</v>
@@ -3856,7 +3856,7 @@
         <v>153</v>
       </c>
       <c r="C151">
-        <v>24.9103565626932</v>
+        <v>16.07490312435362</v>
       </c>
       <c r="D151" t="s">
         <v>304</v>
@@ -3873,7 +3873,7 @@
         <v>154</v>
       </c>
       <c r="C152">
-        <v>18.47658297356843</v>
+        <v>4.409174519297968</v>
       </c>
       <c r="D152" t="s">
         <v>304</v>
@@ -3890,7 +3890,7 @@
         <v>155</v>
       </c>
       <c r="C153">
-        <v>27.37854093838557</v>
+        <v>23.02084743842647</v>
       </c>
       <c r="D153" t="s">
         <v>304</v>
@@ -3907,7 +3907,7 @@
         <v>156</v>
       </c>
       <c r="C154">
-        <v>11.11841578027889</v>
+        <v>30.69612835246139</v>
       </c>
       <c r="D154" t="s">
         <v>304</v>
@@ -3924,7 +3924,7 @@
         <v>157</v>
       </c>
       <c r="C155">
-        <v>10.17690188338502</v>
+        <v>4.125849714646355</v>
       </c>
       <c r="D155" t="s">
         <v>304</v>
@@ -3941,7 +3941,7 @@
         <v>158</v>
       </c>
       <c r="C156">
-        <v>34.50289644120647</v>
+        <v>6.44597012281208</v>
       </c>
       <c r="D156" t="s">
         <v>304</v>
@@ -3958,7 +3958,7 @@
         <v>159</v>
       </c>
       <c r="C157">
-        <v>12.88743822717818</v>
+        <v>15.02848441591698</v>
       </c>
       <c r="D157" t="s">
         <v>304</v>
@@ -3975,7 +3975,7 @@
         <v>160</v>
       </c>
       <c r="C158">
-        <v>50.47903002722639</v>
+        <v>37.92786443064846</v>
       </c>
       <c r="D158" t="s">
         <v>304</v>
@@ -3992,7 +3992,7 @@
         <v>161</v>
       </c>
       <c r="C159">
-        <v>21.50358939019026</v>
+        <v>10.48007769240035</v>
       </c>
       <c r="D159" t="s">
         <v>304</v>
@@ -4009,7 +4009,7 @@
         <v>162</v>
       </c>
       <c r="C160">
-        <v>14.30833134701411</v>
+        <v>25.93693540710023</v>
       </c>
       <c r="D160" t="s">
         <v>304</v>
@@ -4026,7 +4026,7 @@
         <v>163</v>
       </c>
       <c r="C161">
-        <v>25.62471580224191</v>
+        <v>10.12878393683921</v>
       </c>
       <c r="D161" t="s">
         <v>304</v>
@@ -4043,7 +4043,7 @@
         <v>164</v>
       </c>
       <c r="C162">
-        <v>7.218407674940156</v>
+        <v>17.57812973153305</v>
       </c>
       <c r="D162" t="s">
         <v>304</v>
@@ -4060,7 +4060,7 @@
         <v>165</v>
       </c>
       <c r="C163">
-        <v>12.50268676418636</v>
+        <v>24.8027238763057</v>
       </c>
       <c r="D163" t="s">
         <v>304</v>
@@ -4077,7 +4077,7 @@
         <v>166</v>
       </c>
       <c r="C164">
-        <v>12.0574060922718</v>
+        <v>13.02043260610886</v>
       </c>
       <c r="D164" t="s">
         <v>304</v>
@@ -4094,7 +4094,7 @@
         <v>167</v>
       </c>
       <c r="C165">
-        <v>10.83848808435261</v>
+        <v>16.03676124536545</v>
       </c>
       <c r="D165" t="s">
         <v>304</v>
@@ -4111,7 +4111,7 @@
         <v>168</v>
       </c>
       <c r="C166">
-        <v>7.710564983702247</v>
+        <v>52.16710246428404</v>
       </c>
       <c r="D166" t="s">
         <v>304</v>
@@ -4128,7 +4128,7 @@
         <v>169</v>
       </c>
       <c r="C167">
-        <v>13.3912034552187</v>
+        <v>35.8986556877455</v>
       </c>
       <c r="D167" t="s">
         <v>304</v>
@@ -4145,7 +4145,7 @@
         <v>170</v>
       </c>
       <c r="C168">
-        <v>13.42886540335135</v>
+        <v>10.99499045075332</v>
       </c>
       <c r="D168" t="s">
         <v>304</v>
@@ -4162,7 +4162,7 @@
         <v>171</v>
       </c>
       <c r="C169">
-        <v>8.752417867545834</v>
+        <v>15.98955165283589</v>
       </c>
       <c r="D169" t="s">
         <v>304</v>
@@ -4179,7 +4179,7 @@
         <v>172</v>
       </c>
       <c r="C170">
-        <v>19.64667432744364</v>
+        <v>38.96333977904285</v>
       </c>
       <c r="D170" t="s">
         <v>304</v>
@@ -4196,7 +4196,7 @@
         <v>173</v>
       </c>
       <c r="C171">
-        <v>35.30235016652912</v>
+        <v>7.869848893721446</v>
       </c>
       <c r="D171" t="s">
         <v>304</v>
@@ -4213,7 +4213,7 @@
         <v>174</v>
       </c>
       <c r="C172">
-        <v>23.91361444580361</v>
+        <v>14.77831619448622</v>
       </c>
       <c r="D172" t="s">
         <v>304</v>
@@ -4230,7 +4230,7 @@
         <v>175</v>
       </c>
       <c r="C173">
-        <v>11.60591230126786</v>
+        <v>39.5466962542031</v>
       </c>
       <c r="D173" t="s">
         <v>304</v>
@@ -4247,7 +4247,7 @@
         <v>176</v>
       </c>
       <c r="C174">
-        <v>24.92966578618297</v>
+        <v>33.84817797053214</v>
       </c>
       <c r="D174" t="s">
         <v>304</v>
@@ -4264,7 +4264,7 @@
         <v>177</v>
       </c>
       <c r="C175">
-        <v>14.13669684770335</v>
+        <v>4.207551773982196</v>
       </c>
       <c r="D175" t="s">
         <v>304</v>
@@ -4281,7 +4281,7 @@
         <v>178</v>
       </c>
       <c r="C176">
-        <v>39.28071979545608</v>
+        <v>15.36190422267531</v>
       </c>
       <c r="D176" t="s">
         <v>304</v>
@@ -4298,7 +4298,7 @@
         <v>179</v>
       </c>
       <c r="C177">
-        <v>22.79674098513671</v>
+        <v>20.19771689130088</v>
       </c>
       <c r="D177" t="s">
         <v>304</v>
@@ -4315,7 +4315,7 @@
         <v>180</v>
       </c>
       <c r="C178">
-        <v>21.34930230108095</v>
+        <v>10.39419631168204</v>
       </c>
       <c r="D178" t="s">
         <v>304</v>
@@ -4332,7 +4332,7 @@
         <v>181</v>
       </c>
       <c r="C179">
-        <v>9.393763830520108</v>
+        <v>2.197159903859816</v>
       </c>
       <c r="D179" t="s">
         <v>304</v>
@@ -4349,7 +4349,7 @@
         <v>182</v>
       </c>
       <c r="C180">
-        <v>12.40064523264786</v>
+        <v>40.93773462917851</v>
       </c>
       <c r="D180" t="s">
         <v>304</v>
@@ -4366,7 +4366,7 @@
         <v>183</v>
       </c>
       <c r="C181">
-        <v>34.43914395518713</v>
+        <v>20.11015605468455</v>
       </c>
       <c r="D181" t="s">
         <v>304</v>
@@ -4383,7 +4383,7 @@
         <v>184</v>
       </c>
       <c r="C182">
-        <v>28.55222334271714</v>
+        <v>23.90864532168841</v>
       </c>
       <c r="D182" t="s">
         <v>304</v>
@@ -4400,7 +4400,7 @@
         <v>185</v>
       </c>
       <c r="C183">
-        <v>9.487349227490093</v>
+        <v>5.035360080189914</v>
       </c>
       <c r="D183" t="s">
         <v>304</v>
@@ -4417,7 +4417,7 @@
         <v>186</v>
       </c>
       <c r="C184">
-        <v>28.97542943556119</v>
+        <v>7.233533384046698</v>
       </c>
       <c r="D184" t="s">
         <v>304</v>
@@ -4434,7 +4434,7 @@
         <v>187</v>
       </c>
       <c r="C185">
-        <v>5.549897697705587</v>
+        <v>18.34409106970684</v>
       </c>
       <c r="D185" t="s">
         <v>304</v>
@@ -4451,7 +4451,7 @@
         <v>188</v>
       </c>
       <c r="C186">
-        <v>20.69048740779721</v>
+        <v>6.356567628221416</v>
       </c>
       <c r="D186" t="s">
         <v>304</v>
@@ -4468,7 +4468,7 @@
         <v>189</v>
       </c>
       <c r="C187">
-        <v>9.587546635269655</v>
+        <v>20.01378904915827</v>
       </c>
       <c r="D187" t="s">
         <v>304</v>
@@ -4485,7 +4485,7 @@
         <v>190</v>
       </c>
       <c r="C188">
-        <v>13.36547670788499</v>
+        <v>15.07921760931475</v>
       </c>
       <c r="D188" t="s">
         <v>304</v>
@@ -4502,7 +4502,7 @@
         <v>191</v>
       </c>
       <c r="C189">
-        <v>1.151972453741667</v>
+        <v>24.69758607249367</v>
       </c>
       <c r="D189" t="s">
         <v>304</v>
@@ -4519,7 +4519,7 @@
         <v>192</v>
       </c>
       <c r="C190">
-        <v>21.01989873211844</v>
+        <v>21.70705471900088</v>
       </c>
       <c r="D190" t="s">
         <v>304</v>
@@ -4536,7 +4536,7 @@
         <v>193</v>
       </c>
       <c r="C191">
-        <v>16.24003570942304</v>
+        <v>25.15178806677081</v>
       </c>
       <c r="D191" t="s">
         <v>304</v>
@@ -4553,7 +4553,7 @@
         <v>194</v>
       </c>
       <c r="C192">
-        <v>24.20143066981732</v>
+        <v>26.02838369748025</v>
       </c>
       <c r="D192" t="s">
         <v>304</v>
@@ -4570,7 +4570,7 @@
         <v>195</v>
       </c>
       <c r="C193">
-        <v>11.05860373666033</v>
+        <v>12.79982898672307</v>
       </c>
       <c r="D193" t="s">
         <v>304</v>
@@ -4587,7 +4587,7 @@
         <v>196</v>
       </c>
       <c r="C194">
-        <v>13.99337034670308</v>
+        <v>34.26329521641325</v>
       </c>
       <c r="D194" t="s">
         <v>304</v>
@@ -4604,7 +4604,7 @@
         <v>197</v>
       </c>
       <c r="C195">
-        <v>25.13029399704765</v>
+        <v>21.79367882377742</v>
       </c>
       <c r="D195" t="s">
         <v>304</v>
@@ -4621,7 +4621,7 @@
         <v>198</v>
       </c>
       <c r="C196">
-        <v>10.46628387775054</v>
+        <v>19.75605458491338</v>
       </c>
       <c r="D196" t="s">
         <v>304</v>
@@ -4638,7 +4638,7 @@
         <v>199</v>
       </c>
       <c r="C197">
-        <v>48.37964824542456</v>
+        <v>28.16953377050394</v>
       </c>
       <c r="D197" t="s">
         <v>304</v>
@@ -4655,7 +4655,7 @@
         <v>200</v>
       </c>
       <c r="C198">
-        <v>25.92271472860552</v>
+        <v>29.11913691905563</v>
       </c>
       <c r="D198" t="s">
         <v>304</v>
@@ -4672,7 +4672,7 @@
         <v>201</v>
       </c>
       <c r="C199">
-        <v>8.381418009330975</v>
+        <v>25.63220675724234</v>
       </c>
       <c r="D199" t="s">
         <v>304</v>
@@ -4689,7 +4689,7 @@
         <v>202</v>
       </c>
       <c r="C200">
-        <v>18.29399035119608</v>
+        <v>42.5581030899596</v>
       </c>
       <c r="D200" t="s">
         <v>304</v>
@@ -4706,7 +4706,7 @@
         <v>203</v>
       </c>
       <c r="C201">
-        <v>17.97793534154999</v>
+        <v>24.67220564869962</v>
       </c>
       <c r="D201" t="s">
         <v>304</v>
@@ -4723,7 +4723,7 @@
         <v>204</v>
       </c>
       <c r="C202">
-        <v>17.38987010033638</v>
+        <v>12.18091718799135</v>
       </c>
       <c r="D202" t="s">
         <v>304</v>
@@ -4740,7 +4740,7 @@
         <v>205</v>
       </c>
       <c r="C203">
-        <v>7.03526546272832</v>
+        <v>8.503899745701293</v>
       </c>
       <c r="D203" t="s">
         <v>304</v>
@@ -4757,7 +4757,7 @@
         <v>206</v>
       </c>
       <c r="C204">
-        <v>8.895748791736217</v>
+        <v>14.01835911620865</v>
       </c>
       <c r="D204" t="s">
         <v>304</v>
@@ -4774,7 +4774,7 @@
         <v>207</v>
       </c>
       <c r="C205">
-        <v>16.13808482285744</v>
+        <v>21.70106548990248</v>
       </c>
       <c r="D205" t="s">
         <v>304</v>
@@ -4791,7 +4791,7 @@
         <v>208</v>
       </c>
       <c r="C206">
-        <v>13.01832757103332</v>
+        <v>22.35880699602157</v>
       </c>
       <c r="D206" t="s">
         <v>304</v>
@@ -4808,7 +4808,7 @@
         <v>209</v>
       </c>
       <c r="C207">
-        <v>29.1183387063268</v>
+        <v>28.86337003296296</v>
       </c>
       <c r="D207" t="s">
         <v>304</v>
@@ -4825,7 +4825,7 @@
         <v>210</v>
       </c>
       <c r="C208">
-        <v>26.20916446936479</v>
+        <v>3.002021573143667</v>
       </c>
       <c r="D208" t="s">
         <v>304</v>
@@ -4842,7 +4842,7 @@
         <v>211</v>
       </c>
       <c r="C209">
-        <v>24.71961145748327</v>
+        <v>31.60444692253406</v>
       </c>
       <c r="D209" t="s">
         <v>304</v>
@@ -4859,7 +4859,7 @@
         <v>212</v>
       </c>
       <c r="C210">
-        <v>25.81306951573862</v>
+        <v>2.508994498238465</v>
       </c>
       <c r="D210" t="s">
         <v>304</v>
@@ -4876,7 +4876,7 @@
         <v>213</v>
       </c>
       <c r="C211">
-        <v>15.79651676301702</v>
+        <v>19.21655229360337</v>
       </c>
       <c r="D211" t="s">
         <v>304</v>
@@ -4893,7 +4893,7 @@
         <v>214</v>
       </c>
       <c r="C212">
-        <v>19.74838858058533</v>
+        <v>12.57964442843007</v>
       </c>
       <c r="D212" t="s">
         <v>304</v>
@@ -4910,7 +4910,7 @@
         <v>215</v>
       </c>
       <c r="C213">
-        <v>16.34519385398301</v>
+        <v>11.8415492482902</v>
       </c>
       <c r="D213" t="s">
         <v>304</v>
@@ -4927,7 +4927,7 @@
         <v>216</v>
       </c>
       <c r="C214">
-        <v>11.52598443755978</v>
+        <v>7.902312220045953</v>
       </c>
       <c r="D214" t="s">
         <v>304</v>
@@ -4944,7 +4944,7 @@
         <v>217</v>
       </c>
       <c r="C215">
-        <v>35.65296060038924</v>
+        <v>37.91004079738104</v>
       </c>
       <c r="D215" t="s">
         <v>304</v>
@@ -4961,7 +4961,7 @@
         <v>218</v>
       </c>
       <c r="C216">
-        <v>23.66537626304764</v>
+        <v>25.52187038061397</v>
       </c>
       <c r="D216" t="s">
         <v>304</v>
@@ -4978,7 +4978,7 @@
         <v>219</v>
       </c>
       <c r="C217">
-        <v>27.64348084769037</v>
+        <v>22.32835121409863</v>
       </c>
       <c r="D217" t="s">
         <v>304</v>
@@ -4995,7 +4995,7 @@
         <v>220</v>
       </c>
       <c r="C218">
-        <v>14.78292322024913</v>
+        <v>25.85470697996536</v>
       </c>
       <c r="D218" t="s">
         <v>304</v>
@@ -5012,7 +5012,7 @@
         <v>221</v>
       </c>
       <c r="C219">
-        <v>8.447255340173243</v>
+        <v>29.70410910077008</v>
       </c>
       <c r="D219" t="s">
         <v>304</v>
@@ -5029,7 +5029,7 @@
         <v>222</v>
       </c>
       <c r="C220">
-        <v>14.78953505051049</v>
+        <v>52.315280082712</v>
       </c>
       <c r="D220" t="s">
         <v>304</v>
@@ -5046,7 +5046,7 @@
         <v>223</v>
       </c>
       <c r="C221">
-        <v>25.39606626456911</v>
+        <v>38.7735873596347</v>
       </c>
       <c r="D221" t="s">
         <v>304</v>
@@ -5063,7 +5063,7 @@
         <v>224</v>
       </c>
       <c r="C222">
-        <v>22.80346849027539</v>
+        <v>20.61664826780125</v>
       </c>
       <c r="D222" t="s">
         <v>304</v>
@@ -5080,7 +5080,7 @@
         <v>225</v>
       </c>
       <c r="C223">
-        <v>10.82915970615852</v>
+        <v>18.02143258236625</v>
       </c>
       <c r="D223" t="s">
         <v>304</v>
@@ -5097,7 +5097,7 @@
         <v>226</v>
       </c>
       <c r="C224">
-        <v>15.25185937301084</v>
+        <v>24.53190200473468</v>
       </c>
       <c r="D224" t="s">
         <v>304</v>
@@ -5114,7 +5114,7 @@
         <v>227</v>
       </c>
       <c r="C225">
-        <v>11.49668501604879</v>
+        <v>21.06152177064334</v>
       </c>
       <c r="D225" t="s">
         <v>304</v>
@@ -5131,7 +5131,7 @@
         <v>228</v>
       </c>
       <c r="C226">
-        <v>28.94413575698172</v>
+        <v>16.03664149535741</v>
       </c>
       <c r="D226" t="s">
         <v>304</v>
@@ -5148,7 +5148,7 @@
         <v>229</v>
       </c>
       <c r="C227">
-        <v>24.05628417932479</v>
+        <v>31.89355182583478</v>
       </c>
       <c r="D227" t="s">
         <v>304</v>
@@ -5165,7 +5165,7 @@
         <v>230</v>
       </c>
       <c r="C228">
-        <v>10.97039888106531</v>
+        <v>6.954086274233273</v>
       </c>
       <c r="D228" t="s">
         <v>304</v>
@@ -5182,7 +5182,7 @@
         <v>231</v>
       </c>
       <c r="C229">
-        <v>7.442334589075625</v>
+        <v>36.866364869971</v>
       </c>
       <c r="D229" t="s">
         <v>304</v>
@@ -5199,7 +5199,7 @@
         <v>232</v>
       </c>
       <c r="C230">
-        <v>27.88261424923096</v>
+        <v>30.83252090957575</v>
       </c>
       <c r="D230" t="s">
         <v>304</v>
@@ -5216,7 +5216,7 @@
         <v>233</v>
       </c>
       <c r="C231">
-        <v>21.90303180580532</v>
+        <v>13.33878639462529</v>
       </c>
       <c r="D231" t="s">
         <v>304</v>
@@ -5233,7 +5233,7 @@
         <v>234</v>
       </c>
       <c r="C232">
-        <v>24.16965617573804</v>
+        <v>21.65208871353282</v>
       </c>
       <c r="D232" t="s">
         <v>304</v>
@@ -5250,7 +5250,7 @@
         <v>235</v>
       </c>
       <c r="C233">
-        <v>20.88276767706704</v>
+        <v>8.981679677050757</v>
       </c>
       <c r="D233" t="s">
         <v>304</v>
@@ -5267,7 +5267,7 @@
         <v>236</v>
       </c>
       <c r="C234">
-        <v>19.27645884990326</v>
+        <v>18.78870110309154</v>
       </c>
       <c r="D234" t="s">
         <v>304</v>
@@ -5284,7 +5284,7 @@
         <v>237</v>
       </c>
       <c r="C235">
-        <v>27.23103539396413</v>
+        <v>7.632444726181006</v>
       </c>
       <c r="D235" t="s">
         <v>304</v>
@@ -5301,7 +5301,7 @@
         <v>238</v>
       </c>
       <c r="C236">
-        <v>9.657443281000623</v>
+        <v>14.78687923276423</v>
       </c>
       <c r="D236" t="s">
         <v>304</v>
@@ -5318,7 +5318,7 @@
         <v>239</v>
       </c>
       <c r="C237">
-        <v>14.31790940412712</v>
+        <v>15.14014046931553</v>
       </c>
       <c r="D237" t="s">
         <v>304</v>
@@ -5335,7 +5335,7 @@
         <v>240</v>
       </c>
       <c r="C238">
-        <v>26.19662001925222</v>
+        <v>16.17632198311708</v>
       </c>
       <c r="D238" t="s">
         <v>304</v>
@@ -5352,7 +5352,7 @@
         <v>241</v>
       </c>
       <c r="C239">
-        <v>11.91653592318756</v>
+        <v>12.94770411014334</v>
       </c>
       <c r="D239" t="s">
         <v>304</v>
@@ -5369,7 +5369,7 @@
         <v>242</v>
       </c>
       <c r="C240">
-        <v>16.00816794536173</v>
+        <v>9.423457990284295</v>
       </c>
       <c r="D240" t="s">
         <v>304</v>
@@ -5386,7 +5386,7 @@
         <v>243</v>
       </c>
       <c r="C241">
-        <v>21.71712283444378</v>
+        <v>11.80969792241822</v>
       </c>
       <c r="D241" t="s">
         <v>304</v>
@@ -5403,7 +5403,7 @@
         <v>244</v>
       </c>
       <c r="C242">
-        <v>33.48296647049629</v>
+        <v>10.68668132417446</v>
       </c>
       <c r="D242" t="s">
         <v>304</v>
@@ -5420,7 +5420,7 @@
         <v>245</v>
       </c>
       <c r="C243">
-        <v>14.47418766067348</v>
+        <v>22.75105942786183</v>
       </c>
       <c r="D243" t="s">
         <v>304</v>
@@ -5437,7 +5437,7 @@
         <v>246</v>
       </c>
       <c r="C244">
-        <v>14.94042735238769</v>
+        <v>11.63077592352439</v>
       </c>
       <c r="D244" t="s">
         <v>304</v>
@@ -5454,7 +5454,7 @@
         <v>247</v>
       </c>
       <c r="C245">
-        <v>23.91232526410484</v>
+        <v>30.67660710115654</v>
       </c>
       <c r="D245" t="s">
         <v>304</v>
@@ -5471,7 +5471,7 @@
         <v>248</v>
       </c>
       <c r="C246">
-        <v>29.29615156111837</v>
+        <v>8.631892966436244</v>
       </c>
       <c r="D246" t="s">
         <v>304</v>
@@ -5488,7 +5488,7 @@
         <v>249</v>
       </c>
       <c r="C247">
-        <v>15.68437412045345</v>
+        <v>56.30031081080221</v>
       </c>
       <c r="D247" t="s">
         <v>304</v>
@@ -5505,7 +5505,7 @@
         <v>250</v>
       </c>
       <c r="C248">
-        <v>49.78842487009916</v>
+        <v>13.12438972111262</v>
       </c>
       <c r="D248" t="s">
         <v>304</v>
@@ -5522,7 +5522,7 @@
         <v>251</v>
       </c>
       <c r="C249">
-        <v>11.21965783852381</v>
+        <v>11.02300503092669</v>
       </c>
       <c r="D249" t="s">
         <v>304</v>
@@ -5539,7 +5539,7 @@
         <v>252</v>
       </c>
       <c r="C250">
-        <v>18.54720550513093</v>
+        <v>20.15314019310015</v>
       </c>
       <c r="D250" t="s">
         <v>304</v>
@@ -5556,7 +5556,7 @@
         <v>253</v>
       </c>
       <c r="C251">
-        <v>3.600051725886821</v>
+        <v>20.71330003209906</v>
       </c>
       <c r="D251" t="s">
         <v>304</v>
@@ -5573,7 +5573,7 @@
         <v>254</v>
       </c>
       <c r="C252">
-        <v>38.75165367214552</v>
+        <v>20.92957247141927</v>
       </c>
       <c r="D252" t="s">
         <v>304</v>
@@ -5590,7 +5590,7 @@
         <v>255</v>
       </c>
       <c r="C253">
-        <v>19.60094490524659</v>
+        <v>13.40198806682514</v>
       </c>
       <c r="D253" t="s">
         <v>304</v>
@@ -5607,7 +5607,7 @@
         <v>256</v>
       </c>
       <c r="C254">
-        <v>17.23880139789101</v>
+        <v>32.58083215346524</v>
       </c>
       <c r="D254" t="s">
         <v>304</v>
@@ -5624,7 +5624,7 @@
         <v>257</v>
       </c>
       <c r="C255">
-        <v>16.28188046055044</v>
+        <v>7.07532916635294</v>
       </c>
       <c r="D255" t="s">
         <v>304</v>
@@ -5641,7 +5641,7 @@
         <v>258</v>
       </c>
       <c r="C256">
-        <v>9.640291926280579</v>
+        <v>19.65879820069787</v>
       </c>
       <c r="D256" t="s">
         <v>304</v>
@@ -5658,7 +5658,7 @@
         <v>259</v>
       </c>
       <c r="C257">
-        <v>23.15214439924427</v>
+        <v>15.28867966571142</v>
       </c>
       <c r="D257" t="s">
         <v>304</v>
@@ -5675,7 +5675,7 @@
         <v>260</v>
       </c>
       <c r="C258">
-        <v>36.82461297604218</v>
+        <v>29.53537245426433</v>
       </c>
       <c r="D258" t="s">
         <v>304</v>
@@ -5692,7 +5692,7 @@
         <v>261</v>
       </c>
       <c r="C259">
-        <v>16.40270816997744</v>
+        <v>24.27497144677883</v>
       </c>
       <c r="D259" t="s">
         <v>304</v>
@@ -5709,7 +5709,7 @@
         <v>262</v>
       </c>
       <c r="C260">
-        <v>36.38273032197606</v>
+        <v>7.482625248761025</v>
       </c>
       <c r="D260" t="s">
         <v>304</v>
@@ -5726,7 +5726,7 @@
         <v>263</v>
       </c>
       <c r="C261">
-        <v>22.47351656507365</v>
+        <v>9.120637712412744</v>
       </c>
       <c r="D261" t="s">
         <v>304</v>
@@ -5743,7 +5743,7 @@
         <v>264</v>
       </c>
       <c r="C262">
-        <v>23.14447695198452</v>
+        <v>32.32704610144301</v>
       </c>
       <c r="D262" t="s">
         <v>304</v>
@@ -5760,7 +5760,7 @@
         <v>265</v>
       </c>
       <c r="C263">
-        <v>18.47797408373939</v>
+        <v>14.71213283840838</v>
       </c>
       <c r="D263" t="s">
         <v>304</v>
@@ -5777,7 +5777,7 @@
         <v>266</v>
       </c>
       <c r="C264">
-        <v>11.8924215516703</v>
+        <v>15.80902474081074</v>
       </c>
       <c r="D264" t="s">
         <v>304</v>
@@ -5794,7 +5794,7 @@
         <v>267</v>
       </c>
       <c r="C265">
-        <v>4.162104163939425</v>
+        <v>15.93549764848549</v>
       </c>
       <c r="D265" t="s">
         <v>304</v>
@@ -5811,7 +5811,7 @@
         <v>268</v>
       </c>
       <c r="C266">
-        <v>18.27168331088609</v>
+        <v>14.06637946123218</v>
       </c>
       <c r="D266" t="s">
         <v>304</v>
@@ -5828,7 +5828,7 @@
         <v>269</v>
       </c>
       <c r="C267">
-        <v>17.93902524124424</v>
+        <v>11.55688108076816</v>
       </c>
       <c r="D267" t="s">
         <v>304</v>
@@ -5845,7 +5845,7 @@
         <v>270</v>
       </c>
       <c r="C268">
-        <v>13.75223024493571</v>
+        <v>9.60860657681145</v>
       </c>
       <c r="D268" t="s">
         <v>304</v>
@@ -5862,7 +5862,7 @@
         <v>271</v>
       </c>
       <c r="C269">
-        <v>23.00595013836064</v>
+        <v>10.28722093779661</v>
       </c>
       <c r="D269" t="s">
         <v>304</v>
@@ -5879,7 +5879,7 @@
         <v>272</v>
       </c>
       <c r="C270">
-        <v>14.90392750428885</v>
+        <v>13.17744910544092</v>
       </c>
       <c r="D270" t="s">
         <v>304</v>
@@ -5896,7 +5896,7 @@
         <v>273</v>
       </c>
       <c r="C271">
-        <v>4.940122305081458</v>
+        <v>19.27640857643079</v>
       </c>
       <c r="D271" t="s">
         <v>304</v>
@@ -5913,7 +5913,7 @@
         <v>274</v>
       </c>
       <c r="C272">
-        <v>44.01917064263958</v>
+        <v>9.184782050903479</v>
       </c>
       <c r="D272" t="s">
         <v>304</v>
@@ -5930,7 +5930,7 @@
         <v>275</v>
       </c>
       <c r="C273">
-        <v>13.87358837651938</v>
+        <v>53.676387033098</v>
       </c>
       <c r="D273" t="s">
         <v>305</v>
@@ -5947,7 +5947,7 @@
         <v>276</v>
       </c>
       <c r="C274">
-        <v>45.91157442358609</v>
+        <v>25.58114775673775</v>
       </c>
       <c r="D274" t="s">
         <v>305</v>
@@ -5964,7 +5964,7 @@
         <v>277</v>
       </c>
       <c r="C275">
-        <v>17.13482294427354</v>
+        <v>28.47650278471686</v>
       </c>
       <c r="D275" t="s">
         <v>305</v>
@@ -5981,7 +5981,7 @@
         <v>278</v>
       </c>
       <c r="C276">
-        <v>29.89874765831535</v>
+        <v>10.04089348600693</v>
       </c>
       <c r="D276" t="s">
         <v>305</v>
@@ -5998,7 +5998,7 @@
         <v>279</v>
       </c>
       <c r="C277">
-        <v>21.87741439566188</v>
+        <v>19.3167127793144</v>
       </c>
       <c r="D277" t="s">
         <v>305</v>
@@ -6015,7 +6015,7 @@
         <v>280</v>
       </c>
       <c r="C278">
-        <v>8.208226446025275</v>
+        <v>30.78954844772216</v>
       </c>
       <c r="D278" t="s">
         <v>305</v>
@@ -6032,7 +6032,7 @@
         <v>281</v>
       </c>
       <c r="C279">
-        <v>12.48980834654113</v>
+        <v>16.76102376023147</v>
       </c>
       <c r="D279" t="s">
         <v>305</v>
@@ -6049,7 +6049,7 @@
         <v>282</v>
       </c>
       <c r="C280">
-        <v>17.46678263079069</v>
+        <v>30.2456555695343</v>
       </c>
       <c r="D280" t="s">
         <v>305</v>
@@ -6066,7 +6066,7 @@
         <v>283</v>
       </c>
       <c r="C281">
-        <v>16.04963787469344</v>
+        <v>18.6884433416116</v>
       </c>
       <c r="D281" t="s">
         <v>305</v>
@@ -6083,7 +6083,7 @@
         <v>284</v>
       </c>
       <c r="C282">
-        <v>18.9645787002292</v>
+        <v>18.14341350837176</v>
       </c>
       <c r="D282" t="s">
         <v>305</v>
@@ -6100,7 +6100,7 @@
         <v>285</v>
       </c>
       <c r="C283">
-        <v>20.17748489702751</v>
+        <v>31.6728654619996</v>
       </c>
       <c r="D283" t="s">
         <v>305</v>
@@ -6117,7 +6117,7 @@
         <v>286</v>
       </c>
       <c r="C284">
-        <v>8.960381483989273</v>
+        <v>27.56182896817279</v>
       </c>
       <c r="D284" t="s">
         <v>305</v>
@@ -6134,7 +6134,7 @@
         <v>287</v>
       </c>
       <c r="C285">
-        <v>16.98407725191067</v>
+        <v>14.73663804934506</v>
       </c>
       <c r="D285" t="s">
         <v>305</v>
@@ -6151,7 +6151,7 @@
         <v>288</v>
       </c>
       <c r="C286">
-        <v>44.40731055065208</v>
+        <v>17.22382981113002</v>
       </c>
       <c r="D286" t="s">
         <v>305</v>
@@ -6168,7 +6168,7 @@
         <v>289</v>
       </c>
       <c r="C287">
-        <v>26.24717053742405</v>
+        <v>36.5391736119365</v>
       </c>
       <c r="D287" t="s">
         <v>305</v>
@@ -6185,7 +6185,7 @@
         <v>290</v>
       </c>
       <c r="C288">
-        <v>16.32252514583658</v>
+        <v>11.10314120520932</v>
       </c>
       <c r="D288" t="s">
         <v>305</v>
@@ -6202,7 +6202,7 @@
         <v>291</v>
       </c>
       <c r="C289">
-        <v>17.30892997390727</v>
+        <v>22.69496911673725</v>
       </c>
       <c r="D289" t="s">
         <v>305</v>
@@ -6219,7 +6219,7 @@
         <v>292</v>
       </c>
       <c r="C290">
-        <v>19.07943208612391</v>
+        <v>23.1346942471225</v>
       </c>
       <c r="D290" t="s">
         <v>305</v>
@@ -6236,7 +6236,7 @@
         <v>293</v>
       </c>
       <c r="C291">
-        <v>18.61167137792142</v>
+        <v>22.56832293632563</v>
       </c>
       <c r="D291" t="s">
         <v>305</v>
@@ -6253,7 +6253,7 @@
         <v>294</v>
       </c>
       <c r="C292">
-        <v>17.47503249762057</v>
+        <v>13.19560388084465</v>
       </c>
       <c r="D292" t="s">
         <v>305</v>
@@ -6270,7 +6270,7 @@
         <v>295</v>
       </c>
       <c r="C293">
-        <v>43.44648437289835</v>
+        <v>20.20590400185623</v>
       </c>
       <c r="D293" t="s">
         <v>305</v>
@@ -6287,7 +6287,7 @@
         <v>296</v>
       </c>
       <c r="C294">
-        <v>35.99722567863682</v>
+        <v>62.7510875579828</v>
       </c>
       <c r="D294" t="s">
         <v>305</v>
@@ -6304,7 +6304,7 @@
         <v>297</v>
       </c>
       <c r="C295">
-        <v>17.97456154875903</v>
+        <v>20.94147852385647</v>
       </c>
       <c r="D295" t="s">
         <v>305</v>
@@ -6321,7 +6321,7 @@
         <v>298</v>
       </c>
       <c r="C296">
-        <v>10.46149595085942</v>
+        <v>7.623150850845413</v>
       </c>
       <c r="D296" t="s">
         <v>305</v>
@@ -6338,7 +6338,7 @@
         <v>299</v>
       </c>
       <c r="C297">
-        <v>15.21527863257401</v>
+        <v>14.20343296985414</v>
       </c>
       <c r="D297" t="s">
         <v>305</v>
@@ -6355,7 +6355,7 @@
         <v>300</v>
       </c>
       <c r="C298">
-        <v>19.10326167058898</v>
+        <v>20.29446148936682</v>
       </c>
       <c r="D298" t="s">
         <v>305</v>
@@ -6372,7 +6372,7 @@
         <v>301</v>
       </c>
       <c r="C299">
-        <v>24.87998031760033</v>
+        <v>40.57433501146127</v>
       </c>
       <c r="D299" t="s">
         <v>305</v>
@@ -6389,7 +6389,7 @@
         <v>302</v>
       </c>
       <c r="C300">
-        <v>55.0562102411717</v>
+        <v>16.87369146406278</v>
       </c>
       <c r="D300" t="s">
         <v>305</v>
@@ -6406,7 +6406,7 @@
         <v>303</v>
       </c>
       <c r="C301">
-        <v>13.72805385255014</v>
+        <v>10.73551196593366</v>
       </c>
       <c r="D301" t="s">
         <v>305</v>

</xml_diff>